<commit_message>
PROS-5336 - KPI update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/HoReCa Bar Tavern_Night Club PoS 2018.xlsx
+++ b/Projects/CCRU/Data/HoReCa Bar Tavern_Night Club PoS 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="HoReCa Bar Tavern_Night Club" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AQ$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AQ$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AQ$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AP$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AQ$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AP$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AP$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AP$42</definedName>
@@ -37,6 +37,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AP$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AP$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AP$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AP$42</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -63,7 +64,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Aleksandra Danilenko:
+          <t xml:space="preserve">Aleksandra Danilenko:
 comments</t>
         </r>
       </text>
@@ -78,7 +79,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Aleksandra Danilenko:
+          <t xml:space="preserve">Aleksandra Danilenko:
 sku или сцена??</t>
         </r>
       </text>
@@ -93,7 +94,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Aleksandra Danilenko:
+          <t xml:space="preserve">Aleksandra Danilenko:
 sku или сцена??</t>
         </r>
       </text>
@@ -108,7 +109,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Aleksandra Danilenko:
+          <t xml:space="preserve">Aleksandra Danilenko:
 sku или сцена??</t>
         </r>
       </text>
@@ -120,157 +121,157 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="198">
   <si>
-    <t>Sorting</t>
+    <t xml:space="preserve">Sorting</t>
   </si>
   <si>
-    <t>SAP PoS</t>
+    <t xml:space="preserve">SAP PoS</t>
   </si>
   <si>
-    <t>Channel</t>
+    <t xml:space="preserve">Channel</t>
   </si>
   <si>
-    <t>KPI Type</t>
+    <t xml:space="preserve">KPI Type</t>
   </si>
   <si>
-    <t>SAP KPI</t>
+    <t xml:space="preserve">SAP KPI</t>
   </si>
   <si>
-    <t>KPI name Eng</t>
+    <t xml:space="preserve">KPI name Eng</t>
   </si>
   <si>
-    <t>KPI name Rus</t>
+    <t xml:space="preserve">KPI name Rus</t>
   </si>
   <si>
-    <t>Formula</t>
+    <t xml:space="preserve">Formula</t>
   </si>
   <si>
-    <t>Target</t>
+    <t xml:space="preserve">Target</t>
   </si>
   <si>
-    <t>target_min</t>
+    <t xml:space="preserve">target_min</t>
   </si>
   <si>
-    <t>target_max</t>
+    <t xml:space="preserve">target_max</t>
   </si>
   <si>
-    <t>SKU</t>
+    <t xml:space="preserve">SKU</t>
   </si>
   <si>
-    <t>Values</t>
+    <t xml:space="preserve">Values</t>
   </si>
   <si>
-    <t>Product Category</t>
+    <t xml:space="preserve">Product Category</t>
   </si>
   <si>
-    <t>Manufacturer</t>
+    <t xml:space="preserve">Manufacturer</t>
   </si>
   <si>
-    <t>Brand</t>
+    <t xml:space="preserve">Brand</t>
   </si>
   <si>
-    <t>Logical Operator</t>
+    <t xml:space="preserve">Logical Operator</t>
   </si>
   <si>
-    <t>Type</t>
+    <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t>Size</t>
+    <t xml:space="preserve">Size</t>
   </si>
   <si>
-    <t>Form Factor</t>
+    <t xml:space="preserve">Form Factor</t>
   </si>
   <si>
-    <t>Products to exclude</t>
+    <t xml:space="preserve">Products to exclude</t>
   </si>
   <si>
-    <t>Zone to include</t>
+    <t xml:space="preserve">Zone to include</t>
   </si>
   <si>
-    <t>Locations to exclude</t>
+    <t xml:space="preserve">Locations to exclude</t>
   </si>
   <si>
-    <t>Locations to include</t>
+    <t xml:space="preserve">Locations to include</t>
   </si>
   <si>
-    <t>Scenes to include</t>
+    <t xml:space="preserve">Scenes to include</t>
   </si>
   <si>
-    <t>Scenes to exclude</t>
+    <t xml:space="preserve">Scenes to exclude</t>
   </si>
   <si>
-    <t>sub locations to include</t>
+    <t xml:space="preserve">sub locations to include</t>
   </si>
   <si>
-    <t>sub locations to exclude</t>
+    <t xml:space="preserve">sub locations to exclude</t>
   </si>
   <si>
-    <t>Converted?</t>
+    <t xml:space="preserve">Converted?</t>
   </si>
   <si>
-    <t>score_func</t>
+    <t xml:space="preserve">score_func</t>
   </si>
   <si>
-    <t>KPI Weight</t>
+    <t xml:space="preserve">KPI Weight</t>
   </si>
   <si>
-    <t>score_min</t>
+    <t xml:space="preserve">score_min</t>
   </si>
   <si>
-    <t>score_max</t>
+    <t xml:space="preserve">score_max</t>
   </si>
   <si>
-    <t>Comments</t>
+    <t xml:space="preserve">Comments</t>
   </si>
   <si>
-    <t>Base KPI for TOP 5 GAPs</t>
+    <t xml:space="preserve">Base KPI for TOP 5 GAPs</t>
   </si>
   <si>
-    <t>KPI from POS 2016</t>
+    <t xml:space="preserve">KPI from POS 2016</t>
   </si>
   <si>
-    <t>level</t>
+    <t xml:space="preserve">level</t>
   </si>
   <si>
-    <t>KPI ID</t>
+    <t xml:space="preserve">KPI ID</t>
   </si>
   <si>
-    <t>Children</t>
+    <t xml:space="preserve">Children</t>
   </si>
   <si>
-    <t>Parent</t>
+    <t xml:space="preserve">Parent</t>
   </si>
   <si>
-    <t>To include in first calculation?</t>
+    <t xml:space="preserve">To include in first calculation?</t>
   </si>
   <si>
-    <t>Target Execution 2018</t>
+    <t xml:space="preserve">Target Execution 2018</t>
   </si>
   <si>
-    <t>RD38010009</t>
+    <t xml:space="preserve">RD38010009</t>
   </si>
   <si>
-    <t>HoReCa (Bar Tavern/Night Clubs)</t>
+    <t xml:space="preserve">HoReCa (Bar Tavern/Night Clubs)</t>
   </si>
   <si>
-    <t>Group</t>
+    <t xml:space="preserve">Group</t>
   </si>
   <si>
-    <t>STANDARD 1</t>
+    <t xml:space="preserve">STANDARD 1</t>
   </si>
   <si>
-    <t>SSD Availability</t>
+    <t xml:space="preserve">SSD Availability</t>
   </si>
   <si>
-    <t>Представленность SSD</t>
+    <t xml:space="preserve">Представленность SSD</t>
   </si>
   <si>
-    <t>Weighted Average </t>
+    <t xml:space="preserve">Weighted Average </t>
   </si>
   <si>
-    <t>Y</t>
+    <t xml:space="preserve">Y</t>
   </si>
   <si>
-    <t>2
+    <t xml:space="preserve">2
 3
 4
 5
@@ -279,460 +280,460 @@
 8</t>
   </si>
   <si>
-    <t>Coca-Cola - 0.33L Glass</t>
+    <t xml:space="preserve">Coca-Cola - 0.33L Glass</t>
   </si>
   <si>
-    <t>Кока-Кола - 0.33л стекло</t>
+    <t xml:space="preserve">Кока-Кола - 0.33л стекло</t>
   </si>
   <si>
-    <t>number of facings</t>
+    <t xml:space="preserve">number of facings</t>
   </si>
   <si>
-    <t>OR</t>
+    <t xml:space="preserve">OR</t>
   </si>
   <si>
-    <t>SKUs</t>
+    <t xml:space="preserve">SKUs</t>
   </si>
   <si>
-    <t>Other</t>
+    <t xml:space="preserve">Other</t>
   </si>
   <si>
-    <t>Panoramic Photo</t>
+    <t xml:space="preserve">Panoramic Photo</t>
   </si>
   <si>
-    <t>BINARY</t>
+    <t xml:space="preserve">BINARY</t>
   </si>
   <si>
-    <t>Coca-Cola Zero - 0.33L Glass</t>
+    <t xml:space="preserve">Coca-Cola Zero - 0.33L Glass</t>
   </si>
   <si>
-    <t>Кока-Кола Зеро - 0.33л стекло</t>
+    <t xml:space="preserve">Кока-Кола Зеро - 0.33л стекло</t>
   </si>
   <si>
-    <t>Schweppes Tonic - 0.25L Glass</t>
+    <t xml:space="preserve">Schweppes Tonic - 0.25L Glass</t>
   </si>
   <si>
-    <t>Швеппс Тоник - 0.25л стекло</t>
+    <t xml:space="preserve">Швеппс Тоник - 0.25л стекло</t>
   </si>
   <si>
-    <t>Schweppes Bitter Lemon - 0.25L Glass</t>
+    <t xml:space="preserve">Schweppes Bitter Lemon - 0.25L Glass</t>
   </si>
   <si>
-    <t>Швеппс Биттер Лемон - 0.25л стекло</t>
+    <t xml:space="preserve">Швеппс Биттер Лемон - 0.25л стекло</t>
   </si>
   <si>
-    <t>Schweppes Aperol Spritz - 0.25L Glass</t>
+    <t xml:space="preserve">Schweppes Aperol Spritz - 0.25L Glass</t>
   </si>
   <si>
-    <t>Швеппс Шпритц - 0.25л стекло</t>
+    <t xml:space="preserve">Швеппс Шпритц - 0.25л стекло</t>
   </si>
   <si>
-    <t>Sprite - 0.25L Glass</t>
+    <t xml:space="preserve">Sprite - 0.25L Glass</t>
   </si>
   <si>
-    <t>Спрайт - 0.25л стекло</t>
+    <t xml:space="preserve">Спрайт - 0.25л стекло</t>
   </si>
   <si>
-    <t>Fanta Orange - 0.25L Glass</t>
+    <t xml:space="preserve">Fanta Orange - 0.25L Glass</t>
   </si>
   <si>
-    <t>Фанта Апельсин - 0.25л стекло</t>
+    <t xml:space="preserve">Фанта Апельсин - 0.25л стекло</t>
   </si>
   <si>
-    <t>STANDARD 2</t>
+    <t xml:space="preserve">STANDARD 2</t>
   </si>
   <si>
-    <t>Water Availability</t>
+    <t xml:space="preserve">Water Availability</t>
   </si>
   <si>
-    <t>Представленность Воды</t>
+    <t xml:space="preserve">Представленность Воды</t>
   </si>
   <si>
-    <t>10
+    <t xml:space="preserve">10
 11
 12</t>
   </si>
   <si>
-    <t>BonAqua Still - 0.33L Glass</t>
+    <t xml:space="preserve">BonAqua Still - 0.33L Glass</t>
   </si>
   <si>
-    <t>БонАква Негаз - 0.33л стекло</t>
+    <t xml:space="preserve">БонАква Негаз - 0.33л стекло</t>
   </si>
   <si>
-    <t>BonAqua Carb - 0.33L Glass</t>
+    <t xml:space="preserve">BonAqua Carb - 0.33L Glass</t>
   </si>
   <si>
-    <t>БонАква Газ - 0.33л стекло</t>
+    <t xml:space="preserve">БонАква Газ - 0.33л стекло</t>
   </si>
   <si>
-    <t>BonAqua Still - 0.75L Glass</t>
+    <t xml:space="preserve">BonAqua Still - 0.75L Glass</t>
   </si>
   <si>
-    <t>БонАква Негаз - 0.75л стекло</t>
+    <t xml:space="preserve">БонАква Негаз - 0.75л стекло</t>
   </si>
   <si>
-    <t>Energy Availability</t>
+    <t xml:space="preserve">Energy Availability</t>
   </si>
   <si>
-    <t>Представленность Энергетиков</t>
+    <t xml:space="preserve">Представленность Энергетиков</t>
   </si>
   <si>
-    <t>14
+    <t xml:space="preserve">14
 0</t>
   </si>
   <si>
-    <t>Burn Original - 0.33L</t>
+    <t xml:space="preserve">Burn Original - 0.33L</t>
   </si>
   <si>
-    <t>Берн Оригинальный - 0.33л</t>
+    <t xml:space="preserve">Берн Оригинальный - 0.33л</t>
   </si>
   <si>
-    <t>Juice Availability</t>
+    <t xml:space="preserve">Juice Availability</t>
   </si>
   <si>
-    <t>Представленность Сока</t>
+    <t xml:space="preserve">Представленность Сока</t>
   </si>
   <si>
-    <t>16
+    <t xml:space="preserve">16
 17
 18
 19</t>
   </si>
   <si>
-    <t>Rich - Orange - 0.2L Glass</t>
+    <t xml:space="preserve">Rich - Orange - 0.2L Glass</t>
   </si>
   <si>
-    <t>Рич - Апельсин - 0.2л стекло</t>
+    <t xml:space="preserve">Рич - Апельсин - 0.2л стекло</t>
   </si>
   <si>
-    <t>Rich - Apple - 0.2L Glass</t>
+    <t xml:space="preserve">Rich - Apple - 0.2L Glass</t>
   </si>
   <si>
-    <t>Рич - Яблоко - 0.2л стекло</t>
+    <t xml:space="preserve">Рич - Яблоко - 0.2л стекло</t>
   </si>
   <si>
-    <t>Rich - Cherry - 0.2L Glass</t>
+    <t xml:space="preserve">Rich - Cherry - 0.2L Glass</t>
   </si>
   <si>
-    <t>Рич - Вишня - 0.2л стекло</t>
+    <t xml:space="preserve">Рич - Вишня - 0.2л стекло</t>
   </si>
   <si>
-    <t>Rich - Tomato - 0.2L Glass</t>
+    <t xml:space="preserve">Rich - Tomato - 0.2L Glass</t>
   </si>
   <si>
-    <t>Рич - Томат - 0.2л стекло</t>
+    <t xml:space="preserve">Рич - Томат - 0.2л стекло</t>
   </si>
   <si>
-    <t>Local</t>
+    <t xml:space="preserve">Local</t>
   </si>
   <si>
-    <t>LOCAL 3</t>
+    <t xml:space="preserve">LOCAL 3</t>
   </si>
   <si>
-    <t>Spirits Availability</t>
+    <t xml:space="preserve">Spirits Availability</t>
   </si>
   <si>
-    <t>Представленность Алкоголя</t>
+    <t xml:space="preserve">Представленность Алкоголя</t>
   </si>
   <si>
-    <t>Weighted Average</t>
+    <t xml:space="preserve">Weighted Average</t>
   </si>
   <si>
-    <t>21
+    <t xml:space="preserve">21
 22
 23</t>
   </si>
   <si>
-    <t>Red Hackle - 0.7L</t>
+    <t xml:space="preserve">Red Hackle - 0.7L</t>
   </si>
   <si>
-    <t>Рэд Хакл - 0.7л</t>
+    <t xml:space="preserve">Рэд Хакл - 0.7л</t>
   </si>
   <si>
-    <t>Wild Turkey 81 - 0.7L</t>
+    <t xml:space="preserve">Wild Turkey 81 - 0.7L</t>
   </si>
   <si>
-    <t>Уайлд Тёки 81 - 0.7л</t>
+    <t xml:space="preserve">Уайлд Тёки 81 - 0.7л</t>
   </si>
   <si>
-    <t>New Alco Brand</t>
+    <t xml:space="preserve">New Alco Brand</t>
   </si>
   <si>
-    <t>not defined</t>
+    <t xml:space="preserve">not defined</t>
   </si>
   <si>
-    <t>STANDARD 16</t>
+    <t xml:space="preserve">STANDARD 16</t>
   </si>
   <si>
-    <t>Menu Activation</t>
+    <t xml:space="preserve">Menu Activation</t>
   </si>
   <si>
-    <t>Активация Меню</t>
+    <t xml:space="preserve">Активация Меню</t>
   </si>
   <si>
-    <t>Coca Cola Can, Coca Cola Zero Can 0.33, Coca Cola Zero Bottle, Coca Cola Zero Bottle NRGB, Coca Cola Glass, Coca Cola Cup, Coca Cola Bottle NRGB, Coca Cola Bottle</t>
+    <t xml:space="preserve">Coca Cola Can, Coca Cola Zero Can 0.33, Coca Cola Zero Bottle, Coca Cola Zero Bottle NRGB, Coca Cola Glass, Coca Cola Cup, Coca Cola Bottle NRGB, Coca Cola Bottle</t>
   </si>
   <si>
-    <t>5050570, 50111114, 50111112, 50111111, 5000006, 5000101, 5000005, 5000004</t>
+    <t xml:space="preserve">5050570, 50111114, 50111112, 50111111, 5000006, 5000101, 5000005, 5000004</t>
   </si>
   <si>
-    <t>Activation</t>
+    <t xml:space="preserve">Activation</t>
   </si>
   <si>
-    <t>Other Menu Activation, Menu, Menu Insert</t>
+    <t xml:space="preserve">Other Menu Activation, Menu, Menu Insert</t>
   </si>
   <si>
-    <t>STANDARD 17</t>
+    <t xml:space="preserve">STANDARD 17</t>
   </si>
   <si>
-    <t>Impulse Activation</t>
+    <t xml:space="preserve">Impulse Activation</t>
   </si>
   <si>
-    <t>Активация Импульсной зоны</t>
+    <t xml:space="preserve">Активация Импульсной зоны</t>
   </si>
   <si>
-    <t>number of atomic KPI Passed</t>
+    <t xml:space="preserve">number of atomic KPI Passed</t>
   </si>
   <si>
-    <t>Bar Activation</t>
+    <t xml:space="preserve">Bar Activation</t>
   </si>
   <si>
-    <t>26
+    <t xml:space="preserve">26
 27
 28</t>
   </si>
   <si>
-    <t>Impulse: SSD/Water/Juice NRGB</t>
+    <t xml:space="preserve">Impulse: SSD/Water/Juice NRGB</t>
   </si>
   <si>
-    <t>Импульс: SSD/Water/Juice Стекло</t>
+    <t xml:space="preserve">Импульс: SSD/Water/Juice Стекло</t>
   </si>
   <si>
-    <t>Manufacture: TCCC</t>
+    <t xml:space="preserve">Manufacture: TCCC</t>
   </si>
   <si>
-    <t>SSD, Water, Juices</t>
+    <t xml:space="preserve">SSD, Water, Juices</t>
   </si>
   <si>
-    <t>MAN in CAT</t>
+    <t xml:space="preserve">MAN in CAT</t>
   </si>
   <si>
-    <t>glass</t>
+    <t xml:space="preserve">glass</t>
   </si>
   <si>
-    <t>Impulse: Burn CAN</t>
+    <t xml:space="preserve">Impulse: Burn CAN</t>
   </si>
   <si>
-    <t>Импульс: Burn Банка</t>
+    <t xml:space="preserve">Импульс: Burn Банка</t>
   </si>
   <si>
-    <t>Burn</t>
+    <t xml:space="preserve">Burn</t>
   </si>
   <si>
-    <t>BRAND</t>
+    <t xml:space="preserve">BRAND</t>
   </si>
   <si>
-    <t>CAN, can</t>
+    <t xml:space="preserve">CAN, can</t>
   </si>
   <si>
-    <t>Impulse: Alcohol</t>
+    <t xml:space="preserve">Impulse: Alcohol</t>
   </si>
   <si>
-    <t>Импульс: Алкоголь</t>
+    <t xml:space="preserve">Импульс: Алкоголь</t>
   </si>
   <si>
-    <t>number of SKUs</t>
+    <t xml:space="preserve">number of SKUs</t>
   </si>
   <si>
-    <t>Manufacture: TCCC, CAMPARI</t>
+    <t xml:space="preserve">Manufacture: TCCC, CAMPARI</t>
   </si>
   <si>
-    <t>Spirits</t>
+    <t xml:space="preserve">Spirits</t>
   </si>
   <si>
-    <t>TCCC, CAMPARI</t>
+    <t xml:space="preserve">TCCC, CAMPARI</t>
   </si>
   <si>
-    <t>CAT</t>
+    <t xml:space="preserve">CAT</t>
   </si>
   <si>
-    <t>Destination Activation</t>
+    <t xml:space="preserve">Destination Activation</t>
   </si>
   <si>
-    <t>Активация Стола</t>
+    <t xml:space="preserve">Активация Стола</t>
   </si>
   <si>
-    <t>Table Activation</t>
+    <t xml:space="preserve">Table Activation</t>
   </si>
   <si>
-    <t>30
+    <t xml:space="preserve">30
 31</t>
   </si>
   <si>
-    <t>Destination: Images</t>
+    <t xml:space="preserve">Destination: Images</t>
   </si>
   <si>
-    <t>Активация Стола: Имиджи</t>
+    <t xml:space="preserve">Активация Стола: Имиджи</t>
   </si>
   <si>
-    <t>IC Activation</t>
+    <t xml:space="preserve">IC Activation</t>
   </si>
   <si>
-    <t>Any IC Activations w/o Food</t>
+    <t xml:space="preserve">Any IC Activations w/o Food</t>
   </si>
   <si>
-    <t>Destination: Coca-Cola/BonAqua NRGB</t>
+    <t xml:space="preserve">Destination: Coca-Cola/BonAqua NRGB</t>
   </si>
   <si>
-    <t>Активация Стола: Кока-Кола/Бонаква Стекло</t>
+    <t xml:space="preserve">Активация Стола: Кока-Кола/Бонаква Стекло</t>
   </si>
   <si>
-    <t>Coca-Cola, Bonaqua</t>
+    <t xml:space="preserve">Coca-Cola, Bonaqua</t>
   </si>
   <si>
-    <t>OCCASIONS</t>
+    <t xml:space="preserve">OCCASIONS</t>
   </si>
   <si>
-    <t>Drink Out: Evening out</t>
+    <t xml:space="preserve">Drink Out: Evening out</t>
   </si>
   <si>
-    <t>Повод: Начало вечера/препати</t>
+    <t xml:space="preserve">Повод: Начало вечера/препати</t>
   </si>
   <si>
-    <t>RED_HACKLE_0.7L, Aperol_Magnet, Aperol_Cube, Mondoro activation, Espolon activation, Campari activation, Aperol Spritz Activation_1, Aperol Spritz Activation, Red_Hackle_Stiker, Red_Hackle_Menu_Insert_1, Red_Hackle_Menu_Insert_2</t>
+    <t xml:space="preserve">RED_HACKLE_0.7L, Aperol_Magnet, Aperol_Cube, Mondoro activation, Espolon activation, Campari activation, Aperol Spritz Activation_1, Aperol Spritz Activation, Red_Hackle_Stiker, Red_Hackle_Menu_Insert_1, Red_Hackle_Menu_Insert_2</t>
   </si>
   <si>
-    <t>A5B10083, A5B10056, A5B10055, 9000900, 9000800, 9000700, 9000600, 9000500, 5099873001362, 5099873001360, 5099873001361</t>
+    <t xml:space="preserve">A5B10083, A5B10056, A5B10055, 9000900, 9000800, 9000700, 9000600, 9000500, 5099873001362, 5099873001360, 5099873001361</t>
   </si>
   <si>
-    <t>Menu, Menu Insert, Other Menu Activation, Table Activation, Bar Activation</t>
+    <t xml:space="preserve">Menu, Menu Insert, Other Menu Activation, Table Activation, Bar Activation</t>
   </si>
   <si>
-    <t>Drink Out: Midday socializing</t>
+    <t xml:space="preserve">Drink Out: Midday socializing</t>
   </si>
   <si>
-    <t>Повод: Relax после работы</t>
+    <t xml:space="preserve">Повод: Relax после работы</t>
   </si>
   <si>
-    <t>34
+    <t xml:space="preserve">34
 35</t>
   </si>
   <si>
-    <t>Midday socializing: Mixability</t>
+    <t xml:space="preserve">Midday socializing: Mixability</t>
   </si>
   <si>
-    <t>Relax после работы: Миксабилити</t>
+    <t xml:space="preserve">Relax после работы: Миксабилити</t>
   </si>
   <si>
-    <t>RED Hackle mix_img (2), Finlandia and Rich Cherry, Finlandia and Rich menu insert, Finlandia and Rich Mix, Finlandia and Rich Orange, Finlandia and Rich table tent, Finlandia and Schweppes Menu Insert, Finlandia and Schweppes Table Tent, Finlandia and Schweppes, Jack and Coke Menu, Jack and Coke Table tent, Jack Daniles and Coke Mix, Jack Daniles and Coke, Finlandia and Rich Sticker Cherry, Finlandia and Rich Sticker Orange, Finlandia and Rich table tent Cherry</t>
+    <t xml:space="preserve">RED Hackle mix_img (2), Finlandia and Rich Cherry, Finlandia and Rich menu insert, Finlandia and Rich Mix, Finlandia and Rich Orange, Finlandia and Rich table tent, Finlandia and Schweppes Menu Insert, Finlandia and Schweppes Table Tent, Finlandia and Schweppes, Jack and Coke Menu, Jack and Coke Table tent, Jack Daniles and Coke Mix, Jack Daniles and Coke, Finlandia and Rich Sticker Cherry, Finlandia and Rich Sticker Orange, Finlandia and Rich table tent Cherry</t>
   </si>
   <si>
-    <t>A5B10100, A5B10101, 7777888899, 7777888900, 7777888901, 7777888902, 7777888903, 7777888904, 7777888905, 7777888906, 7777888907, 7777888908, 7777888909, 7777888910, 7777889000, 7777889001, 7777889002</t>
+    <t xml:space="preserve">A5B10100, A5B10101, 7777888899, 7777888900, 7777888901, 7777888902, 7777888903, 7777888904, 7777888905, 7777888906, 7777888907, 7777888908, 7777888909, 7777888910, 7777889000, 7777889001, 7777889002</t>
   </si>
   <si>
-    <t>Midday socializing: Moctails</t>
+    <t xml:space="preserve">Midday socializing: Moctails</t>
   </si>
   <si>
-    <t>Relax после работы: Моктели</t>
+    <t xml:space="preserve">Relax после работы: Моктели</t>
   </si>
   <si>
-    <t>new</t>
+    <t xml:space="preserve">new</t>
   </si>
   <si>
-    <t>Drink Out: Party night</t>
+    <t xml:space="preserve">Drink Out: Party night</t>
   </si>
   <si>
-    <t>Повод: Ночная вечеринка</t>
+    <t xml:space="preserve">Повод: Ночная вечеринка</t>
   </si>
   <si>
-    <t>Burn Glass, Monster CAN, BRN_330ml_Burn_AppleKiwi, BRN_330ml_Burn_Original, BRN_500ml_Burn_AppleKiwi, BRN_500ml_Burn_Original</t>
+    <t xml:space="preserve">Burn Glass, Monster CAN, BRN_330ml_Burn_AppleKiwi, BRN_330ml_Burn_Original, BRN_500ml_Burn_AppleKiwi, BRN_500ml_Burn_Original</t>
   </si>
   <si>
-    <t>5000003, 68943577002, 78789, 78790, 78791, 78792</t>
+    <t xml:space="preserve">5000003, 68943577002, 78789, 78790, 78791, 78792</t>
   </si>
   <si>
-    <t>-</t>
+    <t xml:space="preserve">-</t>
   </si>
   <si>
-    <t>Visible Cooler</t>
+    <t xml:space="preserve">Visible Cooler</t>
   </si>
   <si>
-    <t>Видимый ХО</t>
+    <t xml:space="preserve">Видимый ХО</t>
   </si>
   <si>
-    <t>Cooler</t>
+    <t xml:space="preserve">Cooler</t>
   </si>
   <si>
-    <t>38
+    <t xml:space="preserve">38
 39
 40
 41</t>
   </si>
   <si>
-    <t>Cooler is Visible</t>
+    <t xml:space="preserve">Cooler is Visible</t>
   </si>
   <si>
-    <t>ХО виден</t>
+    <t xml:space="preserve">ХО виден</t>
   </si>
   <si>
-    <t>Scenes with no tagging</t>
+    <t xml:space="preserve">Scenes with no tagging</t>
   </si>
   <si>
-    <t>SCENES</t>
+    <t xml:space="preserve">SCENES</t>
   </si>
   <si>
-    <t>Panoramic photo of Cooler</t>
+    <t xml:space="preserve">Panoramic photo of Cooler</t>
   </si>
   <si>
-    <t>Cooler fullness</t>
+    <t xml:space="preserve">Cooler fullness</t>
   </si>
   <si>
-    <t>ХО Заполнен</t>
+    <t xml:space="preserve">ХО Заполнен</t>
   </si>
   <si>
-    <t>number of filled Coolers (scenes)</t>
+    <t xml:space="preserve">number of filled Coolers (scenes)</t>
   </si>
   <si>
-    <t>TCCC</t>
+    <t xml:space="preserve">TCCC</t>
   </si>
   <si>
-    <t>MAN</t>
+    <t xml:space="preserve">MAN</t>
   </si>
   <si>
-    <t>SOS with empty more than 80%</t>
+    <t xml:space="preserve">SOS with empty more than 80%</t>
   </si>
   <si>
-    <t>Cooler wo other products</t>
+    <t xml:space="preserve">Cooler wo other products</t>
   </si>
   <si>
-    <t>ХО без посторонней продукции</t>
+    <t xml:space="preserve">ХО без посторонней продукции</t>
   </si>
   <si>
-    <t>number of pure Coolers</t>
+    <t xml:space="preserve">number of pure Coolers</t>
   </si>
   <si>
-    <t>Share of TCCC product at least 98%</t>
+    <t xml:space="preserve">Share of TCCC product at least 98%</t>
   </si>
   <si>
-    <t>Cooler: Max 14</t>
+    <t xml:space="preserve">Cooler: Max 14</t>
   </si>
   <si>
-    <t>Холодильники: Максимум 14 СКЮ на дверь</t>
+    <t xml:space="preserve">Холодильники: Максимум 14 СКЮ на дверь</t>
   </si>
   <si>
-    <t>number of SKU per Door RANGE</t>
+    <t xml:space="preserve">number of SKU per Door RANGE</t>
   </si>
   <si>
-    <t>Scene</t>
+    <t xml:space="preserve">Scene</t>
   </si>
   <si>
-    <t>KPI Score Formula</t>
+    <t xml:space="preserve">KPI Score Formula</t>
   </si>
   <si>
-    <t>KPI weighted Score</t>
+    <t xml:space="preserve">KPI weighted Score</t>
   </si>
   <si>
-    <t>Will be added on the 16th of December</t>
+    <t xml:space="preserve">Will be added on the 16th of December</t>
   </si>
 </sst>
 </file>
@@ -740,7 +741,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
@@ -768,6 +769,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -847,12 +854,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -917,12 +918,19 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -954,7 +962,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -980,7 +988,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -1001,259 +1012,259 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="10" fillId="0" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1261,19 +1272,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1281,23 +1292,23 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1306,14 +1317,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="SAPBEXstdItem" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1391,7 +1403,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>736920</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>312120</xdr:rowOff>
+      <xdr:rowOff>311760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1401,7 +1413,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="513000" y="0"/>
-          <a:ext cx="16349400" cy="10414800"/>
+          <a:ext cx="16825680" cy="10414440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1436,7 +1448,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>736920</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>312120</xdr:rowOff>
+      <xdr:rowOff>311760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1446,7 +1458,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="513000" y="0"/>
-          <a:ext cx="16349400" cy="10414800"/>
+          <a:ext cx="16825680" cy="10414440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1481,7 +1493,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>736920</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>312120</xdr:rowOff>
+      <xdr:rowOff>311760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1491,7 +1503,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="513000" y="0"/>
-          <a:ext cx="16349400" cy="10414800"/>
+          <a:ext cx="16825680" cy="10414440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1526,7 +1538,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>736920</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>312120</xdr:rowOff>
+      <xdr:rowOff>311760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1536,7 +1548,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="513000" y="0"/>
-          <a:ext cx="16349400" cy="10414800"/>
+          <a:ext cx="16825680" cy="10414440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1569,51 +1581,51 @@
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:42"/>
+  <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="H2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.4604651162791"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="48.1162790697674"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="31.7488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="38.1488372093023"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="22.6418604651163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="30.5209302325581"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="29.9023255813953"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="2" width="33.4744186046512"/>
-    <col collapsed="false" hidden="false" max="19" min="17" style="2" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="22" min="20" style="2" width="22.8883720930233"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="29.9023255813953"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="30.8883720930233"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="46.7627906976744"/>
-    <col collapsed="false" hidden="false" max="28" min="26" style="2" width="28.9209302325581"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="2" width="23.6279069767442"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="3" width="21.4139534883721"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="24.8604651162791"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="2" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="2" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="2" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="38" min="36" style="2" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="1" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="2" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="2" width="24.1209302325581"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="2" width="29.9023255813953"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="2" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="44" style="1" width="16.9813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.4883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="49.5953488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="32.6093023255814"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="39.2558139534884"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="23.2604651162791"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="31.3813953488372"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="2" width="34.4558139534884"/>
+    <col collapsed="false" hidden="false" max="19" min="17" style="2" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="22" min="20" style="2" width="23.506976744186"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="31.7488372093023"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="48.1162790697674"/>
+    <col collapsed="false" hidden="false" max="28" min="26" style="2" width="29.6558139534884"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="2" width="24.2418604651163"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="3" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="25.5953488372093"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="2" width="36.4279069767442"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="2" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="2" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="38" min="36" style="2" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="1" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="2" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="2" width="24.8604651162791"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="2" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="2" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="44" style="1" width="17.4744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8084,7 +8096,7 @@
         <v>65</v>
       </c>
       <c r="M7" s="39" t="n">
-        <v>4607042439070</v>
+        <v>42357278</v>
       </c>
       <c r="N7" s="32"/>
       <c r="O7" s="32"/>
@@ -41530,6 +41542,8 @@
       <c r="AP42" s="34"/>
       <c r="AQ42" s="28"/>
     </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:AQ42"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -41557,7 +41571,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.0604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.306976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-5509 - CCRU - KPI template update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/HoReCa Bar Tavern_Night Club PoS 2018.xlsx
+++ b/Projects/CCRU/Data/HoReCa Bar Tavern_Night Club PoS 2018.xlsx
@@ -23,7 +23,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AS$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AS$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AS$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AS$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
@@ -39,6 +39,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -478,10 +479,10 @@
     <t xml:space="preserve">Активация Меню</t>
   </si>
   <si>
-    <t xml:space="preserve">Coca Cola Can, Coca Cola Zero Can 0.33, Coca Cola Zero Bottle, Coca Cola Zero Bottle NRGB, Coca Cola Glass, Coca Cola Cup, Coca Cola Bottle NRGB, Coca Cola Bottle</t>
+    <t xml:space="preserve">Coca Cola Can, Coca Cola Zero Can 0.33, Coca Cola Zero Bottle, Coca Cola Zero Bottle NRGB, Coca Cola Glass, Coca Cola Cup, Coca Cola Bottle NRGB, Coca Cola Bottle, Cc Graphic, Cc Glass Graphic, Cc Glass And Bottle, CC Hands, Cc Bottle Graphic</t>
   </si>
   <si>
-    <t xml:space="preserve">5050570, 50111114, 50111112, 50111111, 5000006, 5000101, 5000005, 5000004</t>
+    <t xml:space="preserve">5050570, 50111114, 50111112, 50111111, 5000006, 5000101, 5000005, 5000004, 68943577005, 68943577006, 68943577007, 68943577008, 68943577009</t>
   </si>
   <si>
     <t xml:space="preserve">Activation</t>
@@ -1550,9 +1551,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>736920</xdr:colOff>
+      <xdr:colOff>736560</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>311400</xdr:rowOff>
+      <xdr:rowOff>311040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1562,7 +1563,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="513000" y="0"/>
-          <a:ext cx="24369480" cy="10415520"/>
+          <a:ext cx="25083720" cy="10415160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1595,9 +1596,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>736920</xdr:colOff>
+      <xdr:colOff>736560</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>311400</xdr:rowOff>
+      <xdr:rowOff>311040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1607,7 +1608,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="513000" y="0"/>
-          <a:ext cx="24369480" cy="10415520"/>
+          <a:ext cx="25083720" cy="10415160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1640,9 +1641,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>736920</xdr:colOff>
+      <xdr:colOff>736560</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>311400</xdr:rowOff>
+      <xdr:rowOff>311040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1652,7 +1653,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="513000" y="0"/>
-          <a:ext cx="24369480" cy="10415520"/>
+          <a:ext cx="25083720" cy="10415160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1685,9 +1686,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>736920</xdr:colOff>
+      <xdr:colOff>736560</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>311400</xdr:rowOff>
+      <xdr:rowOff>311040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1697,7 +1698,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="513000" y="0"/>
-          <a:ext cx="24369480" cy="10415520"/>
+          <a:ext cx="25083720" cy="10415160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1732,50 +1733,50 @@
   </sheetPr>
   <dimension ref="1:49"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="H29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="43:49"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="H14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="N25" activeCellId="0" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.5674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="51.0697674418605"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="51.0697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="33.5953488372093"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="40.3627906976744"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="23.8744186046512"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="32.2418604651163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="49.9627906976744"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="53.0418604651163"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="31.6279069767442"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="2" width="35.4418604651163"/>
-    <col collapsed="false" hidden="false" max="21" min="19" style="2" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="24" min="22" style="2" width="24.1209302325581"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="31.6279069767442"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="32.6093023255814"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="2" width="49.5953488372093"/>
-    <col collapsed="false" hidden="false" max="30" min="28" style="2" width="30.5209302325581"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="24.9813953488372"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="3" width="22.6418604651163"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="2" width="26.3348837209302"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="2" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="2" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="2" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="40" min="38" style="2" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="1" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="2" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="2" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="2" width="31.6279069767442"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="2" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="46" style="1" width="17.9674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="21.0418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.1813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="52.6697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="52.6697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="34.5813953488372"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="41.5953488372093"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="24.4883720930233"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="33.2279069767442"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="51.4418604651163"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="54.5162790697674"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="2" width="36.5488372093023"/>
+    <col collapsed="false" hidden="false" max="21" min="19" style="2" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="24" min="22" style="2" width="24.8604651162791"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="33.5953488372093"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="2" width="51.0697674418605"/>
+    <col collapsed="false" hidden="false" max="30" min="28" style="2" width="31.3813953488372"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="3" width="23.2604651162791"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="2" width="27.0744186046512"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="2" width="38.5162790697674"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="2" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="2" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="40" min="38" style="2" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="1" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="2" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="2" width="26.3348837209302"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="2" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="2" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="46" style="1" width="18.4604651162791"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41440,6 +41441,985 @@
       </c>
       <c r="AR39" s="36"/>
       <c r="AS39" s="30"/>
+      <c r="AT39" s="0"/>
+      <c r="AU39" s="0"/>
+      <c r="AV39" s="0"/>
+      <c r="AW39" s="0"/>
+      <c r="AX39" s="0"/>
+      <c r="AY39" s="0"/>
+      <c r="AZ39" s="0"/>
+      <c r="BA39" s="0"/>
+      <c r="BB39" s="0"/>
+      <c r="BC39" s="0"/>
+      <c r="BD39" s="0"/>
+      <c r="BE39" s="0"/>
+      <c r="BF39" s="0"/>
+      <c r="BG39" s="0"/>
+      <c r="BH39" s="0"/>
+      <c r="BI39" s="0"/>
+      <c r="BJ39" s="0"/>
+      <c r="BK39" s="0"/>
+      <c r="BL39" s="0"/>
+      <c r="BM39" s="0"/>
+      <c r="BN39" s="0"/>
+      <c r="BO39" s="0"/>
+      <c r="BP39" s="0"/>
+      <c r="BQ39" s="0"/>
+      <c r="BR39" s="0"/>
+      <c r="BS39" s="0"/>
+      <c r="BT39" s="0"/>
+      <c r="BU39" s="0"/>
+      <c r="BV39" s="0"/>
+      <c r="BW39" s="0"/>
+      <c r="BX39" s="0"/>
+      <c r="BY39" s="0"/>
+      <c r="BZ39" s="0"/>
+      <c r="CA39" s="0"/>
+      <c r="CB39" s="0"/>
+      <c r="CC39" s="0"/>
+      <c r="CD39" s="0"/>
+      <c r="CE39" s="0"/>
+      <c r="CF39" s="0"/>
+      <c r="CG39" s="0"/>
+      <c r="CH39" s="0"/>
+      <c r="CI39" s="0"/>
+      <c r="CJ39" s="0"/>
+      <c r="CK39" s="0"/>
+      <c r="CL39" s="0"/>
+      <c r="CM39" s="0"/>
+      <c r="CN39" s="0"/>
+      <c r="CO39" s="0"/>
+      <c r="CP39" s="0"/>
+      <c r="CQ39" s="0"/>
+      <c r="CR39" s="0"/>
+      <c r="CS39" s="0"/>
+      <c r="CT39" s="0"/>
+      <c r="CU39" s="0"/>
+      <c r="CV39" s="0"/>
+      <c r="CW39" s="0"/>
+      <c r="CX39" s="0"/>
+      <c r="CY39" s="0"/>
+      <c r="CZ39" s="0"/>
+      <c r="DA39" s="0"/>
+      <c r="DB39" s="0"/>
+      <c r="DC39" s="0"/>
+      <c r="DD39" s="0"/>
+      <c r="DE39" s="0"/>
+      <c r="DF39" s="0"/>
+      <c r="DG39" s="0"/>
+      <c r="DH39" s="0"/>
+      <c r="DI39" s="0"/>
+      <c r="DJ39" s="0"/>
+      <c r="DK39" s="0"/>
+      <c r="DL39" s="0"/>
+      <c r="DM39" s="0"/>
+      <c r="DN39" s="0"/>
+      <c r="DO39" s="0"/>
+      <c r="DP39" s="0"/>
+      <c r="DQ39" s="0"/>
+      <c r="DR39" s="0"/>
+      <c r="DS39" s="0"/>
+      <c r="DT39" s="0"/>
+      <c r="DU39" s="0"/>
+      <c r="DV39" s="0"/>
+      <c r="DW39" s="0"/>
+      <c r="DX39" s="0"/>
+      <c r="DY39" s="0"/>
+      <c r="DZ39" s="0"/>
+      <c r="EA39" s="0"/>
+      <c r="EB39" s="0"/>
+      <c r="EC39" s="0"/>
+      <c r="ED39" s="0"/>
+      <c r="EE39" s="0"/>
+      <c r="EF39" s="0"/>
+      <c r="EG39" s="0"/>
+      <c r="EH39" s="0"/>
+      <c r="EI39" s="0"/>
+      <c r="EJ39" s="0"/>
+      <c r="EK39" s="0"/>
+      <c r="EL39" s="0"/>
+      <c r="EM39" s="0"/>
+      <c r="EN39" s="0"/>
+      <c r="EO39" s="0"/>
+      <c r="EP39" s="0"/>
+      <c r="EQ39" s="0"/>
+      <c r="ER39" s="0"/>
+      <c r="ES39" s="0"/>
+      <c r="ET39" s="0"/>
+      <c r="EU39" s="0"/>
+      <c r="EV39" s="0"/>
+      <c r="EW39" s="0"/>
+      <c r="EX39" s="0"/>
+      <c r="EY39" s="0"/>
+      <c r="EZ39" s="0"/>
+      <c r="FA39" s="0"/>
+      <c r="FB39" s="0"/>
+      <c r="FC39" s="0"/>
+      <c r="FD39" s="0"/>
+      <c r="FE39" s="0"/>
+      <c r="FF39" s="0"/>
+      <c r="FG39" s="0"/>
+      <c r="FH39" s="0"/>
+      <c r="FI39" s="0"/>
+      <c r="FJ39" s="0"/>
+      <c r="FK39" s="0"/>
+      <c r="FL39" s="0"/>
+      <c r="FM39" s="0"/>
+      <c r="FN39" s="0"/>
+      <c r="FO39" s="0"/>
+      <c r="FP39" s="0"/>
+      <c r="FQ39" s="0"/>
+      <c r="FR39" s="0"/>
+      <c r="FS39" s="0"/>
+      <c r="FT39" s="0"/>
+      <c r="FU39" s="0"/>
+      <c r="FV39" s="0"/>
+      <c r="FW39" s="0"/>
+      <c r="FX39" s="0"/>
+      <c r="FY39" s="0"/>
+      <c r="FZ39" s="0"/>
+      <c r="GA39" s="0"/>
+      <c r="GB39" s="0"/>
+      <c r="GC39" s="0"/>
+      <c r="GD39" s="0"/>
+      <c r="GE39" s="0"/>
+      <c r="GF39" s="0"/>
+      <c r="GG39" s="0"/>
+      <c r="GH39" s="0"/>
+      <c r="GI39" s="0"/>
+      <c r="GJ39" s="0"/>
+      <c r="GK39" s="0"/>
+      <c r="GL39" s="0"/>
+      <c r="GM39" s="0"/>
+      <c r="GN39" s="0"/>
+      <c r="GO39" s="0"/>
+      <c r="GP39" s="0"/>
+      <c r="GQ39" s="0"/>
+      <c r="GR39" s="0"/>
+      <c r="GS39" s="0"/>
+      <c r="GT39" s="0"/>
+      <c r="GU39" s="0"/>
+      <c r="GV39" s="0"/>
+      <c r="GW39" s="0"/>
+      <c r="GX39" s="0"/>
+      <c r="GY39" s="0"/>
+      <c r="GZ39" s="0"/>
+      <c r="HA39" s="0"/>
+      <c r="HB39" s="0"/>
+      <c r="HC39" s="0"/>
+      <c r="HD39" s="0"/>
+      <c r="HE39" s="0"/>
+      <c r="HF39" s="0"/>
+      <c r="HG39" s="0"/>
+      <c r="HH39" s="0"/>
+      <c r="HI39" s="0"/>
+      <c r="HJ39" s="0"/>
+      <c r="HK39" s="0"/>
+      <c r="HL39" s="0"/>
+      <c r="HM39" s="0"/>
+      <c r="HN39" s="0"/>
+      <c r="HO39" s="0"/>
+      <c r="HP39" s="0"/>
+      <c r="HQ39" s="0"/>
+      <c r="HR39" s="0"/>
+      <c r="HS39" s="0"/>
+      <c r="HT39" s="0"/>
+      <c r="HU39" s="0"/>
+      <c r="HV39" s="0"/>
+      <c r="HW39" s="0"/>
+      <c r="HX39" s="0"/>
+      <c r="HY39" s="0"/>
+      <c r="HZ39" s="0"/>
+      <c r="IA39" s="0"/>
+      <c r="IB39" s="0"/>
+      <c r="IC39" s="0"/>
+      <c r="ID39" s="0"/>
+      <c r="IE39" s="0"/>
+      <c r="IF39" s="0"/>
+      <c r="IG39" s="0"/>
+      <c r="IH39" s="0"/>
+      <c r="II39" s="0"/>
+      <c r="IJ39" s="0"/>
+      <c r="IK39" s="0"/>
+      <c r="IL39" s="0"/>
+      <c r="IM39" s="0"/>
+      <c r="IN39" s="0"/>
+      <c r="IO39" s="0"/>
+      <c r="IP39" s="0"/>
+      <c r="IQ39" s="0"/>
+      <c r="IR39" s="0"/>
+      <c r="IS39" s="0"/>
+      <c r="IT39" s="0"/>
+      <c r="IU39" s="0"/>
+      <c r="IV39" s="0"/>
+      <c r="IW39" s="0"/>
+      <c r="IX39" s="0"/>
+      <c r="IY39" s="0"/>
+      <c r="IZ39" s="0"/>
+      <c r="JA39" s="0"/>
+      <c r="JB39" s="0"/>
+      <c r="JC39" s="0"/>
+      <c r="JD39" s="0"/>
+      <c r="JE39" s="0"/>
+      <c r="JF39" s="0"/>
+      <c r="JG39" s="0"/>
+      <c r="JH39" s="0"/>
+      <c r="JI39" s="0"/>
+      <c r="JJ39" s="0"/>
+      <c r="JK39" s="0"/>
+      <c r="JL39" s="0"/>
+      <c r="JM39" s="0"/>
+      <c r="JN39" s="0"/>
+      <c r="JO39" s="0"/>
+      <c r="JP39" s="0"/>
+      <c r="JQ39" s="0"/>
+      <c r="JR39" s="0"/>
+      <c r="JS39" s="0"/>
+      <c r="JT39" s="0"/>
+      <c r="JU39" s="0"/>
+      <c r="JV39" s="0"/>
+      <c r="JW39" s="0"/>
+      <c r="JX39" s="0"/>
+      <c r="JY39" s="0"/>
+      <c r="JZ39" s="0"/>
+      <c r="KA39" s="0"/>
+      <c r="KB39" s="0"/>
+      <c r="KC39" s="0"/>
+      <c r="KD39" s="0"/>
+      <c r="KE39" s="0"/>
+      <c r="KF39" s="0"/>
+      <c r="KG39" s="0"/>
+      <c r="KH39" s="0"/>
+      <c r="KI39" s="0"/>
+      <c r="KJ39" s="0"/>
+      <c r="KK39" s="0"/>
+      <c r="KL39" s="0"/>
+      <c r="KM39" s="0"/>
+      <c r="KN39" s="0"/>
+      <c r="KO39" s="0"/>
+      <c r="KP39" s="0"/>
+      <c r="KQ39" s="0"/>
+      <c r="KR39" s="0"/>
+      <c r="KS39" s="0"/>
+      <c r="KT39" s="0"/>
+      <c r="KU39" s="0"/>
+      <c r="KV39" s="0"/>
+      <c r="KW39" s="0"/>
+      <c r="KX39" s="0"/>
+      <c r="KY39" s="0"/>
+      <c r="KZ39" s="0"/>
+      <c r="LA39" s="0"/>
+      <c r="LB39" s="0"/>
+      <c r="LC39" s="0"/>
+      <c r="LD39" s="0"/>
+      <c r="LE39" s="0"/>
+      <c r="LF39" s="0"/>
+      <c r="LG39" s="0"/>
+      <c r="LH39" s="0"/>
+      <c r="LI39" s="0"/>
+      <c r="LJ39" s="0"/>
+      <c r="LK39" s="0"/>
+      <c r="LL39" s="0"/>
+      <c r="LM39" s="0"/>
+      <c r="LN39" s="0"/>
+      <c r="LO39" s="0"/>
+      <c r="LP39" s="0"/>
+      <c r="LQ39" s="0"/>
+      <c r="LR39" s="0"/>
+      <c r="LS39" s="0"/>
+      <c r="LT39" s="0"/>
+      <c r="LU39" s="0"/>
+      <c r="LV39" s="0"/>
+      <c r="LW39" s="0"/>
+      <c r="LX39" s="0"/>
+      <c r="LY39" s="0"/>
+      <c r="LZ39" s="0"/>
+      <c r="MA39" s="0"/>
+      <c r="MB39" s="0"/>
+      <c r="MC39" s="0"/>
+      <c r="MD39" s="0"/>
+      <c r="ME39" s="0"/>
+      <c r="MF39" s="0"/>
+      <c r="MG39" s="0"/>
+      <c r="MH39" s="0"/>
+      <c r="MI39" s="0"/>
+      <c r="MJ39" s="0"/>
+      <c r="MK39" s="0"/>
+      <c r="ML39" s="0"/>
+      <c r="MM39" s="0"/>
+      <c r="MN39" s="0"/>
+      <c r="MO39" s="0"/>
+      <c r="MP39" s="0"/>
+      <c r="MQ39" s="0"/>
+      <c r="MR39" s="0"/>
+      <c r="MS39" s="0"/>
+      <c r="MT39" s="0"/>
+      <c r="MU39" s="0"/>
+      <c r="MV39" s="0"/>
+      <c r="MW39" s="0"/>
+      <c r="MX39" s="0"/>
+      <c r="MY39" s="0"/>
+      <c r="MZ39" s="0"/>
+      <c r="NA39" s="0"/>
+      <c r="NB39" s="0"/>
+      <c r="NC39" s="0"/>
+      <c r="ND39" s="0"/>
+      <c r="NE39" s="0"/>
+      <c r="NF39" s="0"/>
+      <c r="NG39" s="0"/>
+      <c r="NH39" s="0"/>
+      <c r="NI39" s="0"/>
+      <c r="NJ39" s="0"/>
+      <c r="NK39" s="0"/>
+      <c r="NL39" s="0"/>
+      <c r="NM39" s="0"/>
+      <c r="NN39" s="0"/>
+      <c r="NO39" s="0"/>
+      <c r="NP39" s="0"/>
+      <c r="NQ39" s="0"/>
+      <c r="NR39" s="0"/>
+      <c r="NS39" s="0"/>
+      <c r="NT39" s="0"/>
+      <c r="NU39" s="0"/>
+      <c r="NV39" s="0"/>
+      <c r="NW39" s="0"/>
+      <c r="NX39" s="0"/>
+      <c r="NY39" s="0"/>
+      <c r="NZ39" s="0"/>
+      <c r="OA39" s="0"/>
+      <c r="OB39" s="0"/>
+      <c r="OC39" s="0"/>
+      <c r="OD39" s="0"/>
+      <c r="OE39" s="0"/>
+      <c r="OF39" s="0"/>
+      <c r="OG39" s="0"/>
+      <c r="OH39" s="0"/>
+      <c r="OI39" s="0"/>
+      <c r="OJ39" s="0"/>
+      <c r="OK39" s="0"/>
+      <c r="OL39" s="0"/>
+      <c r="OM39" s="0"/>
+      <c r="ON39" s="0"/>
+      <c r="OO39" s="0"/>
+      <c r="OP39" s="0"/>
+      <c r="OQ39" s="0"/>
+      <c r="OR39" s="0"/>
+      <c r="OS39" s="0"/>
+      <c r="OT39" s="0"/>
+      <c r="OU39" s="0"/>
+      <c r="OV39" s="0"/>
+      <c r="OW39" s="0"/>
+      <c r="OX39" s="0"/>
+      <c r="OY39" s="0"/>
+      <c r="OZ39" s="0"/>
+      <c r="PA39" s="0"/>
+      <c r="PB39" s="0"/>
+      <c r="PC39" s="0"/>
+      <c r="PD39" s="0"/>
+      <c r="PE39" s="0"/>
+      <c r="PF39" s="0"/>
+      <c r="PG39" s="0"/>
+      <c r="PH39" s="0"/>
+      <c r="PI39" s="0"/>
+      <c r="PJ39" s="0"/>
+      <c r="PK39" s="0"/>
+      <c r="PL39" s="0"/>
+      <c r="PM39" s="0"/>
+      <c r="PN39" s="0"/>
+      <c r="PO39" s="0"/>
+      <c r="PP39" s="0"/>
+      <c r="PQ39" s="0"/>
+      <c r="PR39" s="0"/>
+      <c r="PS39" s="0"/>
+      <c r="PT39" s="0"/>
+      <c r="PU39" s="0"/>
+      <c r="PV39" s="0"/>
+      <c r="PW39" s="0"/>
+      <c r="PX39" s="0"/>
+      <c r="PY39" s="0"/>
+      <c r="PZ39" s="0"/>
+      <c r="QA39" s="0"/>
+      <c r="QB39" s="0"/>
+      <c r="QC39" s="0"/>
+      <c r="QD39" s="0"/>
+      <c r="QE39" s="0"/>
+      <c r="QF39" s="0"/>
+      <c r="QG39" s="0"/>
+      <c r="QH39" s="0"/>
+      <c r="QI39" s="0"/>
+      <c r="QJ39" s="0"/>
+      <c r="QK39" s="0"/>
+      <c r="QL39" s="0"/>
+      <c r="QM39" s="0"/>
+      <c r="QN39" s="0"/>
+      <c r="QO39" s="0"/>
+      <c r="QP39" s="0"/>
+      <c r="QQ39" s="0"/>
+      <c r="QR39" s="0"/>
+      <c r="QS39" s="0"/>
+      <c r="QT39" s="0"/>
+      <c r="QU39" s="0"/>
+      <c r="QV39" s="0"/>
+      <c r="QW39" s="0"/>
+      <c r="QX39" s="0"/>
+      <c r="QY39" s="0"/>
+      <c r="QZ39" s="0"/>
+      <c r="RA39" s="0"/>
+      <c r="RB39" s="0"/>
+      <c r="RC39" s="0"/>
+      <c r="RD39" s="0"/>
+      <c r="RE39" s="0"/>
+      <c r="RF39" s="0"/>
+      <c r="RG39" s="0"/>
+      <c r="RH39" s="0"/>
+      <c r="RI39" s="0"/>
+      <c r="RJ39" s="0"/>
+      <c r="RK39" s="0"/>
+      <c r="RL39" s="0"/>
+      <c r="RM39" s="0"/>
+      <c r="RN39" s="0"/>
+      <c r="RO39" s="0"/>
+      <c r="RP39" s="0"/>
+      <c r="RQ39" s="0"/>
+      <c r="RR39" s="0"/>
+      <c r="RS39" s="0"/>
+      <c r="RT39" s="0"/>
+      <c r="RU39" s="0"/>
+      <c r="RV39" s="0"/>
+      <c r="RW39" s="0"/>
+      <c r="RX39" s="0"/>
+      <c r="RY39" s="0"/>
+      <c r="RZ39" s="0"/>
+      <c r="SA39" s="0"/>
+      <c r="SB39" s="0"/>
+      <c r="SC39" s="0"/>
+      <c r="SD39" s="0"/>
+      <c r="SE39" s="0"/>
+      <c r="SF39" s="0"/>
+      <c r="SG39" s="0"/>
+      <c r="SH39" s="0"/>
+      <c r="SI39" s="0"/>
+      <c r="SJ39" s="0"/>
+      <c r="SK39" s="0"/>
+      <c r="SL39" s="0"/>
+      <c r="SM39" s="0"/>
+      <c r="SN39" s="0"/>
+      <c r="SO39" s="0"/>
+      <c r="SP39" s="0"/>
+      <c r="SQ39" s="0"/>
+      <c r="SR39" s="0"/>
+      <c r="SS39" s="0"/>
+      <c r="ST39" s="0"/>
+      <c r="SU39" s="0"/>
+      <c r="SV39" s="0"/>
+      <c r="SW39" s="0"/>
+      <c r="SX39" s="0"/>
+      <c r="SY39" s="0"/>
+      <c r="SZ39" s="0"/>
+      <c r="TA39" s="0"/>
+      <c r="TB39" s="0"/>
+      <c r="TC39" s="0"/>
+      <c r="TD39" s="0"/>
+      <c r="TE39" s="0"/>
+      <c r="TF39" s="0"/>
+      <c r="TG39" s="0"/>
+      <c r="TH39" s="0"/>
+      <c r="TI39" s="0"/>
+      <c r="TJ39" s="0"/>
+      <c r="TK39" s="0"/>
+      <c r="TL39" s="0"/>
+      <c r="TM39" s="0"/>
+      <c r="TN39" s="0"/>
+      <c r="TO39" s="0"/>
+      <c r="TP39" s="0"/>
+      <c r="TQ39" s="0"/>
+      <c r="TR39" s="0"/>
+      <c r="TS39" s="0"/>
+      <c r="TT39" s="0"/>
+      <c r="TU39" s="0"/>
+      <c r="TV39" s="0"/>
+      <c r="TW39" s="0"/>
+      <c r="TX39" s="0"/>
+      <c r="TY39" s="0"/>
+      <c r="TZ39" s="0"/>
+      <c r="UA39" s="0"/>
+      <c r="UB39" s="0"/>
+      <c r="UC39" s="0"/>
+      <c r="UD39" s="0"/>
+      <c r="UE39" s="0"/>
+      <c r="UF39" s="0"/>
+      <c r="UG39" s="0"/>
+      <c r="UH39" s="0"/>
+      <c r="UI39" s="0"/>
+      <c r="UJ39" s="0"/>
+      <c r="UK39" s="0"/>
+      <c r="UL39" s="0"/>
+      <c r="UM39" s="0"/>
+      <c r="UN39" s="0"/>
+      <c r="UO39" s="0"/>
+      <c r="UP39" s="0"/>
+      <c r="UQ39" s="0"/>
+      <c r="UR39" s="0"/>
+      <c r="US39" s="0"/>
+      <c r="UT39" s="0"/>
+      <c r="UU39" s="0"/>
+      <c r="UV39" s="0"/>
+      <c r="UW39" s="0"/>
+      <c r="UX39" s="0"/>
+      <c r="UY39" s="0"/>
+      <c r="UZ39" s="0"/>
+      <c r="VA39" s="0"/>
+      <c r="VB39" s="0"/>
+      <c r="VC39" s="0"/>
+      <c r="VD39" s="0"/>
+      <c r="VE39" s="0"/>
+      <c r="VF39" s="0"/>
+      <c r="VG39" s="0"/>
+      <c r="VH39" s="0"/>
+      <c r="VI39" s="0"/>
+      <c r="VJ39" s="0"/>
+      <c r="VK39" s="0"/>
+      <c r="VL39" s="0"/>
+      <c r="VM39" s="0"/>
+      <c r="VN39" s="0"/>
+      <c r="VO39" s="0"/>
+      <c r="VP39" s="0"/>
+      <c r="VQ39" s="0"/>
+      <c r="VR39" s="0"/>
+      <c r="VS39" s="0"/>
+      <c r="VT39" s="0"/>
+      <c r="VU39" s="0"/>
+      <c r="VV39" s="0"/>
+      <c r="VW39" s="0"/>
+      <c r="VX39" s="0"/>
+      <c r="VY39" s="0"/>
+      <c r="VZ39" s="0"/>
+      <c r="WA39" s="0"/>
+      <c r="WB39" s="0"/>
+      <c r="WC39" s="0"/>
+      <c r="WD39" s="0"/>
+      <c r="WE39" s="0"/>
+      <c r="WF39" s="0"/>
+      <c r="WG39" s="0"/>
+      <c r="WH39" s="0"/>
+      <c r="WI39" s="0"/>
+      <c r="WJ39" s="0"/>
+      <c r="WK39" s="0"/>
+      <c r="WL39" s="0"/>
+      <c r="WM39" s="0"/>
+      <c r="WN39" s="0"/>
+      <c r="WO39" s="0"/>
+      <c r="WP39" s="0"/>
+      <c r="WQ39" s="0"/>
+      <c r="WR39" s="0"/>
+      <c r="WS39" s="0"/>
+      <c r="WT39" s="0"/>
+      <c r="WU39" s="0"/>
+      <c r="WV39" s="0"/>
+      <c r="WW39" s="0"/>
+      <c r="WX39" s="0"/>
+      <c r="WY39" s="0"/>
+      <c r="WZ39" s="0"/>
+      <c r="XA39" s="0"/>
+      <c r="XB39" s="0"/>
+      <c r="XC39" s="0"/>
+      <c r="XD39" s="0"/>
+      <c r="XE39" s="0"/>
+      <c r="XF39" s="0"/>
+      <c r="XG39" s="0"/>
+      <c r="XH39" s="0"/>
+      <c r="XI39" s="0"/>
+      <c r="XJ39" s="0"/>
+      <c r="XK39" s="0"/>
+      <c r="XL39" s="0"/>
+      <c r="XM39" s="0"/>
+      <c r="XN39" s="0"/>
+      <c r="XO39" s="0"/>
+      <c r="XP39" s="0"/>
+      <c r="XQ39" s="0"/>
+      <c r="XR39" s="0"/>
+      <c r="XS39" s="0"/>
+      <c r="XT39" s="0"/>
+      <c r="XU39" s="0"/>
+      <c r="XV39" s="0"/>
+      <c r="XW39" s="0"/>
+      <c r="XX39" s="0"/>
+      <c r="XY39" s="0"/>
+      <c r="XZ39" s="0"/>
+      <c r="YA39" s="0"/>
+      <c r="YB39" s="0"/>
+      <c r="YC39" s="0"/>
+      <c r="YD39" s="0"/>
+      <c r="YE39" s="0"/>
+      <c r="YF39" s="0"/>
+      <c r="YG39" s="0"/>
+      <c r="YH39" s="0"/>
+      <c r="YI39" s="0"/>
+      <c r="YJ39" s="0"/>
+      <c r="YK39" s="0"/>
+      <c r="YL39" s="0"/>
+      <c r="YM39" s="0"/>
+      <c r="YN39" s="0"/>
+      <c r="YO39" s="0"/>
+      <c r="YP39" s="0"/>
+      <c r="YQ39" s="0"/>
+      <c r="YR39" s="0"/>
+      <c r="YS39" s="0"/>
+      <c r="YT39" s="0"/>
+      <c r="YU39" s="0"/>
+      <c r="YV39" s="0"/>
+      <c r="YW39" s="0"/>
+      <c r="YX39" s="0"/>
+      <c r="YY39" s="0"/>
+      <c r="YZ39" s="0"/>
+      <c r="ZA39" s="0"/>
+      <c r="ZB39" s="0"/>
+      <c r="ZC39" s="0"/>
+      <c r="ZD39" s="0"/>
+      <c r="ZE39" s="0"/>
+      <c r="ZF39" s="0"/>
+      <c r="ZG39" s="0"/>
+      <c r="ZH39" s="0"/>
+      <c r="ZI39" s="0"/>
+      <c r="ZJ39" s="0"/>
+      <c r="ZK39" s="0"/>
+      <c r="ZL39" s="0"/>
+      <c r="ZM39" s="0"/>
+      <c r="ZN39" s="0"/>
+      <c r="ZO39" s="0"/>
+      <c r="ZP39" s="0"/>
+      <c r="ZQ39" s="0"/>
+      <c r="ZR39" s="0"/>
+      <c r="ZS39" s="0"/>
+      <c r="ZT39" s="0"/>
+      <c r="ZU39" s="0"/>
+      <c r="ZV39" s="0"/>
+      <c r="ZW39" s="0"/>
+      <c r="ZX39" s="0"/>
+      <c r="ZY39" s="0"/>
+      <c r="ZZ39" s="0"/>
+      <c r="AAA39" s="0"/>
+      <c r="AAB39" s="0"/>
+      <c r="AAC39" s="0"/>
+      <c r="AAD39" s="0"/>
+      <c r="AAE39" s="0"/>
+      <c r="AAF39" s="0"/>
+      <c r="AAG39" s="0"/>
+      <c r="AAH39" s="0"/>
+      <c r="AAI39" s="0"/>
+      <c r="AAJ39" s="0"/>
+      <c r="AAK39" s="0"/>
+      <c r="AAL39" s="0"/>
+      <c r="AAM39" s="0"/>
+      <c r="AAN39" s="0"/>
+      <c r="AAO39" s="0"/>
+      <c r="AAP39" s="0"/>
+      <c r="AAQ39" s="0"/>
+      <c r="AAR39" s="0"/>
+      <c r="AAS39" s="0"/>
+      <c r="AAT39" s="0"/>
+      <c r="AAU39" s="0"/>
+      <c r="AAV39" s="0"/>
+      <c r="AAW39" s="0"/>
+      <c r="AAX39" s="0"/>
+      <c r="AAY39" s="0"/>
+      <c r="AAZ39" s="0"/>
+      <c r="ABA39" s="0"/>
+      <c r="ABB39" s="0"/>
+      <c r="ABC39" s="0"/>
+      <c r="ABD39" s="0"/>
+      <c r="ABE39" s="0"/>
+      <c r="ABF39" s="0"/>
+      <c r="ABG39" s="0"/>
+      <c r="ABH39" s="0"/>
+      <c r="ABI39" s="0"/>
+      <c r="ABJ39" s="0"/>
+      <c r="ABK39" s="0"/>
+      <c r="ABL39" s="0"/>
+      <c r="ABM39" s="0"/>
+      <c r="ABN39" s="0"/>
+      <c r="ABO39" s="0"/>
+      <c r="ABP39" s="0"/>
+      <c r="ABQ39" s="0"/>
+      <c r="ABR39" s="0"/>
+      <c r="ABS39" s="0"/>
+      <c r="ABT39" s="0"/>
+      <c r="ABU39" s="0"/>
+      <c r="ABV39" s="0"/>
+      <c r="ABW39" s="0"/>
+      <c r="ABX39" s="0"/>
+      <c r="ABY39" s="0"/>
+      <c r="ABZ39" s="0"/>
+      <c r="ACA39" s="0"/>
+      <c r="ACB39" s="0"/>
+      <c r="ACC39" s="0"/>
+      <c r="ACD39" s="0"/>
+      <c r="ACE39" s="0"/>
+      <c r="ACF39" s="0"/>
+      <c r="ACG39" s="0"/>
+      <c r="ACH39" s="0"/>
+      <c r="ACI39" s="0"/>
+      <c r="ACJ39" s="0"/>
+      <c r="ACK39" s="0"/>
+      <c r="ACL39" s="0"/>
+      <c r="ACM39" s="0"/>
+      <c r="ACN39" s="0"/>
+      <c r="ACO39" s="0"/>
+      <c r="ACP39" s="0"/>
+      <c r="ACQ39" s="0"/>
+      <c r="ACR39" s="0"/>
+      <c r="ACS39" s="0"/>
+      <c r="ACT39" s="0"/>
+      <c r="ACU39" s="0"/>
+      <c r="ACV39" s="0"/>
+      <c r="ACW39" s="0"/>
+      <c r="ACX39" s="0"/>
+      <c r="ACY39" s="0"/>
+      <c r="ACZ39" s="0"/>
+      <c r="ADA39" s="0"/>
+      <c r="ADB39" s="0"/>
+      <c r="ADC39" s="0"/>
+      <c r="ADD39" s="0"/>
+      <c r="ADE39" s="0"/>
+      <c r="ADF39" s="0"/>
+      <c r="ADG39" s="0"/>
+      <c r="ADH39" s="0"/>
+      <c r="ADI39" s="0"/>
+      <c r="ADJ39" s="0"/>
+      <c r="ADK39" s="0"/>
+      <c r="ADL39" s="0"/>
+      <c r="ADM39" s="0"/>
+      <c r="ADN39" s="0"/>
+      <c r="ADO39" s="0"/>
+      <c r="ADP39" s="0"/>
+      <c r="ADQ39" s="0"/>
+      <c r="ADR39" s="0"/>
+      <c r="ADS39" s="0"/>
+      <c r="ADT39" s="0"/>
+      <c r="ADU39" s="0"/>
+      <c r="ADV39" s="0"/>
+      <c r="ADW39" s="0"/>
+      <c r="ADX39" s="0"/>
+      <c r="ADY39" s="0"/>
+      <c r="ADZ39" s="0"/>
+      <c r="AEA39" s="0"/>
+      <c r="AEB39" s="0"/>
+      <c r="AEC39" s="0"/>
+      <c r="AED39" s="0"/>
+      <c r="AEE39" s="0"/>
+      <c r="AEF39" s="0"/>
+      <c r="AEG39" s="0"/>
+      <c r="AEH39" s="0"/>
+      <c r="AEI39" s="0"/>
+      <c r="AEJ39" s="0"/>
+      <c r="AEK39" s="0"/>
+      <c r="AEL39" s="0"/>
+      <c r="AEM39" s="0"/>
+      <c r="AEN39" s="0"/>
+      <c r="AEO39" s="0"/>
+      <c r="AEP39" s="0"/>
+      <c r="AEQ39" s="0"/>
+      <c r="AER39" s="0"/>
+      <c r="AES39" s="0"/>
+      <c r="AET39" s="0"/>
+      <c r="AEU39" s="0"/>
+      <c r="AEV39" s="0"/>
+      <c r="AEW39" s="0"/>
+      <c r="AEX39" s="0"/>
+      <c r="AEY39" s="0"/>
+      <c r="AEZ39" s="0"/>
+      <c r="AFA39" s="0"/>
+      <c r="AFB39" s="0"/>
+      <c r="AFC39" s="0"/>
+      <c r="AFD39" s="0"/>
+      <c r="AFE39" s="0"/>
+      <c r="AFF39" s="0"/>
+      <c r="AFG39" s="0"/>
+      <c r="AFH39" s="0"/>
+      <c r="AFI39" s="0"/>
+      <c r="AFJ39" s="0"/>
+      <c r="AFK39" s="0"/>
+      <c r="AFL39" s="0"/>
+      <c r="AFM39" s="0"/>
+      <c r="AFN39" s="0"/>
+      <c r="AFO39" s="0"/>
+      <c r="AFP39" s="0"/>
+      <c r="AFQ39" s="0"/>
+      <c r="AFR39" s="0"/>
+      <c r="AFS39" s="0"/>
+      <c r="AFT39" s="0"/>
+      <c r="AFU39" s="0"/>
+      <c r="AFV39" s="0"/>
+      <c r="AFW39" s="0"/>
+      <c r="AFX39" s="0"/>
+      <c r="AFY39" s="0"/>
+      <c r="AFZ39" s="0"/>
+      <c r="AGA39" s="0"/>
+      <c r="AGB39" s="0"/>
+      <c r="AGC39" s="0"/>
+      <c r="AGD39" s="0"/>
+      <c r="AGE39" s="0"/>
+      <c r="AGF39" s="0"/>
+      <c r="AGG39" s="0"/>
+      <c r="AGH39" s="0"/>
+      <c r="AGI39" s="0"/>
+      <c r="AGJ39" s="0"/>
+      <c r="AGK39" s="0"/>
+      <c r="AGL39" s="0"/>
+      <c r="AGM39" s="0"/>
+      <c r="AGN39" s="0"/>
+      <c r="AGO39" s="0"/>
+      <c r="AGP39" s="0"/>
+      <c r="AGQ39" s="0"/>
+      <c r="AGR39" s="0"/>
+      <c r="AGS39" s="0"/>
+      <c r="AGT39" s="0"/>
+      <c r="AGU39" s="0"/>
+      <c r="AGV39" s="0"/>
+      <c r="AGW39" s="0"/>
+      <c r="AGX39" s="0"/>
+      <c r="AGY39" s="0"/>
+      <c r="AGZ39" s="0"/>
+      <c r="AHA39" s="0"/>
+      <c r="AHB39" s="0"/>
+      <c r="AHC39" s="0"/>
+      <c r="AHD39" s="0"/>
+      <c r="AHE39" s="0"/>
+      <c r="AHF39" s="0"/>
+      <c r="AHG39" s="0"/>
+      <c r="AHH39" s="0"/>
+      <c r="AHI39" s="0"/>
+      <c r="AHJ39" s="0"/>
+      <c r="AHK39" s="0"/>
+      <c r="AHL39" s="0"/>
+      <c r="AHM39" s="0"/>
+      <c r="AHN39" s="0"/>
+      <c r="AHO39" s="0"/>
+      <c r="AHP39" s="0"/>
+      <c r="AHQ39" s="0"/>
+      <c r="AHR39" s="0"/>
+      <c r="AHS39" s="0"/>
+      <c r="AHT39" s="0"/>
+      <c r="AHU39" s="0"/>
+      <c r="AHV39" s="0"/>
+      <c r="AHW39" s="0"/>
+      <c r="AHX39" s="0"/>
+      <c r="AHY39" s="0"/>
+      <c r="AHZ39" s="0"/>
+      <c r="AIA39" s="0"/>
+      <c r="AIB39" s="0"/>
+      <c r="AIC39" s="0"/>
+      <c r="AID39" s="0"/>
+      <c r="AIE39" s="0"/>
+      <c r="AIF39" s="0"/>
+      <c r="AIG39" s="0"/>
+      <c r="AIH39" s="0"/>
+      <c r="AII39" s="0"/>
+      <c r="AIJ39" s="0"/>
+      <c r="AIK39" s="0"/>
+      <c r="AIL39" s="0"/>
+      <c r="AIM39" s="0"/>
+      <c r="AIN39" s="0"/>
+      <c r="AIO39" s="0"/>
+      <c r="AIP39" s="0"/>
+      <c r="AIQ39" s="0"/>
+      <c r="AIR39" s="0"/>
+      <c r="AIS39" s="0"/>
+      <c r="AIT39" s="0"/>
+      <c r="AIU39" s="0"/>
+      <c r="AIV39" s="0"/>
+      <c r="AIW39" s="0"/>
+      <c r="AIX39" s="0"/>
+      <c r="AIY39" s="0"/>
+      <c r="AIZ39" s="0"/>
+      <c r="AJA39" s="0"/>
+      <c r="AJB39" s="0"/>
+      <c r="AJC39" s="0"/>
+      <c r="AJD39" s="0"/>
+      <c r="AJE39" s="0"/>
+      <c r="AJF39" s="0"/>
+      <c r="AJG39" s="0"/>
+      <c r="AJH39" s="0"/>
+      <c r="AJI39" s="0"/>
+      <c r="AJJ39" s="0"/>
+      <c r="AJK39" s="0"/>
+      <c r="AJL39" s="0"/>
+      <c r="AJM39" s="0"/>
+      <c r="AJN39" s="0"/>
+      <c r="AJO39" s="0"/>
+      <c r="AJP39" s="0"/>
+      <c r="AJQ39" s="0"/>
+      <c r="AJR39" s="0"/>
+      <c r="AJS39" s="0"/>
+      <c r="AJT39" s="0"/>
+      <c r="AJU39" s="0"/>
+      <c r="AJV39" s="0"/>
+      <c r="AJW39" s="0"/>
+      <c r="AJX39" s="0"/>
+      <c r="AJY39" s="0"/>
+      <c r="AJZ39" s="0"/>
+      <c r="AKA39" s="0"/>
+      <c r="AKB39" s="0"/>
+      <c r="AKC39" s="0"/>
+      <c r="AKD39" s="0"/>
+      <c r="AKE39" s="0"/>
+      <c r="AKF39" s="0"/>
+      <c r="AKG39" s="0"/>
+      <c r="AKH39" s="0"/>
+      <c r="AKI39" s="0"/>
+      <c r="AKJ39" s="0"/>
+      <c r="AKK39" s="0"/>
+      <c r="AKL39" s="0"/>
+      <c r="AKM39" s="0"/>
+      <c r="AKN39" s="0"/>
+      <c r="AKO39" s="0"/>
+      <c r="AKP39" s="0"/>
+      <c r="AKQ39" s="0"/>
+      <c r="AKR39" s="0"/>
+      <c r="AKS39" s="0"/>
+      <c r="AKT39" s="0"/>
+      <c r="AKU39" s="0"/>
+      <c r="AKV39" s="0"/>
+      <c r="AKW39" s="0"/>
+      <c r="AKX39" s="0"/>
+      <c r="AKY39" s="0"/>
+      <c r="AKZ39" s="0"/>
+      <c r="ALA39" s="0"/>
+      <c r="ALB39" s="0"/>
+      <c r="ALC39" s="0"/>
+      <c r="ALD39" s="0"/>
+      <c r="ALE39" s="0"/>
+      <c r="ALF39" s="0"/>
+      <c r="ALG39" s="0"/>
+      <c r="ALH39" s="0"/>
+      <c r="ALI39" s="0"/>
+      <c r="ALJ39" s="0"/>
+      <c r="ALK39" s="0"/>
+      <c r="ALL39" s="0"/>
+      <c r="ALM39" s="0"/>
+      <c r="ALN39" s="0"/>
+      <c r="ALO39" s="0"/>
+      <c r="ALP39" s="0"/>
+      <c r="ALQ39" s="0"/>
+      <c r="ALR39" s="0"/>
+      <c r="ALS39" s="0"/>
+      <c r="ALT39" s="0"/>
+      <c r="ALU39" s="0"/>
+      <c r="ALV39" s="0"/>
+      <c r="ALW39" s="0"/>
+      <c r="ALX39" s="0"/>
+      <c r="ALY39" s="0"/>
+      <c r="ALZ39" s="0"/>
+      <c r="AMA39" s="0"/>
+      <c r="AMB39" s="0"/>
+      <c r="AMC39" s="0"/>
+      <c r="AMD39" s="0"/>
+      <c r="AME39" s="0"/>
+      <c r="AMF39" s="0"/>
+      <c r="AMG39" s="0"/>
+      <c r="AMH39" s="0"/>
+      <c r="AMI39" s="0"/>
+      <c r="AMJ39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="18" t="n">
@@ -41529,6 +42509,985 @@
       </c>
       <c r="AR40" s="36"/>
       <c r="AS40" s="30"/>
+      <c r="AT40" s="0"/>
+      <c r="AU40" s="0"/>
+      <c r="AV40" s="0"/>
+      <c r="AW40" s="0"/>
+      <c r="AX40" s="0"/>
+      <c r="AY40" s="0"/>
+      <c r="AZ40" s="0"/>
+      <c r="BA40" s="0"/>
+      <c r="BB40" s="0"/>
+      <c r="BC40" s="0"/>
+      <c r="BD40" s="0"/>
+      <c r="BE40" s="0"/>
+      <c r="BF40" s="0"/>
+      <c r="BG40" s="0"/>
+      <c r="BH40" s="0"/>
+      <c r="BI40" s="0"/>
+      <c r="BJ40" s="0"/>
+      <c r="BK40" s="0"/>
+      <c r="BL40" s="0"/>
+      <c r="BM40" s="0"/>
+      <c r="BN40" s="0"/>
+      <c r="BO40" s="0"/>
+      <c r="BP40" s="0"/>
+      <c r="BQ40" s="0"/>
+      <c r="BR40" s="0"/>
+      <c r="BS40" s="0"/>
+      <c r="BT40" s="0"/>
+      <c r="BU40" s="0"/>
+      <c r="BV40" s="0"/>
+      <c r="BW40" s="0"/>
+      <c r="BX40" s="0"/>
+      <c r="BY40" s="0"/>
+      <c r="BZ40" s="0"/>
+      <c r="CA40" s="0"/>
+      <c r="CB40" s="0"/>
+      <c r="CC40" s="0"/>
+      <c r="CD40" s="0"/>
+      <c r="CE40" s="0"/>
+      <c r="CF40" s="0"/>
+      <c r="CG40" s="0"/>
+      <c r="CH40" s="0"/>
+      <c r="CI40" s="0"/>
+      <c r="CJ40" s="0"/>
+      <c r="CK40" s="0"/>
+      <c r="CL40" s="0"/>
+      <c r="CM40" s="0"/>
+      <c r="CN40" s="0"/>
+      <c r="CO40" s="0"/>
+      <c r="CP40" s="0"/>
+      <c r="CQ40" s="0"/>
+      <c r="CR40" s="0"/>
+      <c r="CS40" s="0"/>
+      <c r="CT40" s="0"/>
+      <c r="CU40" s="0"/>
+      <c r="CV40" s="0"/>
+      <c r="CW40" s="0"/>
+      <c r="CX40" s="0"/>
+      <c r="CY40" s="0"/>
+      <c r="CZ40" s="0"/>
+      <c r="DA40" s="0"/>
+      <c r="DB40" s="0"/>
+      <c r="DC40" s="0"/>
+      <c r="DD40" s="0"/>
+      <c r="DE40" s="0"/>
+      <c r="DF40" s="0"/>
+      <c r="DG40" s="0"/>
+      <c r="DH40" s="0"/>
+      <c r="DI40" s="0"/>
+      <c r="DJ40" s="0"/>
+      <c r="DK40" s="0"/>
+      <c r="DL40" s="0"/>
+      <c r="DM40" s="0"/>
+      <c r="DN40" s="0"/>
+      <c r="DO40" s="0"/>
+      <c r="DP40" s="0"/>
+      <c r="DQ40" s="0"/>
+      <c r="DR40" s="0"/>
+      <c r="DS40" s="0"/>
+      <c r="DT40" s="0"/>
+      <c r="DU40" s="0"/>
+      <c r="DV40" s="0"/>
+      <c r="DW40" s="0"/>
+      <c r="DX40" s="0"/>
+      <c r="DY40" s="0"/>
+      <c r="DZ40" s="0"/>
+      <c r="EA40" s="0"/>
+      <c r="EB40" s="0"/>
+      <c r="EC40" s="0"/>
+      <c r="ED40" s="0"/>
+      <c r="EE40" s="0"/>
+      <c r="EF40" s="0"/>
+      <c r="EG40" s="0"/>
+      <c r="EH40" s="0"/>
+      <c r="EI40" s="0"/>
+      <c r="EJ40" s="0"/>
+      <c r="EK40" s="0"/>
+      <c r="EL40" s="0"/>
+      <c r="EM40" s="0"/>
+      <c r="EN40" s="0"/>
+      <c r="EO40" s="0"/>
+      <c r="EP40" s="0"/>
+      <c r="EQ40" s="0"/>
+      <c r="ER40" s="0"/>
+      <c r="ES40" s="0"/>
+      <c r="ET40" s="0"/>
+      <c r="EU40" s="0"/>
+      <c r="EV40" s="0"/>
+      <c r="EW40" s="0"/>
+      <c r="EX40" s="0"/>
+      <c r="EY40" s="0"/>
+      <c r="EZ40" s="0"/>
+      <c r="FA40" s="0"/>
+      <c r="FB40" s="0"/>
+      <c r="FC40" s="0"/>
+      <c r="FD40" s="0"/>
+      <c r="FE40" s="0"/>
+      <c r="FF40" s="0"/>
+      <c r="FG40" s="0"/>
+      <c r="FH40" s="0"/>
+      <c r="FI40" s="0"/>
+      <c r="FJ40" s="0"/>
+      <c r="FK40" s="0"/>
+      <c r="FL40" s="0"/>
+      <c r="FM40" s="0"/>
+      <c r="FN40" s="0"/>
+      <c r="FO40" s="0"/>
+      <c r="FP40" s="0"/>
+      <c r="FQ40" s="0"/>
+      <c r="FR40" s="0"/>
+      <c r="FS40" s="0"/>
+      <c r="FT40" s="0"/>
+      <c r="FU40" s="0"/>
+      <c r="FV40" s="0"/>
+      <c r="FW40" s="0"/>
+      <c r="FX40" s="0"/>
+      <c r="FY40" s="0"/>
+      <c r="FZ40" s="0"/>
+      <c r="GA40" s="0"/>
+      <c r="GB40" s="0"/>
+      <c r="GC40" s="0"/>
+      <c r="GD40" s="0"/>
+      <c r="GE40" s="0"/>
+      <c r="GF40" s="0"/>
+      <c r="GG40" s="0"/>
+      <c r="GH40" s="0"/>
+      <c r="GI40" s="0"/>
+      <c r="GJ40" s="0"/>
+      <c r="GK40" s="0"/>
+      <c r="GL40" s="0"/>
+      <c r="GM40" s="0"/>
+      <c r="GN40" s="0"/>
+      <c r="GO40" s="0"/>
+      <c r="GP40" s="0"/>
+      <c r="GQ40" s="0"/>
+      <c r="GR40" s="0"/>
+      <c r="GS40" s="0"/>
+      <c r="GT40" s="0"/>
+      <c r="GU40" s="0"/>
+      <c r="GV40" s="0"/>
+      <c r="GW40" s="0"/>
+      <c r="GX40" s="0"/>
+      <c r="GY40" s="0"/>
+      <c r="GZ40" s="0"/>
+      <c r="HA40" s="0"/>
+      <c r="HB40" s="0"/>
+      <c r="HC40" s="0"/>
+      <c r="HD40" s="0"/>
+      <c r="HE40" s="0"/>
+      <c r="HF40" s="0"/>
+      <c r="HG40" s="0"/>
+      <c r="HH40" s="0"/>
+      <c r="HI40" s="0"/>
+      <c r="HJ40" s="0"/>
+      <c r="HK40" s="0"/>
+      <c r="HL40" s="0"/>
+      <c r="HM40" s="0"/>
+      <c r="HN40" s="0"/>
+      <c r="HO40" s="0"/>
+      <c r="HP40" s="0"/>
+      <c r="HQ40" s="0"/>
+      <c r="HR40" s="0"/>
+      <c r="HS40" s="0"/>
+      <c r="HT40" s="0"/>
+      <c r="HU40" s="0"/>
+      <c r="HV40" s="0"/>
+      <c r="HW40" s="0"/>
+      <c r="HX40" s="0"/>
+      <c r="HY40" s="0"/>
+      <c r="HZ40" s="0"/>
+      <c r="IA40" s="0"/>
+      <c r="IB40" s="0"/>
+      <c r="IC40" s="0"/>
+      <c r="ID40" s="0"/>
+      <c r="IE40" s="0"/>
+      <c r="IF40" s="0"/>
+      <c r="IG40" s="0"/>
+      <c r="IH40" s="0"/>
+      <c r="II40" s="0"/>
+      <c r="IJ40" s="0"/>
+      <c r="IK40" s="0"/>
+      <c r="IL40" s="0"/>
+      <c r="IM40" s="0"/>
+      <c r="IN40" s="0"/>
+      <c r="IO40" s="0"/>
+      <c r="IP40" s="0"/>
+      <c r="IQ40" s="0"/>
+      <c r="IR40" s="0"/>
+      <c r="IS40" s="0"/>
+      <c r="IT40" s="0"/>
+      <c r="IU40" s="0"/>
+      <c r="IV40" s="0"/>
+      <c r="IW40" s="0"/>
+      <c r="IX40" s="0"/>
+      <c r="IY40" s="0"/>
+      <c r="IZ40" s="0"/>
+      <c r="JA40" s="0"/>
+      <c r="JB40" s="0"/>
+      <c r="JC40" s="0"/>
+      <c r="JD40" s="0"/>
+      <c r="JE40" s="0"/>
+      <c r="JF40" s="0"/>
+      <c r="JG40" s="0"/>
+      <c r="JH40" s="0"/>
+      <c r="JI40" s="0"/>
+      <c r="JJ40" s="0"/>
+      <c r="JK40" s="0"/>
+      <c r="JL40" s="0"/>
+      <c r="JM40" s="0"/>
+      <c r="JN40" s="0"/>
+      <c r="JO40" s="0"/>
+      <c r="JP40" s="0"/>
+      <c r="JQ40" s="0"/>
+      <c r="JR40" s="0"/>
+      <c r="JS40" s="0"/>
+      <c r="JT40" s="0"/>
+      <c r="JU40" s="0"/>
+      <c r="JV40" s="0"/>
+      <c r="JW40" s="0"/>
+      <c r="JX40" s="0"/>
+      <c r="JY40" s="0"/>
+      <c r="JZ40" s="0"/>
+      <c r="KA40" s="0"/>
+      <c r="KB40" s="0"/>
+      <c r="KC40" s="0"/>
+      <c r="KD40" s="0"/>
+      <c r="KE40" s="0"/>
+      <c r="KF40" s="0"/>
+      <c r="KG40" s="0"/>
+      <c r="KH40" s="0"/>
+      <c r="KI40" s="0"/>
+      <c r="KJ40" s="0"/>
+      <c r="KK40" s="0"/>
+      <c r="KL40" s="0"/>
+      <c r="KM40" s="0"/>
+      <c r="KN40" s="0"/>
+      <c r="KO40" s="0"/>
+      <c r="KP40" s="0"/>
+      <c r="KQ40" s="0"/>
+      <c r="KR40" s="0"/>
+      <c r="KS40" s="0"/>
+      <c r="KT40" s="0"/>
+      <c r="KU40" s="0"/>
+      <c r="KV40" s="0"/>
+      <c r="KW40" s="0"/>
+      <c r="KX40" s="0"/>
+      <c r="KY40" s="0"/>
+      <c r="KZ40" s="0"/>
+      <c r="LA40" s="0"/>
+      <c r="LB40" s="0"/>
+      <c r="LC40" s="0"/>
+      <c r="LD40" s="0"/>
+      <c r="LE40" s="0"/>
+      <c r="LF40" s="0"/>
+      <c r="LG40" s="0"/>
+      <c r="LH40" s="0"/>
+      <c r="LI40" s="0"/>
+      <c r="LJ40" s="0"/>
+      <c r="LK40" s="0"/>
+      <c r="LL40" s="0"/>
+      <c r="LM40" s="0"/>
+      <c r="LN40" s="0"/>
+      <c r="LO40" s="0"/>
+      <c r="LP40" s="0"/>
+      <c r="LQ40" s="0"/>
+      <c r="LR40" s="0"/>
+      <c r="LS40" s="0"/>
+      <c r="LT40" s="0"/>
+      <c r="LU40" s="0"/>
+      <c r="LV40" s="0"/>
+      <c r="LW40" s="0"/>
+      <c r="LX40" s="0"/>
+      <c r="LY40" s="0"/>
+      <c r="LZ40" s="0"/>
+      <c r="MA40" s="0"/>
+      <c r="MB40" s="0"/>
+      <c r="MC40" s="0"/>
+      <c r="MD40" s="0"/>
+      <c r="ME40" s="0"/>
+      <c r="MF40" s="0"/>
+      <c r="MG40" s="0"/>
+      <c r="MH40" s="0"/>
+      <c r="MI40" s="0"/>
+      <c r="MJ40" s="0"/>
+      <c r="MK40" s="0"/>
+      <c r="ML40" s="0"/>
+      <c r="MM40" s="0"/>
+      <c r="MN40" s="0"/>
+      <c r="MO40" s="0"/>
+      <c r="MP40" s="0"/>
+      <c r="MQ40" s="0"/>
+      <c r="MR40" s="0"/>
+      <c r="MS40" s="0"/>
+      <c r="MT40" s="0"/>
+      <c r="MU40" s="0"/>
+      <c r="MV40" s="0"/>
+      <c r="MW40" s="0"/>
+      <c r="MX40" s="0"/>
+      <c r="MY40" s="0"/>
+      <c r="MZ40" s="0"/>
+      <c r="NA40" s="0"/>
+      <c r="NB40" s="0"/>
+      <c r="NC40" s="0"/>
+      <c r="ND40" s="0"/>
+      <c r="NE40" s="0"/>
+      <c r="NF40" s="0"/>
+      <c r="NG40" s="0"/>
+      <c r="NH40" s="0"/>
+      <c r="NI40" s="0"/>
+      <c r="NJ40" s="0"/>
+      <c r="NK40" s="0"/>
+      <c r="NL40" s="0"/>
+      <c r="NM40" s="0"/>
+      <c r="NN40" s="0"/>
+      <c r="NO40" s="0"/>
+      <c r="NP40" s="0"/>
+      <c r="NQ40" s="0"/>
+      <c r="NR40" s="0"/>
+      <c r="NS40" s="0"/>
+      <c r="NT40" s="0"/>
+      <c r="NU40" s="0"/>
+      <c r="NV40" s="0"/>
+      <c r="NW40" s="0"/>
+      <c r="NX40" s="0"/>
+      <c r="NY40" s="0"/>
+      <c r="NZ40" s="0"/>
+      <c r="OA40" s="0"/>
+      <c r="OB40" s="0"/>
+      <c r="OC40" s="0"/>
+      <c r="OD40" s="0"/>
+      <c r="OE40" s="0"/>
+      <c r="OF40" s="0"/>
+      <c r="OG40" s="0"/>
+      <c r="OH40" s="0"/>
+      <c r="OI40" s="0"/>
+      <c r="OJ40" s="0"/>
+      <c r="OK40" s="0"/>
+      <c r="OL40" s="0"/>
+      <c r="OM40" s="0"/>
+      <c r="ON40" s="0"/>
+      <c r="OO40" s="0"/>
+      <c r="OP40" s="0"/>
+      <c r="OQ40" s="0"/>
+      <c r="OR40" s="0"/>
+      <c r="OS40" s="0"/>
+      <c r="OT40" s="0"/>
+      <c r="OU40" s="0"/>
+      <c r="OV40" s="0"/>
+      <c r="OW40" s="0"/>
+      <c r="OX40" s="0"/>
+      <c r="OY40" s="0"/>
+      <c r="OZ40" s="0"/>
+      <c r="PA40" s="0"/>
+      <c r="PB40" s="0"/>
+      <c r="PC40" s="0"/>
+      <c r="PD40" s="0"/>
+      <c r="PE40" s="0"/>
+      <c r="PF40" s="0"/>
+      <c r="PG40" s="0"/>
+      <c r="PH40" s="0"/>
+      <c r="PI40" s="0"/>
+      <c r="PJ40" s="0"/>
+      <c r="PK40" s="0"/>
+      <c r="PL40" s="0"/>
+      <c r="PM40" s="0"/>
+      <c r="PN40" s="0"/>
+      <c r="PO40" s="0"/>
+      <c r="PP40" s="0"/>
+      <c r="PQ40" s="0"/>
+      <c r="PR40" s="0"/>
+      <c r="PS40" s="0"/>
+      <c r="PT40" s="0"/>
+      <c r="PU40" s="0"/>
+      <c r="PV40" s="0"/>
+      <c r="PW40" s="0"/>
+      <c r="PX40" s="0"/>
+      <c r="PY40" s="0"/>
+      <c r="PZ40" s="0"/>
+      <c r="QA40" s="0"/>
+      <c r="QB40" s="0"/>
+      <c r="QC40" s="0"/>
+      <c r="QD40" s="0"/>
+      <c r="QE40" s="0"/>
+      <c r="QF40" s="0"/>
+      <c r="QG40" s="0"/>
+      <c r="QH40" s="0"/>
+      <c r="QI40" s="0"/>
+      <c r="QJ40" s="0"/>
+      <c r="QK40" s="0"/>
+      <c r="QL40" s="0"/>
+      <c r="QM40" s="0"/>
+      <c r="QN40" s="0"/>
+      <c r="QO40" s="0"/>
+      <c r="QP40" s="0"/>
+      <c r="QQ40" s="0"/>
+      <c r="QR40" s="0"/>
+      <c r="QS40" s="0"/>
+      <c r="QT40" s="0"/>
+      <c r="QU40" s="0"/>
+      <c r="QV40" s="0"/>
+      <c r="QW40" s="0"/>
+      <c r="QX40" s="0"/>
+      <c r="QY40" s="0"/>
+      <c r="QZ40" s="0"/>
+      <c r="RA40" s="0"/>
+      <c r="RB40" s="0"/>
+      <c r="RC40" s="0"/>
+      <c r="RD40" s="0"/>
+      <c r="RE40" s="0"/>
+      <c r="RF40" s="0"/>
+      <c r="RG40" s="0"/>
+      <c r="RH40" s="0"/>
+      <c r="RI40" s="0"/>
+      <c r="RJ40" s="0"/>
+      <c r="RK40" s="0"/>
+      <c r="RL40" s="0"/>
+      <c r="RM40" s="0"/>
+      <c r="RN40" s="0"/>
+      <c r="RO40" s="0"/>
+      <c r="RP40" s="0"/>
+      <c r="RQ40" s="0"/>
+      <c r="RR40" s="0"/>
+      <c r="RS40" s="0"/>
+      <c r="RT40" s="0"/>
+      <c r="RU40" s="0"/>
+      <c r="RV40" s="0"/>
+      <c r="RW40" s="0"/>
+      <c r="RX40" s="0"/>
+      <c r="RY40" s="0"/>
+      <c r="RZ40" s="0"/>
+      <c r="SA40" s="0"/>
+      <c r="SB40" s="0"/>
+      <c r="SC40" s="0"/>
+      <c r="SD40" s="0"/>
+      <c r="SE40" s="0"/>
+      <c r="SF40" s="0"/>
+      <c r="SG40" s="0"/>
+      <c r="SH40" s="0"/>
+      <c r="SI40" s="0"/>
+      <c r="SJ40" s="0"/>
+      <c r="SK40" s="0"/>
+      <c r="SL40" s="0"/>
+      <c r="SM40" s="0"/>
+      <c r="SN40" s="0"/>
+      <c r="SO40" s="0"/>
+      <c r="SP40" s="0"/>
+      <c r="SQ40" s="0"/>
+      <c r="SR40" s="0"/>
+      <c r="SS40" s="0"/>
+      <c r="ST40" s="0"/>
+      <c r="SU40" s="0"/>
+      <c r="SV40" s="0"/>
+      <c r="SW40" s="0"/>
+      <c r="SX40" s="0"/>
+      <c r="SY40" s="0"/>
+      <c r="SZ40" s="0"/>
+      <c r="TA40" s="0"/>
+      <c r="TB40" s="0"/>
+      <c r="TC40" s="0"/>
+      <c r="TD40" s="0"/>
+      <c r="TE40" s="0"/>
+      <c r="TF40" s="0"/>
+      <c r="TG40" s="0"/>
+      <c r="TH40" s="0"/>
+      <c r="TI40" s="0"/>
+      <c r="TJ40" s="0"/>
+      <c r="TK40" s="0"/>
+      <c r="TL40" s="0"/>
+      <c r="TM40" s="0"/>
+      <c r="TN40" s="0"/>
+      <c r="TO40" s="0"/>
+      <c r="TP40" s="0"/>
+      <c r="TQ40" s="0"/>
+      <c r="TR40" s="0"/>
+      <c r="TS40" s="0"/>
+      <c r="TT40" s="0"/>
+      <c r="TU40" s="0"/>
+      <c r="TV40" s="0"/>
+      <c r="TW40" s="0"/>
+      <c r="TX40" s="0"/>
+      <c r="TY40" s="0"/>
+      <c r="TZ40" s="0"/>
+      <c r="UA40" s="0"/>
+      <c r="UB40" s="0"/>
+      <c r="UC40" s="0"/>
+      <c r="UD40" s="0"/>
+      <c r="UE40" s="0"/>
+      <c r="UF40" s="0"/>
+      <c r="UG40" s="0"/>
+      <c r="UH40" s="0"/>
+      <c r="UI40" s="0"/>
+      <c r="UJ40" s="0"/>
+      <c r="UK40" s="0"/>
+      <c r="UL40" s="0"/>
+      <c r="UM40" s="0"/>
+      <c r="UN40" s="0"/>
+      <c r="UO40" s="0"/>
+      <c r="UP40" s="0"/>
+      <c r="UQ40" s="0"/>
+      <c r="UR40" s="0"/>
+      <c r="US40" s="0"/>
+      <c r="UT40" s="0"/>
+      <c r="UU40" s="0"/>
+      <c r="UV40" s="0"/>
+      <c r="UW40" s="0"/>
+      <c r="UX40" s="0"/>
+      <c r="UY40" s="0"/>
+      <c r="UZ40" s="0"/>
+      <c r="VA40" s="0"/>
+      <c r="VB40" s="0"/>
+      <c r="VC40" s="0"/>
+      <c r="VD40" s="0"/>
+      <c r="VE40" s="0"/>
+      <c r="VF40" s="0"/>
+      <c r="VG40" s="0"/>
+      <c r="VH40" s="0"/>
+      <c r="VI40" s="0"/>
+      <c r="VJ40" s="0"/>
+      <c r="VK40" s="0"/>
+      <c r="VL40" s="0"/>
+      <c r="VM40" s="0"/>
+      <c r="VN40" s="0"/>
+      <c r="VO40" s="0"/>
+      <c r="VP40" s="0"/>
+      <c r="VQ40" s="0"/>
+      <c r="VR40" s="0"/>
+      <c r="VS40" s="0"/>
+      <c r="VT40" s="0"/>
+      <c r="VU40" s="0"/>
+      <c r="VV40" s="0"/>
+      <c r="VW40" s="0"/>
+      <c r="VX40" s="0"/>
+      <c r="VY40" s="0"/>
+      <c r="VZ40" s="0"/>
+      <c r="WA40" s="0"/>
+      <c r="WB40" s="0"/>
+      <c r="WC40" s="0"/>
+      <c r="WD40" s="0"/>
+      <c r="WE40" s="0"/>
+      <c r="WF40" s="0"/>
+      <c r="WG40" s="0"/>
+      <c r="WH40" s="0"/>
+      <c r="WI40" s="0"/>
+      <c r="WJ40" s="0"/>
+      <c r="WK40" s="0"/>
+      <c r="WL40" s="0"/>
+      <c r="WM40" s="0"/>
+      <c r="WN40" s="0"/>
+      <c r="WO40" s="0"/>
+      <c r="WP40" s="0"/>
+      <c r="WQ40" s="0"/>
+      <c r="WR40" s="0"/>
+      <c r="WS40" s="0"/>
+      <c r="WT40" s="0"/>
+      <c r="WU40" s="0"/>
+      <c r="WV40" s="0"/>
+      <c r="WW40" s="0"/>
+      <c r="WX40" s="0"/>
+      <c r="WY40" s="0"/>
+      <c r="WZ40" s="0"/>
+      <c r="XA40" s="0"/>
+      <c r="XB40" s="0"/>
+      <c r="XC40" s="0"/>
+      <c r="XD40" s="0"/>
+      <c r="XE40" s="0"/>
+      <c r="XF40" s="0"/>
+      <c r="XG40" s="0"/>
+      <c r="XH40" s="0"/>
+      <c r="XI40" s="0"/>
+      <c r="XJ40" s="0"/>
+      <c r="XK40" s="0"/>
+      <c r="XL40" s="0"/>
+      <c r="XM40" s="0"/>
+      <c r="XN40" s="0"/>
+      <c r="XO40" s="0"/>
+      <c r="XP40" s="0"/>
+      <c r="XQ40" s="0"/>
+      <c r="XR40" s="0"/>
+      <c r="XS40" s="0"/>
+      <c r="XT40" s="0"/>
+      <c r="XU40" s="0"/>
+      <c r="XV40" s="0"/>
+      <c r="XW40" s="0"/>
+      <c r="XX40" s="0"/>
+      <c r="XY40" s="0"/>
+      <c r="XZ40" s="0"/>
+      <c r="YA40" s="0"/>
+      <c r="YB40" s="0"/>
+      <c r="YC40" s="0"/>
+      <c r="YD40" s="0"/>
+      <c r="YE40" s="0"/>
+      <c r="YF40" s="0"/>
+      <c r="YG40" s="0"/>
+      <c r="YH40" s="0"/>
+      <c r="YI40" s="0"/>
+      <c r="YJ40" s="0"/>
+      <c r="YK40" s="0"/>
+      <c r="YL40" s="0"/>
+      <c r="YM40" s="0"/>
+      <c r="YN40" s="0"/>
+      <c r="YO40" s="0"/>
+      <c r="YP40" s="0"/>
+      <c r="YQ40" s="0"/>
+      <c r="YR40" s="0"/>
+      <c r="YS40" s="0"/>
+      <c r="YT40" s="0"/>
+      <c r="YU40" s="0"/>
+      <c r="YV40" s="0"/>
+      <c r="YW40" s="0"/>
+      <c r="YX40" s="0"/>
+      <c r="YY40" s="0"/>
+      <c r="YZ40" s="0"/>
+      <c r="ZA40" s="0"/>
+      <c r="ZB40" s="0"/>
+      <c r="ZC40" s="0"/>
+      <c r="ZD40" s="0"/>
+      <c r="ZE40" s="0"/>
+      <c r="ZF40" s="0"/>
+      <c r="ZG40" s="0"/>
+      <c r="ZH40" s="0"/>
+      <c r="ZI40" s="0"/>
+      <c r="ZJ40" s="0"/>
+      <c r="ZK40" s="0"/>
+      <c r="ZL40" s="0"/>
+      <c r="ZM40" s="0"/>
+      <c r="ZN40" s="0"/>
+      <c r="ZO40" s="0"/>
+      <c r="ZP40" s="0"/>
+      <c r="ZQ40" s="0"/>
+      <c r="ZR40" s="0"/>
+      <c r="ZS40" s="0"/>
+      <c r="ZT40" s="0"/>
+      <c r="ZU40" s="0"/>
+      <c r="ZV40" s="0"/>
+      <c r="ZW40" s="0"/>
+      <c r="ZX40" s="0"/>
+      <c r="ZY40" s="0"/>
+      <c r="ZZ40" s="0"/>
+      <c r="AAA40" s="0"/>
+      <c r="AAB40" s="0"/>
+      <c r="AAC40" s="0"/>
+      <c r="AAD40" s="0"/>
+      <c r="AAE40" s="0"/>
+      <c r="AAF40" s="0"/>
+      <c r="AAG40" s="0"/>
+      <c r="AAH40" s="0"/>
+      <c r="AAI40" s="0"/>
+      <c r="AAJ40" s="0"/>
+      <c r="AAK40" s="0"/>
+      <c r="AAL40" s="0"/>
+      <c r="AAM40" s="0"/>
+      <c r="AAN40" s="0"/>
+      <c r="AAO40" s="0"/>
+      <c r="AAP40" s="0"/>
+      <c r="AAQ40" s="0"/>
+      <c r="AAR40" s="0"/>
+      <c r="AAS40" s="0"/>
+      <c r="AAT40" s="0"/>
+      <c r="AAU40" s="0"/>
+      <c r="AAV40" s="0"/>
+      <c r="AAW40" s="0"/>
+      <c r="AAX40" s="0"/>
+      <c r="AAY40" s="0"/>
+      <c r="AAZ40" s="0"/>
+      <c r="ABA40" s="0"/>
+      <c r="ABB40" s="0"/>
+      <c r="ABC40" s="0"/>
+      <c r="ABD40" s="0"/>
+      <c r="ABE40" s="0"/>
+      <c r="ABF40" s="0"/>
+      <c r="ABG40" s="0"/>
+      <c r="ABH40" s="0"/>
+      <c r="ABI40" s="0"/>
+      <c r="ABJ40" s="0"/>
+      <c r="ABK40" s="0"/>
+      <c r="ABL40" s="0"/>
+      <c r="ABM40" s="0"/>
+      <c r="ABN40" s="0"/>
+      <c r="ABO40" s="0"/>
+      <c r="ABP40" s="0"/>
+      <c r="ABQ40" s="0"/>
+      <c r="ABR40" s="0"/>
+      <c r="ABS40" s="0"/>
+      <c r="ABT40" s="0"/>
+      <c r="ABU40" s="0"/>
+      <c r="ABV40" s="0"/>
+      <c r="ABW40" s="0"/>
+      <c r="ABX40" s="0"/>
+      <c r="ABY40" s="0"/>
+      <c r="ABZ40" s="0"/>
+      <c r="ACA40" s="0"/>
+      <c r="ACB40" s="0"/>
+      <c r="ACC40" s="0"/>
+      <c r="ACD40" s="0"/>
+      <c r="ACE40" s="0"/>
+      <c r="ACF40" s="0"/>
+      <c r="ACG40" s="0"/>
+      <c r="ACH40" s="0"/>
+      <c r="ACI40" s="0"/>
+      <c r="ACJ40" s="0"/>
+      <c r="ACK40" s="0"/>
+      <c r="ACL40" s="0"/>
+      <c r="ACM40" s="0"/>
+      <c r="ACN40" s="0"/>
+      <c r="ACO40" s="0"/>
+      <c r="ACP40" s="0"/>
+      <c r="ACQ40" s="0"/>
+      <c r="ACR40" s="0"/>
+      <c r="ACS40" s="0"/>
+      <c r="ACT40" s="0"/>
+      <c r="ACU40" s="0"/>
+      <c r="ACV40" s="0"/>
+      <c r="ACW40" s="0"/>
+      <c r="ACX40" s="0"/>
+      <c r="ACY40" s="0"/>
+      <c r="ACZ40" s="0"/>
+      <c r="ADA40" s="0"/>
+      <c r="ADB40" s="0"/>
+      <c r="ADC40" s="0"/>
+      <c r="ADD40" s="0"/>
+      <c r="ADE40" s="0"/>
+      <c r="ADF40" s="0"/>
+      <c r="ADG40" s="0"/>
+      <c r="ADH40" s="0"/>
+      <c r="ADI40" s="0"/>
+      <c r="ADJ40" s="0"/>
+      <c r="ADK40" s="0"/>
+      <c r="ADL40" s="0"/>
+      <c r="ADM40" s="0"/>
+      <c r="ADN40" s="0"/>
+      <c r="ADO40" s="0"/>
+      <c r="ADP40" s="0"/>
+      <c r="ADQ40" s="0"/>
+      <c r="ADR40" s="0"/>
+      <c r="ADS40" s="0"/>
+      <c r="ADT40" s="0"/>
+      <c r="ADU40" s="0"/>
+      <c r="ADV40" s="0"/>
+      <c r="ADW40" s="0"/>
+      <c r="ADX40" s="0"/>
+      <c r="ADY40" s="0"/>
+      <c r="ADZ40" s="0"/>
+      <c r="AEA40" s="0"/>
+      <c r="AEB40" s="0"/>
+      <c r="AEC40" s="0"/>
+      <c r="AED40" s="0"/>
+      <c r="AEE40" s="0"/>
+      <c r="AEF40" s="0"/>
+      <c r="AEG40" s="0"/>
+      <c r="AEH40" s="0"/>
+      <c r="AEI40" s="0"/>
+      <c r="AEJ40" s="0"/>
+      <c r="AEK40" s="0"/>
+      <c r="AEL40" s="0"/>
+      <c r="AEM40" s="0"/>
+      <c r="AEN40" s="0"/>
+      <c r="AEO40" s="0"/>
+      <c r="AEP40" s="0"/>
+      <c r="AEQ40" s="0"/>
+      <c r="AER40" s="0"/>
+      <c r="AES40" s="0"/>
+      <c r="AET40" s="0"/>
+      <c r="AEU40" s="0"/>
+      <c r="AEV40" s="0"/>
+      <c r="AEW40" s="0"/>
+      <c r="AEX40" s="0"/>
+      <c r="AEY40" s="0"/>
+      <c r="AEZ40" s="0"/>
+      <c r="AFA40" s="0"/>
+      <c r="AFB40" s="0"/>
+      <c r="AFC40" s="0"/>
+      <c r="AFD40" s="0"/>
+      <c r="AFE40" s="0"/>
+      <c r="AFF40" s="0"/>
+      <c r="AFG40" s="0"/>
+      <c r="AFH40" s="0"/>
+      <c r="AFI40" s="0"/>
+      <c r="AFJ40" s="0"/>
+      <c r="AFK40" s="0"/>
+      <c r="AFL40" s="0"/>
+      <c r="AFM40" s="0"/>
+      <c r="AFN40" s="0"/>
+      <c r="AFO40" s="0"/>
+      <c r="AFP40" s="0"/>
+      <c r="AFQ40" s="0"/>
+      <c r="AFR40" s="0"/>
+      <c r="AFS40" s="0"/>
+      <c r="AFT40" s="0"/>
+      <c r="AFU40" s="0"/>
+      <c r="AFV40" s="0"/>
+      <c r="AFW40" s="0"/>
+      <c r="AFX40" s="0"/>
+      <c r="AFY40" s="0"/>
+      <c r="AFZ40" s="0"/>
+      <c r="AGA40" s="0"/>
+      <c r="AGB40" s="0"/>
+      <c r="AGC40" s="0"/>
+      <c r="AGD40" s="0"/>
+      <c r="AGE40" s="0"/>
+      <c r="AGF40" s="0"/>
+      <c r="AGG40" s="0"/>
+      <c r="AGH40" s="0"/>
+      <c r="AGI40" s="0"/>
+      <c r="AGJ40" s="0"/>
+      <c r="AGK40" s="0"/>
+      <c r="AGL40" s="0"/>
+      <c r="AGM40" s="0"/>
+      <c r="AGN40" s="0"/>
+      <c r="AGO40" s="0"/>
+      <c r="AGP40" s="0"/>
+      <c r="AGQ40" s="0"/>
+      <c r="AGR40" s="0"/>
+      <c r="AGS40" s="0"/>
+      <c r="AGT40" s="0"/>
+      <c r="AGU40" s="0"/>
+      <c r="AGV40" s="0"/>
+      <c r="AGW40" s="0"/>
+      <c r="AGX40" s="0"/>
+      <c r="AGY40" s="0"/>
+      <c r="AGZ40" s="0"/>
+      <c r="AHA40" s="0"/>
+      <c r="AHB40" s="0"/>
+      <c r="AHC40" s="0"/>
+      <c r="AHD40" s="0"/>
+      <c r="AHE40" s="0"/>
+      <c r="AHF40" s="0"/>
+      <c r="AHG40" s="0"/>
+      <c r="AHH40" s="0"/>
+      <c r="AHI40" s="0"/>
+      <c r="AHJ40" s="0"/>
+      <c r="AHK40" s="0"/>
+      <c r="AHL40" s="0"/>
+      <c r="AHM40" s="0"/>
+      <c r="AHN40" s="0"/>
+      <c r="AHO40" s="0"/>
+      <c r="AHP40" s="0"/>
+      <c r="AHQ40" s="0"/>
+      <c r="AHR40" s="0"/>
+      <c r="AHS40" s="0"/>
+      <c r="AHT40" s="0"/>
+      <c r="AHU40" s="0"/>
+      <c r="AHV40" s="0"/>
+      <c r="AHW40" s="0"/>
+      <c r="AHX40" s="0"/>
+      <c r="AHY40" s="0"/>
+      <c r="AHZ40" s="0"/>
+      <c r="AIA40" s="0"/>
+      <c r="AIB40" s="0"/>
+      <c r="AIC40" s="0"/>
+      <c r="AID40" s="0"/>
+      <c r="AIE40" s="0"/>
+      <c r="AIF40" s="0"/>
+      <c r="AIG40" s="0"/>
+      <c r="AIH40" s="0"/>
+      <c r="AII40" s="0"/>
+      <c r="AIJ40" s="0"/>
+      <c r="AIK40" s="0"/>
+      <c r="AIL40" s="0"/>
+      <c r="AIM40" s="0"/>
+      <c r="AIN40" s="0"/>
+      <c r="AIO40" s="0"/>
+      <c r="AIP40" s="0"/>
+      <c r="AIQ40" s="0"/>
+      <c r="AIR40" s="0"/>
+      <c r="AIS40" s="0"/>
+      <c r="AIT40" s="0"/>
+      <c r="AIU40" s="0"/>
+      <c r="AIV40" s="0"/>
+      <c r="AIW40" s="0"/>
+      <c r="AIX40" s="0"/>
+      <c r="AIY40" s="0"/>
+      <c r="AIZ40" s="0"/>
+      <c r="AJA40" s="0"/>
+      <c r="AJB40" s="0"/>
+      <c r="AJC40" s="0"/>
+      <c r="AJD40" s="0"/>
+      <c r="AJE40" s="0"/>
+      <c r="AJF40" s="0"/>
+      <c r="AJG40" s="0"/>
+      <c r="AJH40" s="0"/>
+      <c r="AJI40" s="0"/>
+      <c r="AJJ40" s="0"/>
+      <c r="AJK40" s="0"/>
+      <c r="AJL40" s="0"/>
+      <c r="AJM40" s="0"/>
+      <c r="AJN40" s="0"/>
+      <c r="AJO40" s="0"/>
+      <c r="AJP40" s="0"/>
+      <c r="AJQ40" s="0"/>
+      <c r="AJR40" s="0"/>
+      <c r="AJS40" s="0"/>
+      <c r="AJT40" s="0"/>
+      <c r="AJU40" s="0"/>
+      <c r="AJV40" s="0"/>
+      <c r="AJW40" s="0"/>
+      <c r="AJX40" s="0"/>
+      <c r="AJY40" s="0"/>
+      <c r="AJZ40" s="0"/>
+      <c r="AKA40" s="0"/>
+      <c r="AKB40" s="0"/>
+      <c r="AKC40" s="0"/>
+      <c r="AKD40" s="0"/>
+      <c r="AKE40" s="0"/>
+      <c r="AKF40" s="0"/>
+      <c r="AKG40" s="0"/>
+      <c r="AKH40" s="0"/>
+      <c r="AKI40" s="0"/>
+      <c r="AKJ40" s="0"/>
+      <c r="AKK40" s="0"/>
+      <c r="AKL40" s="0"/>
+      <c r="AKM40" s="0"/>
+      <c r="AKN40" s="0"/>
+      <c r="AKO40" s="0"/>
+      <c r="AKP40" s="0"/>
+      <c r="AKQ40" s="0"/>
+      <c r="AKR40" s="0"/>
+      <c r="AKS40" s="0"/>
+      <c r="AKT40" s="0"/>
+      <c r="AKU40" s="0"/>
+      <c r="AKV40" s="0"/>
+      <c r="AKW40" s="0"/>
+      <c r="AKX40" s="0"/>
+      <c r="AKY40" s="0"/>
+      <c r="AKZ40" s="0"/>
+      <c r="ALA40" s="0"/>
+      <c r="ALB40" s="0"/>
+      <c r="ALC40" s="0"/>
+      <c r="ALD40" s="0"/>
+      <c r="ALE40" s="0"/>
+      <c r="ALF40" s="0"/>
+      <c r="ALG40" s="0"/>
+      <c r="ALH40" s="0"/>
+      <c r="ALI40" s="0"/>
+      <c r="ALJ40" s="0"/>
+      <c r="ALK40" s="0"/>
+      <c r="ALL40" s="0"/>
+      <c r="ALM40" s="0"/>
+      <c r="ALN40" s="0"/>
+      <c r="ALO40" s="0"/>
+      <c r="ALP40" s="0"/>
+      <c r="ALQ40" s="0"/>
+      <c r="ALR40" s="0"/>
+      <c r="ALS40" s="0"/>
+      <c r="ALT40" s="0"/>
+      <c r="ALU40" s="0"/>
+      <c r="ALV40" s="0"/>
+      <c r="ALW40" s="0"/>
+      <c r="ALX40" s="0"/>
+      <c r="ALY40" s="0"/>
+      <c r="ALZ40" s="0"/>
+      <c r="AMA40" s="0"/>
+      <c r="AMB40" s="0"/>
+      <c r="AMC40" s="0"/>
+      <c r="AMD40" s="0"/>
+      <c r="AME40" s="0"/>
+      <c r="AMF40" s="0"/>
+      <c r="AMG40" s="0"/>
+      <c r="AMH40" s="0"/>
+      <c r="AMI40" s="0"/>
+      <c r="AMJ40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="18" t="n">
@@ -41618,6 +43577,985 @@
       </c>
       <c r="AR41" s="36"/>
       <c r="AS41" s="30"/>
+      <c r="AT41" s="0"/>
+      <c r="AU41" s="0"/>
+      <c r="AV41" s="0"/>
+      <c r="AW41" s="0"/>
+      <c r="AX41" s="0"/>
+      <c r="AY41" s="0"/>
+      <c r="AZ41" s="0"/>
+      <c r="BA41" s="0"/>
+      <c r="BB41" s="0"/>
+      <c r="BC41" s="0"/>
+      <c r="BD41" s="0"/>
+      <c r="BE41" s="0"/>
+      <c r="BF41" s="0"/>
+      <c r="BG41" s="0"/>
+      <c r="BH41" s="0"/>
+      <c r="BI41" s="0"/>
+      <c r="BJ41" s="0"/>
+      <c r="BK41" s="0"/>
+      <c r="BL41" s="0"/>
+      <c r="BM41" s="0"/>
+      <c r="BN41" s="0"/>
+      <c r="BO41" s="0"/>
+      <c r="BP41" s="0"/>
+      <c r="BQ41" s="0"/>
+      <c r="BR41" s="0"/>
+      <c r="BS41" s="0"/>
+      <c r="BT41" s="0"/>
+      <c r="BU41" s="0"/>
+      <c r="BV41" s="0"/>
+      <c r="BW41" s="0"/>
+      <c r="BX41" s="0"/>
+      <c r="BY41" s="0"/>
+      <c r="BZ41" s="0"/>
+      <c r="CA41" s="0"/>
+      <c r="CB41" s="0"/>
+      <c r="CC41" s="0"/>
+      <c r="CD41" s="0"/>
+      <c r="CE41" s="0"/>
+      <c r="CF41" s="0"/>
+      <c r="CG41" s="0"/>
+      <c r="CH41" s="0"/>
+      <c r="CI41" s="0"/>
+      <c r="CJ41" s="0"/>
+      <c r="CK41" s="0"/>
+      <c r="CL41" s="0"/>
+      <c r="CM41" s="0"/>
+      <c r="CN41" s="0"/>
+      <c r="CO41" s="0"/>
+      <c r="CP41" s="0"/>
+      <c r="CQ41" s="0"/>
+      <c r="CR41" s="0"/>
+      <c r="CS41" s="0"/>
+      <c r="CT41" s="0"/>
+      <c r="CU41" s="0"/>
+      <c r="CV41" s="0"/>
+      <c r="CW41" s="0"/>
+      <c r="CX41" s="0"/>
+      <c r="CY41" s="0"/>
+      <c r="CZ41" s="0"/>
+      <c r="DA41" s="0"/>
+      <c r="DB41" s="0"/>
+      <c r="DC41" s="0"/>
+      <c r="DD41" s="0"/>
+      <c r="DE41" s="0"/>
+      <c r="DF41" s="0"/>
+      <c r="DG41" s="0"/>
+      <c r="DH41" s="0"/>
+      <c r="DI41" s="0"/>
+      <c r="DJ41" s="0"/>
+      <c r="DK41" s="0"/>
+      <c r="DL41" s="0"/>
+      <c r="DM41" s="0"/>
+      <c r="DN41" s="0"/>
+      <c r="DO41" s="0"/>
+      <c r="DP41" s="0"/>
+      <c r="DQ41" s="0"/>
+      <c r="DR41" s="0"/>
+      <c r="DS41" s="0"/>
+      <c r="DT41" s="0"/>
+      <c r="DU41" s="0"/>
+      <c r="DV41" s="0"/>
+      <c r="DW41" s="0"/>
+      <c r="DX41" s="0"/>
+      <c r="DY41" s="0"/>
+      <c r="DZ41" s="0"/>
+      <c r="EA41" s="0"/>
+      <c r="EB41" s="0"/>
+      <c r="EC41" s="0"/>
+      <c r="ED41" s="0"/>
+      <c r="EE41" s="0"/>
+      <c r="EF41" s="0"/>
+      <c r="EG41" s="0"/>
+      <c r="EH41" s="0"/>
+      <c r="EI41" s="0"/>
+      <c r="EJ41" s="0"/>
+      <c r="EK41" s="0"/>
+      <c r="EL41" s="0"/>
+      <c r="EM41" s="0"/>
+      <c r="EN41" s="0"/>
+      <c r="EO41" s="0"/>
+      <c r="EP41" s="0"/>
+      <c r="EQ41" s="0"/>
+      <c r="ER41" s="0"/>
+      <c r="ES41" s="0"/>
+      <c r="ET41" s="0"/>
+      <c r="EU41" s="0"/>
+      <c r="EV41" s="0"/>
+      <c r="EW41" s="0"/>
+      <c r="EX41" s="0"/>
+      <c r="EY41" s="0"/>
+      <c r="EZ41" s="0"/>
+      <c r="FA41" s="0"/>
+      <c r="FB41" s="0"/>
+      <c r="FC41" s="0"/>
+      <c r="FD41" s="0"/>
+      <c r="FE41" s="0"/>
+      <c r="FF41" s="0"/>
+      <c r="FG41" s="0"/>
+      <c r="FH41" s="0"/>
+      <c r="FI41" s="0"/>
+      <c r="FJ41" s="0"/>
+      <c r="FK41" s="0"/>
+      <c r="FL41" s="0"/>
+      <c r="FM41" s="0"/>
+      <c r="FN41" s="0"/>
+      <c r="FO41" s="0"/>
+      <c r="FP41" s="0"/>
+      <c r="FQ41" s="0"/>
+      <c r="FR41" s="0"/>
+      <c r="FS41" s="0"/>
+      <c r="FT41" s="0"/>
+      <c r="FU41" s="0"/>
+      <c r="FV41" s="0"/>
+      <c r="FW41" s="0"/>
+      <c r="FX41" s="0"/>
+      <c r="FY41" s="0"/>
+      <c r="FZ41" s="0"/>
+      <c r="GA41" s="0"/>
+      <c r="GB41" s="0"/>
+      <c r="GC41" s="0"/>
+      <c r="GD41" s="0"/>
+      <c r="GE41" s="0"/>
+      <c r="GF41" s="0"/>
+      <c r="GG41" s="0"/>
+      <c r="GH41" s="0"/>
+      <c r="GI41" s="0"/>
+      <c r="GJ41" s="0"/>
+      <c r="GK41" s="0"/>
+      <c r="GL41" s="0"/>
+      <c r="GM41" s="0"/>
+      <c r="GN41" s="0"/>
+      <c r="GO41" s="0"/>
+      <c r="GP41" s="0"/>
+      <c r="GQ41" s="0"/>
+      <c r="GR41" s="0"/>
+      <c r="GS41" s="0"/>
+      <c r="GT41" s="0"/>
+      <c r="GU41" s="0"/>
+      <c r="GV41" s="0"/>
+      <c r="GW41" s="0"/>
+      <c r="GX41" s="0"/>
+      <c r="GY41" s="0"/>
+      <c r="GZ41" s="0"/>
+      <c r="HA41" s="0"/>
+      <c r="HB41" s="0"/>
+      <c r="HC41" s="0"/>
+      <c r="HD41" s="0"/>
+      <c r="HE41" s="0"/>
+      <c r="HF41" s="0"/>
+      <c r="HG41" s="0"/>
+      <c r="HH41" s="0"/>
+      <c r="HI41" s="0"/>
+      <c r="HJ41" s="0"/>
+      <c r="HK41" s="0"/>
+      <c r="HL41" s="0"/>
+      <c r="HM41" s="0"/>
+      <c r="HN41" s="0"/>
+      <c r="HO41" s="0"/>
+      <c r="HP41" s="0"/>
+      <c r="HQ41" s="0"/>
+      <c r="HR41" s="0"/>
+      <c r="HS41" s="0"/>
+      <c r="HT41" s="0"/>
+      <c r="HU41" s="0"/>
+      <c r="HV41" s="0"/>
+      <c r="HW41" s="0"/>
+      <c r="HX41" s="0"/>
+      <c r="HY41" s="0"/>
+      <c r="HZ41" s="0"/>
+      <c r="IA41" s="0"/>
+      <c r="IB41" s="0"/>
+      <c r="IC41" s="0"/>
+      <c r="ID41" s="0"/>
+      <c r="IE41" s="0"/>
+      <c r="IF41" s="0"/>
+      <c r="IG41" s="0"/>
+      <c r="IH41" s="0"/>
+      <c r="II41" s="0"/>
+      <c r="IJ41" s="0"/>
+      <c r="IK41" s="0"/>
+      <c r="IL41" s="0"/>
+      <c r="IM41" s="0"/>
+      <c r="IN41" s="0"/>
+      <c r="IO41" s="0"/>
+      <c r="IP41" s="0"/>
+      <c r="IQ41" s="0"/>
+      <c r="IR41" s="0"/>
+      <c r="IS41" s="0"/>
+      <c r="IT41" s="0"/>
+      <c r="IU41" s="0"/>
+      <c r="IV41" s="0"/>
+      <c r="IW41" s="0"/>
+      <c r="IX41" s="0"/>
+      <c r="IY41" s="0"/>
+      <c r="IZ41" s="0"/>
+      <c r="JA41" s="0"/>
+      <c r="JB41" s="0"/>
+      <c r="JC41" s="0"/>
+      <c r="JD41" s="0"/>
+      <c r="JE41" s="0"/>
+      <c r="JF41" s="0"/>
+      <c r="JG41" s="0"/>
+      <c r="JH41" s="0"/>
+      <c r="JI41" s="0"/>
+      <c r="JJ41" s="0"/>
+      <c r="JK41" s="0"/>
+      <c r="JL41" s="0"/>
+      <c r="JM41" s="0"/>
+      <c r="JN41" s="0"/>
+      <c r="JO41" s="0"/>
+      <c r="JP41" s="0"/>
+      <c r="JQ41" s="0"/>
+      <c r="JR41" s="0"/>
+      <c r="JS41" s="0"/>
+      <c r="JT41" s="0"/>
+      <c r="JU41" s="0"/>
+      <c r="JV41" s="0"/>
+      <c r="JW41" s="0"/>
+      <c r="JX41" s="0"/>
+      <c r="JY41" s="0"/>
+      <c r="JZ41" s="0"/>
+      <c r="KA41" s="0"/>
+      <c r="KB41" s="0"/>
+      <c r="KC41" s="0"/>
+      <c r="KD41" s="0"/>
+      <c r="KE41" s="0"/>
+      <c r="KF41" s="0"/>
+      <c r="KG41" s="0"/>
+      <c r="KH41" s="0"/>
+      <c r="KI41" s="0"/>
+      <c r="KJ41" s="0"/>
+      <c r="KK41" s="0"/>
+      <c r="KL41" s="0"/>
+      <c r="KM41" s="0"/>
+      <c r="KN41" s="0"/>
+      <c r="KO41" s="0"/>
+      <c r="KP41" s="0"/>
+      <c r="KQ41" s="0"/>
+      <c r="KR41" s="0"/>
+      <c r="KS41" s="0"/>
+      <c r="KT41" s="0"/>
+      <c r="KU41" s="0"/>
+      <c r="KV41" s="0"/>
+      <c r="KW41" s="0"/>
+      <c r="KX41" s="0"/>
+      <c r="KY41" s="0"/>
+      <c r="KZ41" s="0"/>
+      <c r="LA41" s="0"/>
+      <c r="LB41" s="0"/>
+      <c r="LC41" s="0"/>
+      <c r="LD41" s="0"/>
+      <c r="LE41" s="0"/>
+      <c r="LF41" s="0"/>
+      <c r="LG41" s="0"/>
+      <c r="LH41" s="0"/>
+      <c r="LI41" s="0"/>
+      <c r="LJ41" s="0"/>
+      <c r="LK41" s="0"/>
+      <c r="LL41" s="0"/>
+      <c r="LM41" s="0"/>
+      <c r="LN41" s="0"/>
+      <c r="LO41" s="0"/>
+      <c r="LP41" s="0"/>
+      <c r="LQ41" s="0"/>
+      <c r="LR41" s="0"/>
+      <c r="LS41" s="0"/>
+      <c r="LT41" s="0"/>
+      <c r="LU41" s="0"/>
+      <c r="LV41" s="0"/>
+      <c r="LW41" s="0"/>
+      <c r="LX41" s="0"/>
+      <c r="LY41" s="0"/>
+      <c r="LZ41" s="0"/>
+      <c r="MA41" s="0"/>
+      <c r="MB41" s="0"/>
+      <c r="MC41" s="0"/>
+      <c r="MD41" s="0"/>
+      <c r="ME41" s="0"/>
+      <c r="MF41" s="0"/>
+      <c r="MG41" s="0"/>
+      <c r="MH41" s="0"/>
+      <c r="MI41" s="0"/>
+      <c r="MJ41" s="0"/>
+      <c r="MK41" s="0"/>
+      <c r="ML41" s="0"/>
+      <c r="MM41" s="0"/>
+      <c r="MN41" s="0"/>
+      <c r="MO41" s="0"/>
+      <c r="MP41" s="0"/>
+      <c r="MQ41" s="0"/>
+      <c r="MR41" s="0"/>
+      <c r="MS41" s="0"/>
+      <c r="MT41" s="0"/>
+      <c r="MU41" s="0"/>
+      <c r="MV41" s="0"/>
+      <c r="MW41" s="0"/>
+      <c r="MX41" s="0"/>
+      <c r="MY41" s="0"/>
+      <c r="MZ41" s="0"/>
+      <c r="NA41" s="0"/>
+      <c r="NB41" s="0"/>
+      <c r="NC41" s="0"/>
+      <c r="ND41" s="0"/>
+      <c r="NE41" s="0"/>
+      <c r="NF41" s="0"/>
+      <c r="NG41" s="0"/>
+      <c r="NH41" s="0"/>
+      <c r="NI41" s="0"/>
+      <c r="NJ41" s="0"/>
+      <c r="NK41" s="0"/>
+      <c r="NL41" s="0"/>
+      <c r="NM41" s="0"/>
+      <c r="NN41" s="0"/>
+      <c r="NO41" s="0"/>
+      <c r="NP41" s="0"/>
+      <c r="NQ41" s="0"/>
+      <c r="NR41" s="0"/>
+      <c r="NS41" s="0"/>
+      <c r="NT41" s="0"/>
+      <c r="NU41" s="0"/>
+      <c r="NV41" s="0"/>
+      <c r="NW41" s="0"/>
+      <c r="NX41" s="0"/>
+      <c r="NY41" s="0"/>
+      <c r="NZ41" s="0"/>
+      <c r="OA41" s="0"/>
+      <c r="OB41" s="0"/>
+      <c r="OC41" s="0"/>
+      <c r="OD41" s="0"/>
+      <c r="OE41" s="0"/>
+      <c r="OF41" s="0"/>
+      <c r="OG41" s="0"/>
+      <c r="OH41" s="0"/>
+      <c r="OI41" s="0"/>
+      <c r="OJ41" s="0"/>
+      <c r="OK41" s="0"/>
+      <c r="OL41" s="0"/>
+      <c r="OM41" s="0"/>
+      <c r="ON41" s="0"/>
+      <c r="OO41" s="0"/>
+      <c r="OP41" s="0"/>
+      <c r="OQ41" s="0"/>
+      <c r="OR41" s="0"/>
+      <c r="OS41" s="0"/>
+      <c r="OT41" s="0"/>
+      <c r="OU41" s="0"/>
+      <c r="OV41" s="0"/>
+      <c r="OW41" s="0"/>
+      <c r="OX41" s="0"/>
+      <c r="OY41" s="0"/>
+      <c r="OZ41" s="0"/>
+      <c r="PA41" s="0"/>
+      <c r="PB41" s="0"/>
+      <c r="PC41" s="0"/>
+      <c r="PD41" s="0"/>
+      <c r="PE41" s="0"/>
+      <c r="PF41" s="0"/>
+      <c r="PG41" s="0"/>
+      <c r="PH41" s="0"/>
+      <c r="PI41" s="0"/>
+      <c r="PJ41" s="0"/>
+      <c r="PK41" s="0"/>
+      <c r="PL41" s="0"/>
+      <c r="PM41" s="0"/>
+      <c r="PN41" s="0"/>
+      <c r="PO41" s="0"/>
+      <c r="PP41" s="0"/>
+      <c r="PQ41" s="0"/>
+      <c r="PR41" s="0"/>
+      <c r="PS41" s="0"/>
+      <c r="PT41" s="0"/>
+      <c r="PU41" s="0"/>
+      <c r="PV41" s="0"/>
+      <c r="PW41" s="0"/>
+      <c r="PX41" s="0"/>
+      <c r="PY41" s="0"/>
+      <c r="PZ41" s="0"/>
+      <c r="QA41" s="0"/>
+      <c r="QB41" s="0"/>
+      <c r="QC41" s="0"/>
+      <c r="QD41" s="0"/>
+      <c r="QE41" s="0"/>
+      <c r="QF41" s="0"/>
+      <c r="QG41" s="0"/>
+      <c r="QH41" s="0"/>
+      <c r="QI41" s="0"/>
+      <c r="QJ41" s="0"/>
+      <c r="QK41" s="0"/>
+      <c r="QL41" s="0"/>
+      <c r="QM41" s="0"/>
+      <c r="QN41" s="0"/>
+      <c r="QO41" s="0"/>
+      <c r="QP41" s="0"/>
+      <c r="QQ41" s="0"/>
+      <c r="QR41" s="0"/>
+      <c r="QS41" s="0"/>
+      <c r="QT41" s="0"/>
+      <c r="QU41" s="0"/>
+      <c r="QV41" s="0"/>
+      <c r="QW41" s="0"/>
+      <c r="QX41" s="0"/>
+      <c r="QY41" s="0"/>
+      <c r="QZ41" s="0"/>
+      <c r="RA41" s="0"/>
+      <c r="RB41" s="0"/>
+      <c r="RC41" s="0"/>
+      <c r="RD41" s="0"/>
+      <c r="RE41" s="0"/>
+      <c r="RF41" s="0"/>
+      <c r="RG41" s="0"/>
+      <c r="RH41" s="0"/>
+      <c r="RI41" s="0"/>
+      <c r="RJ41" s="0"/>
+      <c r="RK41" s="0"/>
+      <c r="RL41" s="0"/>
+      <c r="RM41" s="0"/>
+      <c r="RN41" s="0"/>
+      <c r="RO41" s="0"/>
+      <c r="RP41" s="0"/>
+      <c r="RQ41" s="0"/>
+      <c r="RR41" s="0"/>
+      <c r="RS41" s="0"/>
+      <c r="RT41" s="0"/>
+      <c r="RU41" s="0"/>
+      <c r="RV41" s="0"/>
+      <c r="RW41" s="0"/>
+      <c r="RX41" s="0"/>
+      <c r="RY41" s="0"/>
+      <c r="RZ41" s="0"/>
+      <c r="SA41" s="0"/>
+      <c r="SB41" s="0"/>
+      <c r="SC41" s="0"/>
+      <c r="SD41" s="0"/>
+      <c r="SE41" s="0"/>
+      <c r="SF41" s="0"/>
+      <c r="SG41" s="0"/>
+      <c r="SH41" s="0"/>
+      <c r="SI41" s="0"/>
+      <c r="SJ41" s="0"/>
+      <c r="SK41" s="0"/>
+      <c r="SL41" s="0"/>
+      <c r="SM41" s="0"/>
+      <c r="SN41" s="0"/>
+      <c r="SO41" s="0"/>
+      <c r="SP41" s="0"/>
+      <c r="SQ41" s="0"/>
+      <c r="SR41" s="0"/>
+      <c r="SS41" s="0"/>
+      <c r="ST41" s="0"/>
+      <c r="SU41" s="0"/>
+      <c r="SV41" s="0"/>
+      <c r="SW41" s="0"/>
+      <c r="SX41" s="0"/>
+      <c r="SY41" s="0"/>
+      <c r="SZ41" s="0"/>
+      <c r="TA41" s="0"/>
+      <c r="TB41" s="0"/>
+      <c r="TC41" s="0"/>
+      <c r="TD41" s="0"/>
+      <c r="TE41" s="0"/>
+      <c r="TF41" s="0"/>
+      <c r="TG41" s="0"/>
+      <c r="TH41" s="0"/>
+      <c r="TI41" s="0"/>
+      <c r="TJ41" s="0"/>
+      <c r="TK41" s="0"/>
+      <c r="TL41" s="0"/>
+      <c r="TM41" s="0"/>
+      <c r="TN41" s="0"/>
+      <c r="TO41" s="0"/>
+      <c r="TP41" s="0"/>
+      <c r="TQ41" s="0"/>
+      <c r="TR41" s="0"/>
+      <c r="TS41" s="0"/>
+      <c r="TT41" s="0"/>
+      <c r="TU41" s="0"/>
+      <c r="TV41" s="0"/>
+      <c r="TW41" s="0"/>
+      <c r="TX41" s="0"/>
+      <c r="TY41" s="0"/>
+      <c r="TZ41" s="0"/>
+      <c r="UA41" s="0"/>
+      <c r="UB41" s="0"/>
+      <c r="UC41" s="0"/>
+      <c r="UD41" s="0"/>
+      <c r="UE41" s="0"/>
+      <c r="UF41" s="0"/>
+      <c r="UG41" s="0"/>
+      <c r="UH41" s="0"/>
+      <c r="UI41" s="0"/>
+      <c r="UJ41" s="0"/>
+      <c r="UK41" s="0"/>
+      <c r="UL41" s="0"/>
+      <c r="UM41" s="0"/>
+      <c r="UN41" s="0"/>
+      <c r="UO41" s="0"/>
+      <c r="UP41" s="0"/>
+      <c r="UQ41" s="0"/>
+      <c r="UR41" s="0"/>
+      <c r="US41" s="0"/>
+      <c r="UT41" s="0"/>
+      <c r="UU41" s="0"/>
+      <c r="UV41" s="0"/>
+      <c r="UW41" s="0"/>
+      <c r="UX41" s="0"/>
+      <c r="UY41" s="0"/>
+      <c r="UZ41" s="0"/>
+      <c r="VA41" s="0"/>
+      <c r="VB41" s="0"/>
+      <c r="VC41" s="0"/>
+      <c r="VD41" s="0"/>
+      <c r="VE41" s="0"/>
+      <c r="VF41" s="0"/>
+      <c r="VG41" s="0"/>
+      <c r="VH41" s="0"/>
+      <c r="VI41" s="0"/>
+      <c r="VJ41" s="0"/>
+      <c r="VK41" s="0"/>
+      <c r="VL41" s="0"/>
+      <c r="VM41" s="0"/>
+      <c r="VN41" s="0"/>
+      <c r="VO41" s="0"/>
+      <c r="VP41" s="0"/>
+      <c r="VQ41" s="0"/>
+      <c r="VR41" s="0"/>
+      <c r="VS41" s="0"/>
+      <c r="VT41" s="0"/>
+      <c r="VU41" s="0"/>
+      <c r="VV41" s="0"/>
+      <c r="VW41" s="0"/>
+      <c r="VX41" s="0"/>
+      <c r="VY41" s="0"/>
+      <c r="VZ41" s="0"/>
+      <c r="WA41" s="0"/>
+      <c r="WB41" s="0"/>
+      <c r="WC41" s="0"/>
+      <c r="WD41" s="0"/>
+      <c r="WE41" s="0"/>
+      <c r="WF41" s="0"/>
+      <c r="WG41" s="0"/>
+      <c r="WH41" s="0"/>
+      <c r="WI41" s="0"/>
+      <c r="WJ41" s="0"/>
+      <c r="WK41" s="0"/>
+      <c r="WL41" s="0"/>
+      <c r="WM41" s="0"/>
+      <c r="WN41" s="0"/>
+      <c r="WO41" s="0"/>
+      <c r="WP41" s="0"/>
+      <c r="WQ41" s="0"/>
+      <c r="WR41" s="0"/>
+      <c r="WS41" s="0"/>
+      <c r="WT41" s="0"/>
+      <c r="WU41" s="0"/>
+      <c r="WV41" s="0"/>
+      <c r="WW41" s="0"/>
+      <c r="WX41" s="0"/>
+      <c r="WY41" s="0"/>
+      <c r="WZ41" s="0"/>
+      <c r="XA41" s="0"/>
+      <c r="XB41" s="0"/>
+      <c r="XC41" s="0"/>
+      <c r="XD41" s="0"/>
+      <c r="XE41" s="0"/>
+      <c r="XF41" s="0"/>
+      <c r="XG41" s="0"/>
+      <c r="XH41" s="0"/>
+      <c r="XI41" s="0"/>
+      <c r="XJ41" s="0"/>
+      <c r="XK41" s="0"/>
+      <c r="XL41" s="0"/>
+      <c r="XM41" s="0"/>
+      <c r="XN41" s="0"/>
+      <c r="XO41" s="0"/>
+      <c r="XP41" s="0"/>
+      <c r="XQ41" s="0"/>
+      <c r="XR41" s="0"/>
+      <c r="XS41" s="0"/>
+      <c r="XT41" s="0"/>
+      <c r="XU41" s="0"/>
+      <c r="XV41" s="0"/>
+      <c r="XW41" s="0"/>
+      <c r="XX41" s="0"/>
+      <c r="XY41" s="0"/>
+      <c r="XZ41" s="0"/>
+      <c r="YA41" s="0"/>
+      <c r="YB41" s="0"/>
+      <c r="YC41" s="0"/>
+      <c r="YD41" s="0"/>
+      <c r="YE41" s="0"/>
+      <c r="YF41" s="0"/>
+      <c r="YG41" s="0"/>
+      <c r="YH41" s="0"/>
+      <c r="YI41" s="0"/>
+      <c r="YJ41" s="0"/>
+      <c r="YK41" s="0"/>
+      <c r="YL41" s="0"/>
+      <c r="YM41" s="0"/>
+      <c r="YN41" s="0"/>
+      <c r="YO41" s="0"/>
+      <c r="YP41" s="0"/>
+      <c r="YQ41" s="0"/>
+      <c r="YR41" s="0"/>
+      <c r="YS41" s="0"/>
+      <c r="YT41" s="0"/>
+      <c r="YU41" s="0"/>
+      <c r="YV41" s="0"/>
+      <c r="YW41" s="0"/>
+      <c r="YX41" s="0"/>
+      <c r="YY41" s="0"/>
+      <c r="YZ41" s="0"/>
+      <c r="ZA41" s="0"/>
+      <c r="ZB41" s="0"/>
+      <c r="ZC41" s="0"/>
+      <c r="ZD41" s="0"/>
+      <c r="ZE41" s="0"/>
+      <c r="ZF41" s="0"/>
+      <c r="ZG41" s="0"/>
+      <c r="ZH41" s="0"/>
+      <c r="ZI41" s="0"/>
+      <c r="ZJ41" s="0"/>
+      <c r="ZK41" s="0"/>
+      <c r="ZL41" s="0"/>
+      <c r="ZM41" s="0"/>
+      <c r="ZN41" s="0"/>
+      <c r="ZO41" s="0"/>
+      <c r="ZP41" s="0"/>
+      <c r="ZQ41" s="0"/>
+      <c r="ZR41" s="0"/>
+      <c r="ZS41" s="0"/>
+      <c r="ZT41" s="0"/>
+      <c r="ZU41" s="0"/>
+      <c r="ZV41" s="0"/>
+      <c r="ZW41" s="0"/>
+      <c r="ZX41" s="0"/>
+      <c r="ZY41" s="0"/>
+      <c r="ZZ41" s="0"/>
+      <c r="AAA41" s="0"/>
+      <c r="AAB41" s="0"/>
+      <c r="AAC41" s="0"/>
+      <c r="AAD41" s="0"/>
+      <c r="AAE41" s="0"/>
+      <c r="AAF41" s="0"/>
+      <c r="AAG41" s="0"/>
+      <c r="AAH41" s="0"/>
+      <c r="AAI41" s="0"/>
+      <c r="AAJ41" s="0"/>
+      <c r="AAK41" s="0"/>
+      <c r="AAL41" s="0"/>
+      <c r="AAM41" s="0"/>
+      <c r="AAN41" s="0"/>
+      <c r="AAO41" s="0"/>
+      <c r="AAP41" s="0"/>
+      <c r="AAQ41" s="0"/>
+      <c r="AAR41" s="0"/>
+      <c r="AAS41" s="0"/>
+      <c r="AAT41" s="0"/>
+      <c r="AAU41" s="0"/>
+      <c r="AAV41" s="0"/>
+      <c r="AAW41" s="0"/>
+      <c r="AAX41" s="0"/>
+      <c r="AAY41" s="0"/>
+      <c r="AAZ41" s="0"/>
+      <c r="ABA41" s="0"/>
+      <c r="ABB41" s="0"/>
+      <c r="ABC41" s="0"/>
+      <c r="ABD41" s="0"/>
+      <c r="ABE41" s="0"/>
+      <c r="ABF41" s="0"/>
+      <c r="ABG41" s="0"/>
+      <c r="ABH41" s="0"/>
+      <c r="ABI41" s="0"/>
+      <c r="ABJ41" s="0"/>
+      <c r="ABK41" s="0"/>
+      <c r="ABL41" s="0"/>
+      <c r="ABM41" s="0"/>
+      <c r="ABN41" s="0"/>
+      <c r="ABO41" s="0"/>
+      <c r="ABP41" s="0"/>
+      <c r="ABQ41" s="0"/>
+      <c r="ABR41" s="0"/>
+      <c r="ABS41" s="0"/>
+      <c r="ABT41" s="0"/>
+      <c r="ABU41" s="0"/>
+      <c r="ABV41" s="0"/>
+      <c r="ABW41" s="0"/>
+      <c r="ABX41" s="0"/>
+      <c r="ABY41" s="0"/>
+      <c r="ABZ41" s="0"/>
+      <c r="ACA41" s="0"/>
+      <c r="ACB41" s="0"/>
+      <c r="ACC41" s="0"/>
+      <c r="ACD41" s="0"/>
+      <c r="ACE41" s="0"/>
+      <c r="ACF41" s="0"/>
+      <c r="ACG41" s="0"/>
+      <c r="ACH41" s="0"/>
+      <c r="ACI41" s="0"/>
+      <c r="ACJ41" s="0"/>
+      <c r="ACK41" s="0"/>
+      <c r="ACL41" s="0"/>
+      <c r="ACM41" s="0"/>
+      <c r="ACN41" s="0"/>
+      <c r="ACO41" s="0"/>
+      <c r="ACP41" s="0"/>
+      <c r="ACQ41" s="0"/>
+      <c r="ACR41" s="0"/>
+      <c r="ACS41" s="0"/>
+      <c r="ACT41" s="0"/>
+      <c r="ACU41" s="0"/>
+      <c r="ACV41" s="0"/>
+      <c r="ACW41" s="0"/>
+      <c r="ACX41" s="0"/>
+      <c r="ACY41" s="0"/>
+      <c r="ACZ41" s="0"/>
+      <c r="ADA41" s="0"/>
+      <c r="ADB41" s="0"/>
+      <c r="ADC41" s="0"/>
+      <c r="ADD41" s="0"/>
+      <c r="ADE41" s="0"/>
+      <c r="ADF41" s="0"/>
+      <c r="ADG41" s="0"/>
+      <c r="ADH41" s="0"/>
+      <c r="ADI41" s="0"/>
+      <c r="ADJ41" s="0"/>
+      <c r="ADK41" s="0"/>
+      <c r="ADL41" s="0"/>
+      <c r="ADM41" s="0"/>
+      <c r="ADN41" s="0"/>
+      <c r="ADO41" s="0"/>
+      <c r="ADP41" s="0"/>
+      <c r="ADQ41" s="0"/>
+      <c r="ADR41" s="0"/>
+      <c r="ADS41" s="0"/>
+      <c r="ADT41" s="0"/>
+      <c r="ADU41" s="0"/>
+      <c r="ADV41" s="0"/>
+      <c r="ADW41" s="0"/>
+      <c r="ADX41" s="0"/>
+      <c r="ADY41" s="0"/>
+      <c r="ADZ41" s="0"/>
+      <c r="AEA41" s="0"/>
+      <c r="AEB41" s="0"/>
+      <c r="AEC41" s="0"/>
+      <c r="AED41" s="0"/>
+      <c r="AEE41" s="0"/>
+      <c r="AEF41" s="0"/>
+      <c r="AEG41" s="0"/>
+      <c r="AEH41" s="0"/>
+      <c r="AEI41" s="0"/>
+      <c r="AEJ41" s="0"/>
+      <c r="AEK41" s="0"/>
+      <c r="AEL41" s="0"/>
+      <c r="AEM41" s="0"/>
+      <c r="AEN41" s="0"/>
+      <c r="AEO41" s="0"/>
+      <c r="AEP41" s="0"/>
+      <c r="AEQ41" s="0"/>
+      <c r="AER41" s="0"/>
+      <c r="AES41" s="0"/>
+      <c r="AET41" s="0"/>
+      <c r="AEU41" s="0"/>
+      <c r="AEV41" s="0"/>
+      <c r="AEW41" s="0"/>
+      <c r="AEX41" s="0"/>
+      <c r="AEY41" s="0"/>
+      <c r="AEZ41" s="0"/>
+      <c r="AFA41" s="0"/>
+      <c r="AFB41" s="0"/>
+      <c r="AFC41" s="0"/>
+      <c r="AFD41" s="0"/>
+      <c r="AFE41" s="0"/>
+      <c r="AFF41" s="0"/>
+      <c r="AFG41" s="0"/>
+      <c r="AFH41" s="0"/>
+      <c r="AFI41" s="0"/>
+      <c r="AFJ41" s="0"/>
+      <c r="AFK41" s="0"/>
+      <c r="AFL41" s="0"/>
+      <c r="AFM41" s="0"/>
+      <c r="AFN41" s="0"/>
+      <c r="AFO41" s="0"/>
+      <c r="AFP41" s="0"/>
+      <c r="AFQ41" s="0"/>
+      <c r="AFR41" s="0"/>
+      <c r="AFS41" s="0"/>
+      <c r="AFT41" s="0"/>
+      <c r="AFU41" s="0"/>
+      <c r="AFV41" s="0"/>
+      <c r="AFW41" s="0"/>
+      <c r="AFX41" s="0"/>
+      <c r="AFY41" s="0"/>
+      <c r="AFZ41" s="0"/>
+      <c r="AGA41" s="0"/>
+      <c r="AGB41" s="0"/>
+      <c r="AGC41" s="0"/>
+      <c r="AGD41" s="0"/>
+      <c r="AGE41" s="0"/>
+      <c r="AGF41" s="0"/>
+      <c r="AGG41" s="0"/>
+      <c r="AGH41" s="0"/>
+      <c r="AGI41" s="0"/>
+      <c r="AGJ41" s="0"/>
+      <c r="AGK41" s="0"/>
+      <c r="AGL41" s="0"/>
+      <c r="AGM41" s="0"/>
+      <c r="AGN41" s="0"/>
+      <c r="AGO41" s="0"/>
+      <c r="AGP41" s="0"/>
+      <c r="AGQ41" s="0"/>
+      <c r="AGR41" s="0"/>
+      <c r="AGS41" s="0"/>
+      <c r="AGT41" s="0"/>
+      <c r="AGU41" s="0"/>
+      <c r="AGV41" s="0"/>
+      <c r="AGW41" s="0"/>
+      <c r="AGX41" s="0"/>
+      <c r="AGY41" s="0"/>
+      <c r="AGZ41" s="0"/>
+      <c r="AHA41" s="0"/>
+      <c r="AHB41" s="0"/>
+      <c r="AHC41" s="0"/>
+      <c r="AHD41" s="0"/>
+      <c r="AHE41" s="0"/>
+      <c r="AHF41" s="0"/>
+      <c r="AHG41" s="0"/>
+      <c r="AHH41" s="0"/>
+      <c r="AHI41" s="0"/>
+      <c r="AHJ41" s="0"/>
+      <c r="AHK41" s="0"/>
+      <c r="AHL41" s="0"/>
+      <c r="AHM41" s="0"/>
+      <c r="AHN41" s="0"/>
+      <c r="AHO41" s="0"/>
+      <c r="AHP41" s="0"/>
+      <c r="AHQ41" s="0"/>
+      <c r="AHR41" s="0"/>
+      <c r="AHS41" s="0"/>
+      <c r="AHT41" s="0"/>
+      <c r="AHU41" s="0"/>
+      <c r="AHV41" s="0"/>
+      <c r="AHW41" s="0"/>
+      <c r="AHX41" s="0"/>
+      <c r="AHY41" s="0"/>
+      <c r="AHZ41" s="0"/>
+      <c r="AIA41" s="0"/>
+      <c r="AIB41" s="0"/>
+      <c r="AIC41" s="0"/>
+      <c r="AID41" s="0"/>
+      <c r="AIE41" s="0"/>
+      <c r="AIF41" s="0"/>
+      <c r="AIG41" s="0"/>
+      <c r="AIH41" s="0"/>
+      <c r="AII41" s="0"/>
+      <c r="AIJ41" s="0"/>
+      <c r="AIK41" s="0"/>
+      <c r="AIL41" s="0"/>
+      <c r="AIM41" s="0"/>
+      <c r="AIN41" s="0"/>
+      <c r="AIO41" s="0"/>
+      <c r="AIP41" s="0"/>
+      <c r="AIQ41" s="0"/>
+      <c r="AIR41" s="0"/>
+      <c r="AIS41" s="0"/>
+      <c r="AIT41" s="0"/>
+      <c r="AIU41" s="0"/>
+      <c r="AIV41" s="0"/>
+      <c r="AIW41" s="0"/>
+      <c r="AIX41" s="0"/>
+      <c r="AIY41" s="0"/>
+      <c r="AIZ41" s="0"/>
+      <c r="AJA41" s="0"/>
+      <c r="AJB41" s="0"/>
+      <c r="AJC41" s="0"/>
+      <c r="AJD41" s="0"/>
+      <c r="AJE41" s="0"/>
+      <c r="AJF41" s="0"/>
+      <c r="AJG41" s="0"/>
+      <c r="AJH41" s="0"/>
+      <c r="AJI41" s="0"/>
+      <c r="AJJ41" s="0"/>
+      <c r="AJK41" s="0"/>
+      <c r="AJL41" s="0"/>
+      <c r="AJM41" s="0"/>
+      <c r="AJN41" s="0"/>
+      <c r="AJO41" s="0"/>
+      <c r="AJP41" s="0"/>
+      <c r="AJQ41" s="0"/>
+      <c r="AJR41" s="0"/>
+      <c r="AJS41" s="0"/>
+      <c r="AJT41" s="0"/>
+      <c r="AJU41" s="0"/>
+      <c r="AJV41" s="0"/>
+      <c r="AJW41" s="0"/>
+      <c r="AJX41" s="0"/>
+      <c r="AJY41" s="0"/>
+      <c r="AJZ41" s="0"/>
+      <c r="AKA41" s="0"/>
+      <c r="AKB41" s="0"/>
+      <c r="AKC41" s="0"/>
+      <c r="AKD41" s="0"/>
+      <c r="AKE41" s="0"/>
+      <c r="AKF41" s="0"/>
+      <c r="AKG41" s="0"/>
+      <c r="AKH41" s="0"/>
+      <c r="AKI41" s="0"/>
+      <c r="AKJ41" s="0"/>
+      <c r="AKK41" s="0"/>
+      <c r="AKL41" s="0"/>
+      <c r="AKM41" s="0"/>
+      <c r="AKN41" s="0"/>
+      <c r="AKO41" s="0"/>
+      <c r="AKP41" s="0"/>
+      <c r="AKQ41" s="0"/>
+      <c r="AKR41" s="0"/>
+      <c r="AKS41" s="0"/>
+      <c r="AKT41" s="0"/>
+      <c r="AKU41" s="0"/>
+      <c r="AKV41" s="0"/>
+      <c r="AKW41" s="0"/>
+      <c r="AKX41" s="0"/>
+      <c r="AKY41" s="0"/>
+      <c r="AKZ41" s="0"/>
+      <c r="ALA41" s="0"/>
+      <c r="ALB41" s="0"/>
+      <c r="ALC41" s="0"/>
+      <c r="ALD41" s="0"/>
+      <c r="ALE41" s="0"/>
+      <c r="ALF41" s="0"/>
+      <c r="ALG41" s="0"/>
+      <c r="ALH41" s="0"/>
+      <c r="ALI41" s="0"/>
+      <c r="ALJ41" s="0"/>
+      <c r="ALK41" s="0"/>
+      <c r="ALL41" s="0"/>
+      <c r="ALM41" s="0"/>
+      <c r="ALN41" s="0"/>
+      <c r="ALO41" s="0"/>
+      <c r="ALP41" s="0"/>
+      <c r="ALQ41" s="0"/>
+      <c r="ALR41" s="0"/>
+      <c r="ALS41" s="0"/>
+      <c r="ALT41" s="0"/>
+      <c r="ALU41" s="0"/>
+      <c r="ALV41" s="0"/>
+      <c r="ALW41" s="0"/>
+      <c r="ALX41" s="0"/>
+      <c r="ALY41" s="0"/>
+      <c r="ALZ41" s="0"/>
+      <c r="AMA41" s="0"/>
+      <c r="AMB41" s="0"/>
+      <c r="AMC41" s="0"/>
+      <c r="AMD41" s="0"/>
+      <c r="AME41" s="0"/>
+      <c r="AMF41" s="0"/>
+      <c r="AMG41" s="0"/>
+      <c r="AMH41" s="0"/>
+      <c r="AMI41" s="0"/>
+      <c r="AMJ41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="18" t="n">
@@ -41705,6 +44643,985 @@
       </c>
       <c r="AR42" s="36"/>
       <c r="AS42" s="30"/>
+      <c r="AT42" s="0"/>
+      <c r="AU42" s="0"/>
+      <c r="AV42" s="0"/>
+      <c r="AW42" s="0"/>
+      <c r="AX42" s="0"/>
+      <c r="AY42" s="0"/>
+      <c r="AZ42" s="0"/>
+      <c r="BA42" s="0"/>
+      <c r="BB42" s="0"/>
+      <c r="BC42" s="0"/>
+      <c r="BD42" s="0"/>
+      <c r="BE42" s="0"/>
+      <c r="BF42" s="0"/>
+      <c r="BG42" s="0"/>
+      <c r="BH42" s="0"/>
+      <c r="BI42" s="0"/>
+      <c r="BJ42" s="0"/>
+      <c r="BK42" s="0"/>
+      <c r="BL42" s="0"/>
+      <c r="BM42" s="0"/>
+      <c r="BN42" s="0"/>
+      <c r="BO42" s="0"/>
+      <c r="BP42" s="0"/>
+      <c r="BQ42" s="0"/>
+      <c r="BR42" s="0"/>
+      <c r="BS42" s="0"/>
+      <c r="BT42" s="0"/>
+      <c r="BU42" s="0"/>
+      <c r="BV42" s="0"/>
+      <c r="BW42" s="0"/>
+      <c r="BX42" s="0"/>
+      <c r="BY42" s="0"/>
+      <c r="BZ42" s="0"/>
+      <c r="CA42" s="0"/>
+      <c r="CB42" s="0"/>
+      <c r="CC42" s="0"/>
+      <c r="CD42" s="0"/>
+      <c r="CE42" s="0"/>
+      <c r="CF42" s="0"/>
+      <c r="CG42" s="0"/>
+      <c r="CH42" s="0"/>
+      <c r="CI42" s="0"/>
+      <c r="CJ42" s="0"/>
+      <c r="CK42" s="0"/>
+      <c r="CL42" s="0"/>
+      <c r="CM42" s="0"/>
+      <c r="CN42" s="0"/>
+      <c r="CO42" s="0"/>
+      <c r="CP42" s="0"/>
+      <c r="CQ42" s="0"/>
+      <c r="CR42" s="0"/>
+      <c r="CS42" s="0"/>
+      <c r="CT42" s="0"/>
+      <c r="CU42" s="0"/>
+      <c r="CV42" s="0"/>
+      <c r="CW42" s="0"/>
+      <c r="CX42" s="0"/>
+      <c r="CY42" s="0"/>
+      <c r="CZ42" s="0"/>
+      <c r="DA42" s="0"/>
+      <c r="DB42" s="0"/>
+      <c r="DC42" s="0"/>
+      <c r="DD42" s="0"/>
+      <c r="DE42" s="0"/>
+      <c r="DF42" s="0"/>
+      <c r="DG42" s="0"/>
+      <c r="DH42" s="0"/>
+      <c r="DI42" s="0"/>
+      <c r="DJ42" s="0"/>
+      <c r="DK42" s="0"/>
+      <c r="DL42" s="0"/>
+      <c r="DM42" s="0"/>
+      <c r="DN42" s="0"/>
+      <c r="DO42" s="0"/>
+      <c r="DP42" s="0"/>
+      <c r="DQ42" s="0"/>
+      <c r="DR42" s="0"/>
+      <c r="DS42" s="0"/>
+      <c r="DT42" s="0"/>
+      <c r="DU42" s="0"/>
+      <c r="DV42" s="0"/>
+      <c r="DW42" s="0"/>
+      <c r="DX42" s="0"/>
+      <c r="DY42" s="0"/>
+      <c r="DZ42" s="0"/>
+      <c r="EA42" s="0"/>
+      <c r="EB42" s="0"/>
+      <c r="EC42" s="0"/>
+      <c r="ED42" s="0"/>
+      <c r="EE42" s="0"/>
+      <c r="EF42" s="0"/>
+      <c r="EG42" s="0"/>
+      <c r="EH42" s="0"/>
+      <c r="EI42" s="0"/>
+      <c r="EJ42" s="0"/>
+      <c r="EK42" s="0"/>
+      <c r="EL42" s="0"/>
+      <c r="EM42" s="0"/>
+      <c r="EN42" s="0"/>
+      <c r="EO42" s="0"/>
+      <c r="EP42" s="0"/>
+      <c r="EQ42" s="0"/>
+      <c r="ER42" s="0"/>
+      <c r="ES42" s="0"/>
+      <c r="ET42" s="0"/>
+      <c r="EU42" s="0"/>
+      <c r="EV42" s="0"/>
+      <c r="EW42" s="0"/>
+      <c r="EX42" s="0"/>
+      <c r="EY42" s="0"/>
+      <c r="EZ42" s="0"/>
+      <c r="FA42" s="0"/>
+      <c r="FB42" s="0"/>
+      <c r="FC42" s="0"/>
+      <c r="FD42" s="0"/>
+      <c r="FE42" s="0"/>
+      <c r="FF42" s="0"/>
+      <c r="FG42" s="0"/>
+      <c r="FH42" s="0"/>
+      <c r="FI42" s="0"/>
+      <c r="FJ42" s="0"/>
+      <c r="FK42" s="0"/>
+      <c r="FL42" s="0"/>
+      <c r="FM42" s="0"/>
+      <c r="FN42" s="0"/>
+      <c r="FO42" s="0"/>
+      <c r="FP42" s="0"/>
+      <c r="FQ42" s="0"/>
+      <c r="FR42" s="0"/>
+      <c r="FS42" s="0"/>
+      <c r="FT42" s="0"/>
+      <c r="FU42" s="0"/>
+      <c r="FV42" s="0"/>
+      <c r="FW42" s="0"/>
+      <c r="FX42" s="0"/>
+      <c r="FY42" s="0"/>
+      <c r="FZ42" s="0"/>
+      <c r="GA42" s="0"/>
+      <c r="GB42" s="0"/>
+      <c r="GC42" s="0"/>
+      <c r="GD42" s="0"/>
+      <c r="GE42" s="0"/>
+      <c r="GF42" s="0"/>
+      <c r="GG42" s="0"/>
+      <c r="GH42" s="0"/>
+      <c r="GI42" s="0"/>
+      <c r="GJ42" s="0"/>
+      <c r="GK42" s="0"/>
+      <c r="GL42" s="0"/>
+      <c r="GM42" s="0"/>
+      <c r="GN42" s="0"/>
+      <c r="GO42" s="0"/>
+      <c r="GP42" s="0"/>
+      <c r="GQ42" s="0"/>
+      <c r="GR42" s="0"/>
+      <c r="GS42" s="0"/>
+      <c r="GT42" s="0"/>
+      <c r="GU42" s="0"/>
+      <c r="GV42" s="0"/>
+      <c r="GW42" s="0"/>
+      <c r="GX42" s="0"/>
+      <c r="GY42" s="0"/>
+      <c r="GZ42" s="0"/>
+      <c r="HA42" s="0"/>
+      <c r="HB42" s="0"/>
+      <c r="HC42" s="0"/>
+      <c r="HD42" s="0"/>
+      <c r="HE42" s="0"/>
+      <c r="HF42" s="0"/>
+      <c r="HG42" s="0"/>
+      <c r="HH42" s="0"/>
+      <c r="HI42" s="0"/>
+      <c r="HJ42" s="0"/>
+      <c r="HK42" s="0"/>
+      <c r="HL42" s="0"/>
+      <c r="HM42" s="0"/>
+      <c r="HN42" s="0"/>
+      <c r="HO42" s="0"/>
+      <c r="HP42" s="0"/>
+      <c r="HQ42" s="0"/>
+      <c r="HR42" s="0"/>
+      <c r="HS42" s="0"/>
+      <c r="HT42" s="0"/>
+      <c r="HU42" s="0"/>
+      <c r="HV42" s="0"/>
+      <c r="HW42" s="0"/>
+      <c r="HX42" s="0"/>
+      <c r="HY42" s="0"/>
+      <c r="HZ42" s="0"/>
+      <c r="IA42" s="0"/>
+      <c r="IB42" s="0"/>
+      <c r="IC42" s="0"/>
+      <c r="ID42" s="0"/>
+      <c r="IE42" s="0"/>
+      <c r="IF42" s="0"/>
+      <c r="IG42" s="0"/>
+      <c r="IH42" s="0"/>
+      <c r="II42" s="0"/>
+      <c r="IJ42" s="0"/>
+      <c r="IK42" s="0"/>
+      <c r="IL42" s="0"/>
+      <c r="IM42" s="0"/>
+      <c r="IN42" s="0"/>
+      <c r="IO42" s="0"/>
+      <c r="IP42" s="0"/>
+      <c r="IQ42" s="0"/>
+      <c r="IR42" s="0"/>
+      <c r="IS42" s="0"/>
+      <c r="IT42" s="0"/>
+      <c r="IU42" s="0"/>
+      <c r="IV42" s="0"/>
+      <c r="IW42" s="0"/>
+      <c r="IX42" s="0"/>
+      <c r="IY42" s="0"/>
+      <c r="IZ42" s="0"/>
+      <c r="JA42" s="0"/>
+      <c r="JB42" s="0"/>
+      <c r="JC42" s="0"/>
+      <c r="JD42" s="0"/>
+      <c r="JE42" s="0"/>
+      <c r="JF42" s="0"/>
+      <c r="JG42" s="0"/>
+      <c r="JH42" s="0"/>
+      <c r="JI42" s="0"/>
+      <c r="JJ42" s="0"/>
+      <c r="JK42" s="0"/>
+      <c r="JL42" s="0"/>
+      <c r="JM42" s="0"/>
+      <c r="JN42" s="0"/>
+      <c r="JO42" s="0"/>
+      <c r="JP42" s="0"/>
+      <c r="JQ42" s="0"/>
+      <c r="JR42" s="0"/>
+      <c r="JS42" s="0"/>
+      <c r="JT42" s="0"/>
+      <c r="JU42" s="0"/>
+      <c r="JV42" s="0"/>
+      <c r="JW42" s="0"/>
+      <c r="JX42" s="0"/>
+      <c r="JY42" s="0"/>
+      <c r="JZ42" s="0"/>
+      <c r="KA42" s="0"/>
+      <c r="KB42" s="0"/>
+      <c r="KC42" s="0"/>
+      <c r="KD42" s="0"/>
+      <c r="KE42" s="0"/>
+      <c r="KF42" s="0"/>
+      <c r="KG42" s="0"/>
+      <c r="KH42" s="0"/>
+      <c r="KI42" s="0"/>
+      <c r="KJ42" s="0"/>
+      <c r="KK42" s="0"/>
+      <c r="KL42" s="0"/>
+      <c r="KM42" s="0"/>
+      <c r="KN42" s="0"/>
+      <c r="KO42" s="0"/>
+      <c r="KP42" s="0"/>
+      <c r="KQ42" s="0"/>
+      <c r="KR42" s="0"/>
+      <c r="KS42" s="0"/>
+      <c r="KT42" s="0"/>
+      <c r="KU42" s="0"/>
+      <c r="KV42" s="0"/>
+      <c r="KW42" s="0"/>
+      <c r="KX42" s="0"/>
+      <c r="KY42" s="0"/>
+      <c r="KZ42" s="0"/>
+      <c r="LA42" s="0"/>
+      <c r="LB42" s="0"/>
+      <c r="LC42" s="0"/>
+      <c r="LD42" s="0"/>
+      <c r="LE42" s="0"/>
+      <c r="LF42" s="0"/>
+      <c r="LG42" s="0"/>
+      <c r="LH42" s="0"/>
+      <c r="LI42" s="0"/>
+      <c r="LJ42" s="0"/>
+      <c r="LK42" s="0"/>
+      <c r="LL42" s="0"/>
+      <c r="LM42" s="0"/>
+      <c r="LN42" s="0"/>
+      <c r="LO42" s="0"/>
+      <c r="LP42" s="0"/>
+      <c r="LQ42" s="0"/>
+      <c r="LR42" s="0"/>
+      <c r="LS42" s="0"/>
+      <c r="LT42" s="0"/>
+      <c r="LU42" s="0"/>
+      <c r="LV42" s="0"/>
+      <c r="LW42" s="0"/>
+      <c r="LX42" s="0"/>
+      <c r="LY42" s="0"/>
+      <c r="LZ42" s="0"/>
+      <c r="MA42" s="0"/>
+      <c r="MB42" s="0"/>
+      <c r="MC42" s="0"/>
+      <c r="MD42" s="0"/>
+      <c r="ME42" s="0"/>
+      <c r="MF42" s="0"/>
+      <c r="MG42" s="0"/>
+      <c r="MH42" s="0"/>
+      <c r="MI42" s="0"/>
+      <c r="MJ42" s="0"/>
+      <c r="MK42" s="0"/>
+      <c r="ML42" s="0"/>
+      <c r="MM42" s="0"/>
+      <c r="MN42" s="0"/>
+      <c r="MO42" s="0"/>
+      <c r="MP42" s="0"/>
+      <c r="MQ42" s="0"/>
+      <c r="MR42" s="0"/>
+      <c r="MS42" s="0"/>
+      <c r="MT42" s="0"/>
+      <c r="MU42" s="0"/>
+      <c r="MV42" s="0"/>
+      <c r="MW42" s="0"/>
+      <c r="MX42" s="0"/>
+      <c r="MY42" s="0"/>
+      <c r="MZ42" s="0"/>
+      <c r="NA42" s="0"/>
+      <c r="NB42" s="0"/>
+      <c r="NC42" s="0"/>
+      <c r="ND42" s="0"/>
+      <c r="NE42" s="0"/>
+      <c r="NF42" s="0"/>
+      <c r="NG42" s="0"/>
+      <c r="NH42" s="0"/>
+      <c r="NI42" s="0"/>
+      <c r="NJ42" s="0"/>
+      <c r="NK42" s="0"/>
+      <c r="NL42" s="0"/>
+      <c r="NM42" s="0"/>
+      <c r="NN42" s="0"/>
+      <c r="NO42" s="0"/>
+      <c r="NP42" s="0"/>
+      <c r="NQ42" s="0"/>
+      <c r="NR42" s="0"/>
+      <c r="NS42" s="0"/>
+      <c r="NT42" s="0"/>
+      <c r="NU42" s="0"/>
+      <c r="NV42" s="0"/>
+      <c r="NW42" s="0"/>
+      <c r="NX42" s="0"/>
+      <c r="NY42" s="0"/>
+      <c r="NZ42" s="0"/>
+      <c r="OA42" s="0"/>
+      <c r="OB42" s="0"/>
+      <c r="OC42" s="0"/>
+      <c r="OD42" s="0"/>
+      <c r="OE42" s="0"/>
+      <c r="OF42" s="0"/>
+      <c r="OG42" s="0"/>
+      <c r="OH42" s="0"/>
+      <c r="OI42" s="0"/>
+      <c r="OJ42" s="0"/>
+      <c r="OK42" s="0"/>
+      <c r="OL42" s="0"/>
+      <c r="OM42" s="0"/>
+      <c r="ON42" s="0"/>
+      <c r="OO42" s="0"/>
+      <c r="OP42" s="0"/>
+      <c r="OQ42" s="0"/>
+      <c r="OR42" s="0"/>
+      <c r="OS42" s="0"/>
+      <c r="OT42" s="0"/>
+      <c r="OU42" s="0"/>
+      <c r="OV42" s="0"/>
+      <c r="OW42" s="0"/>
+      <c r="OX42" s="0"/>
+      <c r="OY42" s="0"/>
+      <c r="OZ42" s="0"/>
+      <c r="PA42" s="0"/>
+      <c r="PB42" s="0"/>
+      <c r="PC42" s="0"/>
+      <c r="PD42" s="0"/>
+      <c r="PE42" s="0"/>
+      <c r="PF42" s="0"/>
+      <c r="PG42" s="0"/>
+      <c r="PH42" s="0"/>
+      <c r="PI42" s="0"/>
+      <c r="PJ42" s="0"/>
+      <c r="PK42" s="0"/>
+      <c r="PL42" s="0"/>
+      <c r="PM42" s="0"/>
+      <c r="PN42" s="0"/>
+      <c r="PO42" s="0"/>
+      <c r="PP42" s="0"/>
+      <c r="PQ42" s="0"/>
+      <c r="PR42" s="0"/>
+      <c r="PS42" s="0"/>
+      <c r="PT42" s="0"/>
+      <c r="PU42" s="0"/>
+      <c r="PV42" s="0"/>
+      <c r="PW42" s="0"/>
+      <c r="PX42" s="0"/>
+      <c r="PY42" s="0"/>
+      <c r="PZ42" s="0"/>
+      <c r="QA42" s="0"/>
+      <c r="QB42" s="0"/>
+      <c r="QC42" s="0"/>
+      <c r="QD42" s="0"/>
+      <c r="QE42" s="0"/>
+      <c r="QF42" s="0"/>
+      <c r="QG42" s="0"/>
+      <c r="QH42" s="0"/>
+      <c r="QI42" s="0"/>
+      <c r="QJ42" s="0"/>
+      <c r="QK42" s="0"/>
+      <c r="QL42" s="0"/>
+      <c r="QM42" s="0"/>
+      <c r="QN42" s="0"/>
+      <c r="QO42" s="0"/>
+      <c r="QP42" s="0"/>
+      <c r="QQ42" s="0"/>
+      <c r="QR42" s="0"/>
+      <c r="QS42" s="0"/>
+      <c r="QT42" s="0"/>
+      <c r="QU42" s="0"/>
+      <c r="QV42" s="0"/>
+      <c r="QW42" s="0"/>
+      <c r="QX42" s="0"/>
+      <c r="QY42" s="0"/>
+      <c r="QZ42" s="0"/>
+      <c r="RA42" s="0"/>
+      <c r="RB42" s="0"/>
+      <c r="RC42" s="0"/>
+      <c r="RD42" s="0"/>
+      <c r="RE42" s="0"/>
+      <c r="RF42" s="0"/>
+      <c r="RG42" s="0"/>
+      <c r="RH42" s="0"/>
+      <c r="RI42" s="0"/>
+      <c r="RJ42" s="0"/>
+      <c r="RK42" s="0"/>
+      <c r="RL42" s="0"/>
+      <c r="RM42" s="0"/>
+      <c r="RN42" s="0"/>
+      <c r="RO42" s="0"/>
+      <c r="RP42" s="0"/>
+      <c r="RQ42" s="0"/>
+      <c r="RR42" s="0"/>
+      <c r="RS42" s="0"/>
+      <c r="RT42" s="0"/>
+      <c r="RU42" s="0"/>
+      <c r="RV42" s="0"/>
+      <c r="RW42" s="0"/>
+      <c r="RX42" s="0"/>
+      <c r="RY42" s="0"/>
+      <c r="RZ42" s="0"/>
+      <c r="SA42" s="0"/>
+      <c r="SB42" s="0"/>
+      <c r="SC42" s="0"/>
+      <c r="SD42" s="0"/>
+      <c r="SE42" s="0"/>
+      <c r="SF42" s="0"/>
+      <c r="SG42" s="0"/>
+      <c r="SH42" s="0"/>
+      <c r="SI42" s="0"/>
+      <c r="SJ42" s="0"/>
+      <c r="SK42" s="0"/>
+      <c r="SL42" s="0"/>
+      <c r="SM42" s="0"/>
+      <c r="SN42" s="0"/>
+      <c r="SO42" s="0"/>
+      <c r="SP42" s="0"/>
+      <c r="SQ42" s="0"/>
+      <c r="SR42" s="0"/>
+      <c r="SS42" s="0"/>
+      <c r="ST42" s="0"/>
+      <c r="SU42" s="0"/>
+      <c r="SV42" s="0"/>
+      <c r="SW42" s="0"/>
+      <c r="SX42" s="0"/>
+      <c r="SY42" s="0"/>
+      <c r="SZ42" s="0"/>
+      <c r="TA42" s="0"/>
+      <c r="TB42" s="0"/>
+      <c r="TC42" s="0"/>
+      <c r="TD42" s="0"/>
+      <c r="TE42" s="0"/>
+      <c r="TF42" s="0"/>
+      <c r="TG42" s="0"/>
+      <c r="TH42" s="0"/>
+      <c r="TI42" s="0"/>
+      <c r="TJ42" s="0"/>
+      <c r="TK42" s="0"/>
+      <c r="TL42" s="0"/>
+      <c r="TM42" s="0"/>
+      <c r="TN42" s="0"/>
+      <c r="TO42" s="0"/>
+      <c r="TP42" s="0"/>
+      <c r="TQ42" s="0"/>
+      <c r="TR42" s="0"/>
+      <c r="TS42" s="0"/>
+      <c r="TT42" s="0"/>
+      <c r="TU42" s="0"/>
+      <c r="TV42" s="0"/>
+      <c r="TW42" s="0"/>
+      <c r="TX42" s="0"/>
+      <c r="TY42" s="0"/>
+      <c r="TZ42" s="0"/>
+      <c r="UA42" s="0"/>
+      <c r="UB42" s="0"/>
+      <c r="UC42" s="0"/>
+      <c r="UD42" s="0"/>
+      <c r="UE42" s="0"/>
+      <c r="UF42" s="0"/>
+      <c r="UG42" s="0"/>
+      <c r="UH42" s="0"/>
+      <c r="UI42" s="0"/>
+      <c r="UJ42" s="0"/>
+      <c r="UK42" s="0"/>
+      <c r="UL42" s="0"/>
+      <c r="UM42" s="0"/>
+      <c r="UN42" s="0"/>
+      <c r="UO42" s="0"/>
+      <c r="UP42" s="0"/>
+      <c r="UQ42" s="0"/>
+      <c r="UR42" s="0"/>
+      <c r="US42" s="0"/>
+      <c r="UT42" s="0"/>
+      <c r="UU42" s="0"/>
+      <c r="UV42" s="0"/>
+      <c r="UW42" s="0"/>
+      <c r="UX42" s="0"/>
+      <c r="UY42" s="0"/>
+      <c r="UZ42" s="0"/>
+      <c r="VA42" s="0"/>
+      <c r="VB42" s="0"/>
+      <c r="VC42" s="0"/>
+      <c r="VD42" s="0"/>
+      <c r="VE42" s="0"/>
+      <c r="VF42" s="0"/>
+      <c r="VG42" s="0"/>
+      <c r="VH42" s="0"/>
+      <c r="VI42" s="0"/>
+      <c r="VJ42" s="0"/>
+      <c r="VK42" s="0"/>
+      <c r="VL42" s="0"/>
+      <c r="VM42" s="0"/>
+      <c r="VN42" s="0"/>
+      <c r="VO42" s="0"/>
+      <c r="VP42" s="0"/>
+      <c r="VQ42" s="0"/>
+      <c r="VR42" s="0"/>
+      <c r="VS42" s="0"/>
+      <c r="VT42" s="0"/>
+      <c r="VU42" s="0"/>
+      <c r="VV42" s="0"/>
+      <c r="VW42" s="0"/>
+      <c r="VX42" s="0"/>
+      <c r="VY42" s="0"/>
+      <c r="VZ42" s="0"/>
+      <c r="WA42" s="0"/>
+      <c r="WB42" s="0"/>
+      <c r="WC42" s="0"/>
+      <c r="WD42" s="0"/>
+      <c r="WE42" s="0"/>
+      <c r="WF42" s="0"/>
+      <c r="WG42" s="0"/>
+      <c r="WH42" s="0"/>
+      <c r="WI42" s="0"/>
+      <c r="WJ42" s="0"/>
+      <c r="WK42" s="0"/>
+      <c r="WL42" s="0"/>
+      <c r="WM42" s="0"/>
+      <c r="WN42" s="0"/>
+      <c r="WO42" s="0"/>
+      <c r="WP42" s="0"/>
+      <c r="WQ42" s="0"/>
+      <c r="WR42" s="0"/>
+      <c r="WS42" s="0"/>
+      <c r="WT42" s="0"/>
+      <c r="WU42" s="0"/>
+      <c r="WV42" s="0"/>
+      <c r="WW42" s="0"/>
+      <c r="WX42" s="0"/>
+      <c r="WY42" s="0"/>
+      <c r="WZ42" s="0"/>
+      <c r="XA42" s="0"/>
+      <c r="XB42" s="0"/>
+      <c r="XC42" s="0"/>
+      <c r="XD42" s="0"/>
+      <c r="XE42" s="0"/>
+      <c r="XF42" s="0"/>
+      <c r="XG42" s="0"/>
+      <c r="XH42" s="0"/>
+      <c r="XI42" s="0"/>
+      <c r="XJ42" s="0"/>
+      <c r="XK42" s="0"/>
+      <c r="XL42" s="0"/>
+      <c r="XM42" s="0"/>
+      <c r="XN42" s="0"/>
+      <c r="XO42" s="0"/>
+      <c r="XP42" s="0"/>
+      <c r="XQ42" s="0"/>
+      <c r="XR42" s="0"/>
+      <c r="XS42" s="0"/>
+      <c r="XT42" s="0"/>
+      <c r="XU42" s="0"/>
+      <c r="XV42" s="0"/>
+      <c r="XW42" s="0"/>
+      <c r="XX42" s="0"/>
+      <c r="XY42" s="0"/>
+      <c r="XZ42" s="0"/>
+      <c r="YA42" s="0"/>
+      <c r="YB42" s="0"/>
+      <c r="YC42" s="0"/>
+      <c r="YD42" s="0"/>
+      <c r="YE42" s="0"/>
+      <c r="YF42" s="0"/>
+      <c r="YG42" s="0"/>
+      <c r="YH42" s="0"/>
+      <c r="YI42" s="0"/>
+      <c r="YJ42" s="0"/>
+      <c r="YK42" s="0"/>
+      <c r="YL42" s="0"/>
+      <c r="YM42" s="0"/>
+      <c r="YN42" s="0"/>
+      <c r="YO42" s="0"/>
+      <c r="YP42" s="0"/>
+      <c r="YQ42" s="0"/>
+      <c r="YR42" s="0"/>
+      <c r="YS42" s="0"/>
+      <c r="YT42" s="0"/>
+      <c r="YU42" s="0"/>
+      <c r="YV42" s="0"/>
+      <c r="YW42" s="0"/>
+      <c r="YX42" s="0"/>
+      <c r="YY42" s="0"/>
+      <c r="YZ42" s="0"/>
+      <c r="ZA42" s="0"/>
+      <c r="ZB42" s="0"/>
+      <c r="ZC42" s="0"/>
+      <c r="ZD42" s="0"/>
+      <c r="ZE42" s="0"/>
+      <c r="ZF42" s="0"/>
+      <c r="ZG42" s="0"/>
+      <c r="ZH42" s="0"/>
+      <c r="ZI42" s="0"/>
+      <c r="ZJ42" s="0"/>
+      <c r="ZK42" s="0"/>
+      <c r="ZL42" s="0"/>
+      <c r="ZM42" s="0"/>
+      <c r="ZN42" s="0"/>
+      <c r="ZO42" s="0"/>
+      <c r="ZP42" s="0"/>
+      <c r="ZQ42" s="0"/>
+      <c r="ZR42" s="0"/>
+      <c r="ZS42" s="0"/>
+      <c r="ZT42" s="0"/>
+      <c r="ZU42" s="0"/>
+      <c r="ZV42" s="0"/>
+      <c r="ZW42" s="0"/>
+      <c r="ZX42" s="0"/>
+      <c r="ZY42" s="0"/>
+      <c r="ZZ42" s="0"/>
+      <c r="AAA42" s="0"/>
+      <c r="AAB42" s="0"/>
+      <c r="AAC42" s="0"/>
+      <c r="AAD42" s="0"/>
+      <c r="AAE42" s="0"/>
+      <c r="AAF42" s="0"/>
+      <c r="AAG42" s="0"/>
+      <c r="AAH42" s="0"/>
+      <c r="AAI42" s="0"/>
+      <c r="AAJ42" s="0"/>
+      <c r="AAK42" s="0"/>
+      <c r="AAL42" s="0"/>
+      <c r="AAM42" s="0"/>
+      <c r="AAN42" s="0"/>
+      <c r="AAO42" s="0"/>
+      <c r="AAP42" s="0"/>
+      <c r="AAQ42" s="0"/>
+      <c r="AAR42" s="0"/>
+      <c r="AAS42" s="0"/>
+      <c r="AAT42" s="0"/>
+      <c r="AAU42" s="0"/>
+      <c r="AAV42" s="0"/>
+      <c r="AAW42" s="0"/>
+      <c r="AAX42" s="0"/>
+      <c r="AAY42" s="0"/>
+      <c r="AAZ42" s="0"/>
+      <c r="ABA42" s="0"/>
+      <c r="ABB42" s="0"/>
+      <c r="ABC42" s="0"/>
+      <c r="ABD42" s="0"/>
+      <c r="ABE42" s="0"/>
+      <c r="ABF42" s="0"/>
+      <c r="ABG42" s="0"/>
+      <c r="ABH42" s="0"/>
+      <c r="ABI42" s="0"/>
+      <c r="ABJ42" s="0"/>
+      <c r="ABK42" s="0"/>
+      <c r="ABL42" s="0"/>
+      <c r="ABM42" s="0"/>
+      <c r="ABN42" s="0"/>
+      <c r="ABO42" s="0"/>
+      <c r="ABP42" s="0"/>
+      <c r="ABQ42" s="0"/>
+      <c r="ABR42" s="0"/>
+      <c r="ABS42" s="0"/>
+      <c r="ABT42" s="0"/>
+      <c r="ABU42" s="0"/>
+      <c r="ABV42" s="0"/>
+      <c r="ABW42" s="0"/>
+      <c r="ABX42" s="0"/>
+      <c r="ABY42" s="0"/>
+      <c r="ABZ42" s="0"/>
+      <c r="ACA42" s="0"/>
+      <c r="ACB42" s="0"/>
+      <c r="ACC42" s="0"/>
+      <c r="ACD42" s="0"/>
+      <c r="ACE42" s="0"/>
+      <c r="ACF42" s="0"/>
+      <c r="ACG42" s="0"/>
+      <c r="ACH42" s="0"/>
+      <c r="ACI42" s="0"/>
+      <c r="ACJ42" s="0"/>
+      <c r="ACK42" s="0"/>
+      <c r="ACL42" s="0"/>
+      <c r="ACM42" s="0"/>
+      <c r="ACN42" s="0"/>
+      <c r="ACO42" s="0"/>
+      <c r="ACP42" s="0"/>
+      <c r="ACQ42" s="0"/>
+      <c r="ACR42" s="0"/>
+      <c r="ACS42" s="0"/>
+      <c r="ACT42" s="0"/>
+      <c r="ACU42" s="0"/>
+      <c r="ACV42" s="0"/>
+      <c r="ACW42" s="0"/>
+      <c r="ACX42" s="0"/>
+      <c r="ACY42" s="0"/>
+      <c r="ACZ42" s="0"/>
+      <c r="ADA42" s="0"/>
+      <c r="ADB42" s="0"/>
+      <c r="ADC42" s="0"/>
+      <c r="ADD42" s="0"/>
+      <c r="ADE42" s="0"/>
+      <c r="ADF42" s="0"/>
+      <c r="ADG42" s="0"/>
+      <c r="ADH42" s="0"/>
+      <c r="ADI42" s="0"/>
+      <c r="ADJ42" s="0"/>
+      <c r="ADK42" s="0"/>
+      <c r="ADL42" s="0"/>
+      <c r="ADM42" s="0"/>
+      <c r="ADN42" s="0"/>
+      <c r="ADO42" s="0"/>
+      <c r="ADP42" s="0"/>
+      <c r="ADQ42" s="0"/>
+      <c r="ADR42" s="0"/>
+      <c r="ADS42" s="0"/>
+      <c r="ADT42" s="0"/>
+      <c r="ADU42" s="0"/>
+      <c r="ADV42" s="0"/>
+      <c r="ADW42" s="0"/>
+      <c r="ADX42" s="0"/>
+      <c r="ADY42" s="0"/>
+      <c r="ADZ42" s="0"/>
+      <c r="AEA42" s="0"/>
+      <c r="AEB42" s="0"/>
+      <c r="AEC42" s="0"/>
+      <c r="AED42" s="0"/>
+      <c r="AEE42" s="0"/>
+      <c r="AEF42" s="0"/>
+      <c r="AEG42" s="0"/>
+      <c r="AEH42" s="0"/>
+      <c r="AEI42" s="0"/>
+      <c r="AEJ42" s="0"/>
+      <c r="AEK42" s="0"/>
+      <c r="AEL42" s="0"/>
+      <c r="AEM42" s="0"/>
+      <c r="AEN42" s="0"/>
+      <c r="AEO42" s="0"/>
+      <c r="AEP42" s="0"/>
+      <c r="AEQ42" s="0"/>
+      <c r="AER42" s="0"/>
+      <c r="AES42" s="0"/>
+      <c r="AET42" s="0"/>
+      <c r="AEU42" s="0"/>
+      <c r="AEV42" s="0"/>
+      <c r="AEW42" s="0"/>
+      <c r="AEX42" s="0"/>
+      <c r="AEY42" s="0"/>
+      <c r="AEZ42" s="0"/>
+      <c r="AFA42" s="0"/>
+      <c r="AFB42" s="0"/>
+      <c r="AFC42" s="0"/>
+      <c r="AFD42" s="0"/>
+      <c r="AFE42" s="0"/>
+      <c r="AFF42" s="0"/>
+      <c r="AFG42" s="0"/>
+      <c r="AFH42" s="0"/>
+      <c r="AFI42" s="0"/>
+      <c r="AFJ42" s="0"/>
+      <c r="AFK42" s="0"/>
+      <c r="AFL42" s="0"/>
+      <c r="AFM42" s="0"/>
+      <c r="AFN42" s="0"/>
+      <c r="AFO42" s="0"/>
+      <c r="AFP42" s="0"/>
+      <c r="AFQ42" s="0"/>
+      <c r="AFR42" s="0"/>
+      <c r="AFS42" s="0"/>
+      <c r="AFT42" s="0"/>
+      <c r="AFU42" s="0"/>
+      <c r="AFV42" s="0"/>
+      <c r="AFW42" s="0"/>
+      <c r="AFX42" s="0"/>
+      <c r="AFY42" s="0"/>
+      <c r="AFZ42" s="0"/>
+      <c r="AGA42" s="0"/>
+      <c r="AGB42" s="0"/>
+      <c r="AGC42" s="0"/>
+      <c r="AGD42" s="0"/>
+      <c r="AGE42" s="0"/>
+      <c r="AGF42" s="0"/>
+      <c r="AGG42" s="0"/>
+      <c r="AGH42" s="0"/>
+      <c r="AGI42" s="0"/>
+      <c r="AGJ42" s="0"/>
+      <c r="AGK42" s="0"/>
+      <c r="AGL42" s="0"/>
+      <c r="AGM42" s="0"/>
+      <c r="AGN42" s="0"/>
+      <c r="AGO42" s="0"/>
+      <c r="AGP42" s="0"/>
+      <c r="AGQ42" s="0"/>
+      <c r="AGR42" s="0"/>
+      <c r="AGS42" s="0"/>
+      <c r="AGT42" s="0"/>
+      <c r="AGU42" s="0"/>
+      <c r="AGV42" s="0"/>
+      <c r="AGW42" s="0"/>
+      <c r="AGX42" s="0"/>
+      <c r="AGY42" s="0"/>
+      <c r="AGZ42" s="0"/>
+      <c r="AHA42" s="0"/>
+      <c r="AHB42" s="0"/>
+      <c r="AHC42" s="0"/>
+      <c r="AHD42" s="0"/>
+      <c r="AHE42" s="0"/>
+      <c r="AHF42" s="0"/>
+      <c r="AHG42" s="0"/>
+      <c r="AHH42" s="0"/>
+      <c r="AHI42" s="0"/>
+      <c r="AHJ42" s="0"/>
+      <c r="AHK42" s="0"/>
+      <c r="AHL42" s="0"/>
+      <c r="AHM42" s="0"/>
+      <c r="AHN42" s="0"/>
+      <c r="AHO42" s="0"/>
+      <c r="AHP42" s="0"/>
+      <c r="AHQ42" s="0"/>
+      <c r="AHR42" s="0"/>
+      <c r="AHS42" s="0"/>
+      <c r="AHT42" s="0"/>
+      <c r="AHU42" s="0"/>
+      <c r="AHV42" s="0"/>
+      <c r="AHW42" s="0"/>
+      <c r="AHX42" s="0"/>
+      <c r="AHY42" s="0"/>
+      <c r="AHZ42" s="0"/>
+      <c r="AIA42" s="0"/>
+      <c r="AIB42" s="0"/>
+      <c r="AIC42" s="0"/>
+      <c r="AID42" s="0"/>
+      <c r="AIE42" s="0"/>
+      <c r="AIF42" s="0"/>
+      <c r="AIG42" s="0"/>
+      <c r="AIH42" s="0"/>
+      <c r="AII42" s="0"/>
+      <c r="AIJ42" s="0"/>
+      <c r="AIK42" s="0"/>
+      <c r="AIL42" s="0"/>
+      <c r="AIM42" s="0"/>
+      <c r="AIN42" s="0"/>
+      <c r="AIO42" s="0"/>
+      <c r="AIP42" s="0"/>
+      <c r="AIQ42" s="0"/>
+      <c r="AIR42" s="0"/>
+      <c r="AIS42" s="0"/>
+      <c r="AIT42" s="0"/>
+      <c r="AIU42" s="0"/>
+      <c r="AIV42" s="0"/>
+      <c r="AIW42" s="0"/>
+      <c r="AIX42" s="0"/>
+      <c r="AIY42" s="0"/>
+      <c r="AIZ42" s="0"/>
+      <c r="AJA42" s="0"/>
+      <c r="AJB42" s="0"/>
+      <c r="AJC42" s="0"/>
+      <c r="AJD42" s="0"/>
+      <c r="AJE42" s="0"/>
+      <c r="AJF42" s="0"/>
+      <c r="AJG42" s="0"/>
+      <c r="AJH42" s="0"/>
+      <c r="AJI42" s="0"/>
+      <c r="AJJ42" s="0"/>
+      <c r="AJK42" s="0"/>
+      <c r="AJL42" s="0"/>
+      <c r="AJM42" s="0"/>
+      <c r="AJN42" s="0"/>
+      <c r="AJO42" s="0"/>
+      <c r="AJP42" s="0"/>
+      <c r="AJQ42" s="0"/>
+      <c r="AJR42" s="0"/>
+      <c r="AJS42" s="0"/>
+      <c r="AJT42" s="0"/>
+      <c r="AJU42" s="0"/>
+      <c r="AJV42" s="0"/>
+      <c r="AJW42" s="0"/>
+      <c r="AJX42" s="0"/>
+      <c r="AJY42" s="0"/>
+      <c r="AJZ42" s="0"/>
+      <c r="AKA42" s="0"/>
+      <c r="AKB42" s="0"/>
+      <c r="AKC42" s="0"/>
+      <c r="AKD42" s="0"/>
+      <c r="AKE42" s="0"/>
+      <c r="AKF42" s="0"/>
+      <c r="AKG42" s="0"/>
+      <c r="AKH42" s="0"/>
+      <c r="AKI42" s="0"/>
+      <c r="AKJ42" s="0"/>
+      <c r="AKK42" s="0"/>
+      <c r="AKL42" s="0"/>
+      <c r="AKM42" s="0"/>
+      <c r="AKN42" s="0"/>
+      <c r="AKO42" s="0"/>
+      <c r="AKP42" s="0"/>
+      <c r="AKQ42" s="0"/>
+      <c r="AKR42" s="0"/>
+      <c r="AKS42" s="0"/>
+      <c r="AKT42" s="0"/>
+      <c r="AKU42" s="0"/>
+      <c r="AKV42" s="0"/>
+      <c r="AKW42" s="0"/>
+      <c r="AKX42" s="0"/>
+      <c r="AKY42" s="0"/>
+      <c r="AKZ42" s="0"/>
+      <c r="ALA42" s="0"/>
+      <c r="ALB42" s="0"/>
+      <c r="ALC42" s="0"/>
+      <c r="ALD42" s="0"/>
+      <c r="ALE42" s="0"/>
+      <c r="ALF42" s="0"/>
+      <c r="ALG42" s="0"/>
+      <c r="ALH42" s="0"/>
+      <c r="ALI42" s="0"/>
+      <c r="ALJ42" s="0"/>
+      <c r="ALK42" s="0"/>
+      <c r="ALL42" s="0"/>
+      <c r="ALM42" s="0"/>
+      <c r="ALN42" s="0"/>
+      <c r="ALO42" s="0"/>
+      <c r="ALP42" s="0"/>
+      <c r="ALQ42" s="0"/>
+      <c r="ALR42" s="0"/>
+      <c r="ALS42" s="0"/>
+      <c r="ALT42" s="0"/>
+      <c r="ALU42" s="0"/>
+      <c r="ALV42" s="0"/>
+      <c r="ALW42" s="0"/>
+      <c r="ALX42" s="0"/>
+      <c r="ALY42" s="0"/>
+      <c r="ALZ42" s="0"/>
+      <c r="AMA42" s="0"/>
+      <c r="AMB42" s="0"/>
+      <c r="AMC42" s="0"/>
+      <c r="AMD42" s="0"/>
+      <c r="AME42" s="0"/>
+      <c r="AMF42" s="0"/>
+      <c r="AMG42" s="0"/>
+      <c r="AMH42" s="0"/>
+      <c r="AMI42" s="0"/>
+      <c r="AMJ42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="18" t="n">
@@ -49116,12 +53033,12 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="43:49 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.553488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
CCRU - template fix
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/HoReCa Bar Tavern_Night Club PoS 2018.xlsx
+++ b/Projects/CCRU/Data/HoReCa Bar Tavern_Night Club PoS 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="HoReCa Bar Tavern_Night Club" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,12 +25,12 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AS$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AS$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AS$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AS$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AS$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AS$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AS$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AS$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AS$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
@@ -41,6 +41,12 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$B$1:$AR$42</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -122,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="223">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -634,10 +640,10 @@
     <t xml:space="preserve">Relax после работы: Миксабилити</t>
   </si>
   <si>
-    <t xml:space="preserve">RED Hackle mix_img (2), Finlandia and Rich Cherry, Finlandia and Rich menu insert, Finlandia and Rich Mix, Finlandia and Rich Orange, Finlandia and Rich table tent, Finlandia and Schweppes Menu Insert, Finlandia and Schweppes Table Tent, Finlandia and Schweppes, Jack and Coke Menu, Jack and Coke Table tent, Jack Daniles and Coke Mix, Jack Daniles and Coke, Finlandia and Rich Sticker Cherry, Finlandia and Rich Sticker Orange, Finlandia and Rich table tent Cherry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A5B10100, A5B10101, 7777888899, 7777888900, 7777888901, 7777888902, 7777888903, 7777888904, 7777888905, 7777888906, 7777888907, 7777888908, 7777888909, 7777888910, 7777889000, 7777889001, 7777889002</t>
+    <t xml:space="preserve">RED Hackle mix_img (2), Finlandia and Rich Cherry, Finlandia and Rich menu insert, Finlandia and Rich Mix, Finlandia and Rich Orange, Finlandia and Rich table tent, Finlandia and Schweppes Menu Insert, Finlandia and Schweppes Table Tent, Finlandia and Schweppes, Jack and Coke Menu, Jack and Coke Table tent, Jack Daniles and Coke Mix, Jack Daniles and Coke, Finlandia and Rich Sticker Cherry, Finlandia and Rich Sticker Orange, Finlandia and Rich table tent Cherry, CC_FWC_Cocktail_WRK-01, CC_FWC_Cocktail_WRK-02, CC_FWC_Cocktail_WRK-03, CC_FWC_Cocktail_WRK-04, Cocktails_2018, Schweppes_Magnit_2, Schweppes_Magnit_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5B10100, A5B10101, 7777888899, 7777888900, 7777888901, 7777888902, 7777888903, 7777888904, 7777888905, 7777888906, 7777888907, 7777888908, 7777888909, 7777888910, 7777889000, 7777889001, 7777889002, A5B10105, A5B10106, A5B10107, A5B10108, A5B10112, A5B10111</t>
   </si>
   <si>
     <t xml:space="preserve">Midday socializing: Moctails</t>
@@ -646,7 +652,10 @@
     <t xml:space="preserve">Relax после работы: Моктели</t>
   </si>
   <si>
-    <t xml:space="preserve">new</t>
+    <t xml:space="preserve">Mocktails_2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5B10109</t>
   </si>
   <si>
     <t xml:space="preserve">Drink Out: Party night</t>
@@ -902,10 +911,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+      <charset val="204"/>
     </font>
     <font>
       <b val="true"/>
@@ -933,8 +943,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -975,7 +985,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1001,11 +1011,14 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1110,10 +1123,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="7" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1130,7 +1139,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1175,14 +1192,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Good" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1195,7 +1213,7 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006100"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -1220,7 +1238,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFC6EFCE"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -1258,9 +1276,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>736200</xdr:colOff>
+      <xdr:colOff>734040</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>311040</xdr:rowOff>
+      <xdr:rowOff>308880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1270,7 +1288,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="513000" y="0"/>
-          <a:ext cx="17472240" cy="12548520"/>
+          <a:ext cx="20623320" cy="12546360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1303,9 +1321,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>736200</xdr:colOff>
+      <xdr:colOff>734040</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>311040</xdr:rowOff>
+      <xdr:rowOff>308880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1315,7 +1333,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="513000" y="0"/>
-          <a:ext cx="17472240" cy="12548520"/>
+          <a:ext cx="20623320" cy="12546360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1348,9 +1366,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>736200</xdr:colOff>
+      <xdr:colOff>734040</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>311040</xdr:rowOff>
+      <xdr:rowOff>308880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1360,7 +1378,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="513000" y="0"/>
-          <a:ext cx="17472240" cy="12548520"/>
+          <a:ext cx="20623320" cy="12546360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1393,9 +1411,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>736200</xdr:colOff>
+      <xdr:colOff>734040</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>311040</xdr:rowOff>
+      <xdr:rowOff>308880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1405,7 +1423,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="513000" y="0"/>
-          <a:ext cx="17472240" cy="12548520"/>
+          <a:ext cx="20623320" cy="12546360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1440,19 +1458,19 @@
   </sheetPr>
   <dimension ref="A1:AS49"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="H2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="H29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="O35" activeCellId="0" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="43.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="14.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="51.4418604651163"/>
-    <col collapsed="false" hidden="false" max="32" min="9" style="1" width="14.9953488372093"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="2" width="14.9953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="34" style="1" width="14.9953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="17.6"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="61.4093023255814"/>
+    <col collapsed="false" hidden="false" max="32" min="9" style="1" width="17.6"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="2" width="17.6"/>
+    <col collapsed="false" hidden="false" max="1025" min="34" style="1" width="17.6"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3496,7 +3514,7 @@
       <c r="G24" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="H24" s="26" t="s">
+      <c r="H24" s="23" t="s">
         <v>110</v>
       </c>
       <c r="I24" s="11" t="s">
@@ -3633,10 +3651,10 @@
       <c r="AG25" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH25" s="27" t="n">
+      <c r="AH25" s="26" t="n">
         <v>0.15</v>
       </c>
-      <c r="AI25" s="28"/>
+      <c r="AI25" s="27"/>
       <c r="AJ25" s="13"/>
       <c r="AK25" s="13"/>
       <c r="AL25" s="13"/>
@@ -3708,15 +3726,15 @@
       </c>
       <c r="AB26" s="11"/>
       <c r="AC26" s="11"/>
-      <c r="AD26" s="29"/>
-      <c r="AE26" s="29"/>
+      <c r="AD26" s="28"/>
+      <c r="AE26" s="28"/>
       <c r="AF26" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG26" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH26" s="27" t="n">
+      <c r="AH26" s="26" t="n">
         <v>0.05</v>
       </c>
       <c r="AI26" s="11"/>
@@ -3803,20 +3821,20 @@
       </c>
       <c r="AB27" s="11"/>
       <c r="AC27" s="11"/>
-      <c r="AD27" s="29"/>
-      <c r="AE27" s="29"/>
+      <c r="AD27" s="28"/>
+      <c r="AE27" s="28"/>
       <c r="AF27" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG27" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH27" s="27" t="n">
+      <c r="AH27" s="26" t="n">
         <v>0</v>
       </c>
       <c r="AI27" s="11"/>
       <c r="AJ27" s="13"/>
-      <c r="AK27" s="30"/>
+      <c r="AK27" s="29"/>
       <c r="AL27" s="13"/>
       <c r="AM27" s="13"/>
       <c r="AN27" s="13" t="n">
@@ -3894,20 +3912,20 @@
       </c>
       <c r="AB28" s="11"/>
       <c r="AC28" s="11"/>
-      <c r="AD28" s="29"/>
-      <c r="AE28" s="29"/>
+      <c r="AD28" s="28"/>
+      <c r="AE28" s="28"/>
       <c r="AF28" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG28" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH28" s="27" t="n">
+      <c r="AH28" s="26" t="n">
         <v>0</v>
       </c>
       <c r="AI28" s="11"/>
       <c r="AJ28" s="13"/>
-      <c r="AK28" s="30"/>
+      <c r="AK28" s="29"/>
       <c r="AL28" s="13"/>
       <c r="AM28" s="13"/>
       <c r="AN28" s="13" t="n">
@@ -3949,6 +3967,7 @@
       <c r="I29" s="1" t="s">
         <v>137</v>
       </c>
+      <c r="J29" s="0"/>
       <c r="K29" s="11" t="n">
         <v>2</v>
       </c>
@@ -3986,20 +4005,20 @@
       </c>
       <c r="AB29" s="11"/>
       <c r="AC29" s="11"/>
-      <c r="AD29" s="29"/>
-      <c r="AE29" s="29"/>
+      <c r="AD29" s="28"/>
+      <c r="AE29" s="28"/>
       <c r="AF29" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG29" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH29" s="27" t="n">
+      <c r="AH29" s="26" t="n">
         <v>0</v>
       </c>
       <c r="AI29" s="11"/>
       <c r="AJ29" s="13"/>
-      <c r="AK29" s="30"/>
+      <c r="AK29" s="29"/>
       <c r="AL29" s="13"/>
       <c r="AM29" s="13"/>
       <c r="AN29" s="13" t="n">
@@ -4069,15 +4088,15 @@
       </c>
       <c r="AB30" s="11"/>
       <c r="AC30" s="11"/>
-      <c r="AD30" s="29"/>
-      <c r="AE30" s="29"/>
+      <c r="AD30" s="28"/>
+      <c r="AE30" s="28"/>
       <c r="AF30" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG30" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH30" s="27" t="n">
+      <c r="AH30" s="26" t="n">
         <v>0.05</v>
       </c>
       <c r="AI30" s="11"/>
@@ -4162,15 +4181,15 @@
       </c>
       <c r="AB31" s="11"/>
       <c r="AC31" s="11"/>
-      <c r="AD31" s="29"/>
-      <c r="AE31" s="29"/>
+      <c r="AD31" s="28"/>
+      <c r="AE31" s="28"/>
       <c r="AF31" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG31" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH31" s="27" t="n">
+      <c r="AH31" s="26" t="n">
         <v>0</v>
       </c>
       <c r="AI31" s="11"/>
@@ -4255,15 +4274,15 @@
       </c>
       <c r="AB32" s="11"/>
       <c r="AC32" s="11"/>
-      <c r="AD32" s="29"/>
-      <c r="AE32" s="29"/>
+      <c r="AD32" s="28"/>
+      <c r="AE32" s="28"/>
       <c r="AF32" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG32" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH32" s="27" t="n">
+      <c r="AH32" s="26" t="n">
         <v>0</v>
       </c>
       <c r="AI32" s="11"/>
@@ -4346,15 +4365,15 @@
       </c>
       <c r="AB33" s="11"/>
       <c r="AC33" s="11"/>
-      <c r="AD33" s="29"/>
-      <c r="AE33" s="29"/>
+      <c r="AD33" s="28"/>
+      <c r="AE33" s="28"/>
       <c r="AF33" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG33" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH33" s="27" t="n">
+      <c r="AH33" s="26" t="n">
         <v>0.05</v>
       </c>
       <c r="AI33" s="11"/>
@@ -4429,15 +4448,15 @@
       </c>
       <c r="AB34" s="11"/>
       <c r="AC34" s="11"/>
-      <c r="AD34" s="29"/>
-      <c r="AE34" s="29"/>
+      <c r="AD34" s="28"/>
+      <c r="AE34" s="28"/>
       <c r="AF34" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG34" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH34" s="27" t="n">
+      <c r="AH34" s="26" t="n">
         <v>0.05</v>
       </c>
       <c r="AI34" s="11"/>
@@ -4492,7 +4511,7 @@
       </c>
       <c r="L35" s="13"/>
       <c r="M35" s="13"/>
-      <c r="N35" s="11" t="s">
+      <c r="N35" s="30" t="s">
         <v>164</v>
       </c>
       <c r="O35" s="31" t="s">
@@ -4506,7 +4525,7 @@
       <c r="S35" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="T35" s="11" t="s">
+      <c r="T35" s="32" t="s">
         <v>57</v>
       </c>
       <c r="U35" s="11"/>
@@ -4522,15 +4541,15 @@
       </c>
       <c r="AB35" s="11"/>
       <c r="AC35" s="11"/>
-      <c r="AD35" s="29"/>
-      <c r="AE35" s="29"/>
+      <c r="AD35" s="28"/>
+      <c r="AE35" s="28"/>
       <c r="AF35" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG35" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH35" s="27" t="n">
+      <c r="AH35" s="26" t="n">
         <v>0</v>
       </c>
       <c r="AI35" s="11"/>
@@ -4583,20 +4602,22 @@
       </c>
       <c r="L36" s="13"/>
       <c r="M36" s="13"/>
-      <c r="N36" s="11" t="s">
+      <c r="N36" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="O36" s="11" t="s">
-        <v>168</v>
+      <c r="O36" s="30" t="s">
+        <v>169</v>
       </c>
       <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
+      <c r="Q36" s="11" t="s">
+        <v>140</v>
+      </c>
       <c r="R36" s="11"/>
       <c r="S36" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="T36" s="11" t="s">
-        <v>128</v>
+      <c r="T36" s="32" t="s">
+        <v>57</v>
       </c>
       <c r="U36" s="11"/>
       <c r="V36" s="11"/>
@@ -4611,15 +4632,15 @@
       </c>
       <c r="AB36" s="11"/>
       <c r="AC36" s="11"/>
-      <c r="AD36" s="29"/>
-      <c r="AE36" s="29"/>
+      <c r="AD36" s="28"/>
+      <c r="AE36" s="28"/>
       <c r="AF36" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG36" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH36" s="27" t="n">
+      <c r="AH36" s="26" t="n">
         <v>0</v>
       </c>
       <c r="AI36" s="11"/>
@@ -4658,10 +4679,10 @@
       </c>
       <c r="F37" s="13"/>
       <c r="G37" s="13" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I37" s="11" t="s">
         <v>55</v>
@@ -4673,10 +4694,10 @@
       <c r="L37" s="13"/>
       <c r="M37" s="13"/>
       <c r="N37" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="O37" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="P37" s="11"/>
       <c r="Q37" s="11" t="s">
@@ -4702,15 +4723,15 @@
       </c>
       <c r="AB37" s="11"/>
       <c r="AC37" s="11"/>
-      <c r="AD37" s="29"/>
-      <c r="AE37" s="29"/>
+      <c r="AD37" s="28"/>
+      <c r="AE37" s="28"/>
       <c r="AF37" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG37" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH37" s="27" t="n">
+      <c r="AH37" s="26" t="n">
         <v>0.05</v>
       </c>
       <c r="AI37" s="11"/>
@@ -4745,14 +4766,14 @@
         <v>99</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F38" s="13"/>
       <c r="G38" s="13" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I38" s="11" t="s">
         <v>121</v>
@@ -4776,20 +4797,20 @@
       <c r="X38" s="11"/>
       <c r="Y38" s="11"/>
       <c r="Z38" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AA38" s="11"/>
       <c r="AB38" s="11"/>
       <c r="AC38" s="11"/>
-      <c r="AD38" s="29"/>
-      <c r="AE38" s="29"/>
+      <c r="AD38" s="28"/>
+      <c r="AE38" s="28"/>
       <c r="AF38" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG38" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH38" s="27" t="n">
+      <c r="AH38" s="26" t="n">
         <v>0.2</v>
       </c>
       <c r="AI38" s="11"/>
@@ -4804,8 +4825,9 @@
         <v>37</v>
       </c>
       <c r="AP38" s="14" t="s">
-        <v>177</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="AQ38" s="0"/>
       <c r="AR38" s="13"/>
       <c r="AS38" s="16"/>
     </row>
@@ -4823,18 +4845,19 @@
         <v>99</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F39" s="13"/>
       <c r="G39" s="13" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>180</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="J39" s="0"/>
       <c r="K39" s="15" t="n">
         <v>1</v>
       </c>
@@ -4849,7 +4872,7 @@
         <v>56</v>
       </c>
       <c r="T39" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="U39" s="11"/>
       <c r="V39" s="11"/>
@@ -4859,20 +4882,20 @@
       <c r="Z39" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AA39" s="32" t="s">
-        <v>182</v>
+      <c r="AA39" s="33" t="s">
+        <v>183</v>
       </c>
       <c r="AB39" s="11"/>
       <c r="AC39" s="11"/>
-      <c r="AD39" s="29"/>
-      <c r="AE39" s="29"/>
+      <c r="AD39" s="28"/>
+      <c r="AE39" s="28"/>
       <c r="AF39" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG39" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH39" s="27" t="n">
+      <c r="AH39" s="26" t="n">
         <v>0</v>
       </c>
       <c r="AI39" s="11"/>
@@ -4888,7 +4911,7 @@
       </c>
       <c r="AP39" s="13"/>
       <c r="AQ39" s="13" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AR39" s="13"/>
       <c r="AS39" s="16"/>
@@ -4907,18 +4930,19 @@
         <v>99</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F40" s="13"/>
       <c r="G40" s="13" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>185</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="J40" s="0"/>
       <c r="K40" s="13" t="n">
         <v>1</v>
       </c>
@@ -4928,7 +4952,7 @@
         <v>126</v>
       </c>
       <c r="O40" s="11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="P40" s="11"/>
       <c r="Q40" s="11"/>
@@ -4937,7 +4961,7 @@
         <v>56</v>
       </c>
       <c r="T40" s="11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="U40" s="11"/>
       <c r="V40" s="11"/>
@@ -4945,26 +4969,26 @@
       <c r="X40" s="11"/>
       <c r="Y40" s="11"/>
       <c r="Z40" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AA40" s="11"/>
       <c r="AB40" s="11"/>
       <c r="AC40" s="11"/>
-      <c r="AD40" s="29"/>
-      <c r="AE40" s="29"/>
+      <c r="AD40" s="28"/>
+      <c r="AE40" s="28"/>
       <c r="AF40" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG40" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH40" s="27" t="n">
+      <c r="AH40" s="26" t="n">
         <v>0</v>
       </c>
       <c r="AI40" s="11"/>
       <c r="AJ40" s="11"/>
       <c r="AK40" s="11" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AL40" s="13"/>
       <c r="AM40" s="13"/>
@@ -4976,7 +5000,7 @@
       </c>
       <c r="AP40" s="13"/>
       <c r="AQ40" s="13" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AR40" s="13"/>
       <c r="AS40" s="16"/>
@@ -4995,17 +5019,17 @@
         <v>99</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F41" s="13"/>
       <c r="G41" s="13" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J41" s="11"/>
       <c r="K41" s="13" t="n">
@@ -5017,7 +5041,7 @@
         <v>126</v>
       </c>
       <c r="O41" s="11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="P41" s="11"/>
       <c r="Q41" s="11"/>
@@ -5026,7 +5050,7 @@
         <v>56</v>
       </c>
       <c r="T41" s="11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="U41" s="11"/>
       <c r="V41" s="11"/>
@@ -5034,26 +5058,26 @@
       <c r="X41" s="11"/>
       <c r="Y41" s="11"/>
       <c r="Z41" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AA41" s="11"/>
       <c r="AB41" s="11"/>
       <c r="AC41" s="11"/>
-      <c r="AD41" s="29"/>
-      <c r="AE41" s="29"/>
+      <c r="AD41" s="28"/>
+      <c r="AE41" s="28"/>
       <c r="AF41" s="11" t="s">
         <v>51</v>
       </c>
       <c r="AG41" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH41" s="27" t="n">
+      <c r="AH41" s="26" t="n">
         <v>0</v>
       </c>
       <c r="AI41" s="11"/>
       <c r="AJ41" s="11"/>
       <c r="AK41" s="11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AL41" s="13"/>
       <c r="AM41" s="13"/>
@@ -5065,7 +5089,7 @@
       </c>
       <c r="AP41" s="13"/>
       <c r="AQ41" s="13" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AR41" s="13"/>
       <c r="AS41" s="16"/>
@@ -5086,15 +5110,15 @@
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
       <c r="G42" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="I42" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="J42" s="33"/>
+      <c r="I42" s="34" t="s">
+        <v>196</v>
+      </c>
+      <c r="J42" s="34"/>
       <c r="K42" s="15"/>
       <c r="L42" s="15" t="n">
         <v>1</v>
@@ -5106,7 +5130,7 @@
         <v>126</v>
       </c>
       <c r="O42" s="24" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="P42" s="24"/>
       <c r="Q42" s="24"/>
@@ -5115,7 +5139,7 @@
         <v>56</v>
       </c>
       <c r="T42" s="11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="U42" s="13"/>
       <c r="V42" s="13"/>
@@ -5123,7 +5147,7 @@
       <c r="X42" s="13"/>
       <c r="Y42" s="13"/>
       <c r="Z42" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AA42" s="13"/>
       <c r="AB42" s="13"/>
@@ -5136,7 +5160,7 @@
       <c r="AG42" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AH42" s="27" t="n">
+      <c r="AH42" s="26" t="n">
         <v>0</v>
       </c>
       <c r="AI42" s="11"/>
@@ -5152,7 +5176,7 @@
       </c>
       <c r="AP42" s="13"/>
       <c r="AQ42" s="13" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AR42" s="13"/>
       <c r="AS42" s="16"/>
@@ -5167,68 +5191,68 @@
       <c r="C43" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="E43" s="35" t="s">
+      <c r="D43" s="35" t="s">
         <v>197</v>
       </c>
-      <c r="F43" s="35" t="s">
+      <c r="E43" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="G43" s="35" t="s">
+      <c r="F43" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="H43" s="36" t="s">
+      <c r="G43" s="36" t="s">
         <v>200</v>
       </c>
-      <c r="I43" s="36" t="s">
+      <c r="H43" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="J43" s="36" t="s">
+      <c r="I43" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="K43" s="36"/>
-      <c r="L43" s="36"/>
+      <c r="J43" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="K43" s="37"/>
+      <c r="L43" s="37"/>
       <c r="M43" s="17"/>
       <c r="N43" s="17"/>
-      <c r="O43" s="36"/>
-      <c r="P43" s="36"/>
-      <c r="Q43" s="36"/>
-      <c r="R43" s="36"/>
-      <c r="S43" s="36"/>
-      <c r="T43" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="U43" s="36"/>
-      <c r="V43" s="36"/>
-      <c r="W43" s="36"/>
-      <c r="X43" s="36"/>
-      <c r="Y43" s="36"/>
-      <c r="Z43" s="36"/>
-      <c r="AA43" s="36"/>
-      <c r="AB43" s="36"/>
-      <c r="AC43" s="36"/>
-      <c r="AD43" s="36"/>
-      <c r="AE43" s="36"/>
-      <c r="AF43" s="37" t="n">
+      <c r="O43" s="37"/>
+      <c r="P43" s="37"/>
+      <c r="Q43" s="37"/>
+      <c r="R43" s="37"/>
+      <c r="S43" s="37"/>
+      <c r="T43" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="U43" s="37"/>
+      <c r="V43" s="37"/>
+      <c r="W43" s="37"/>
+      <c r="X43" s="37"/>
+      <c r="Y43" s="37"/>
+      <c r="Z43" s="37"/>
+      <c r="AA43" s="37"/>
+      <c r="AB43" s="37"/>
+      <c r="AC43" s="37"/>
+      <c r="AD43" s="37"/>
+      <c r="AE43" s="37"/>
+      <c r="AF43" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="AG43" s="36"/>
-      <c r="AH43" s="36"/>
-      <c r="AI43" s="36"/>
-      <c r="AJ43" s="36"/>
-      <c r="AK43" s="36"/>
+      <c r="AG43" s="37"/>
+      <c r="AH43" s="37"/>
+      <c r="AI43" s="37"/>
+      <c r="AJ43" s="37"/>
+      <c r="AK43" s="37"/>
       <c r="AL43" s="13"/>
-      <c r="AM43" s="36"/>
-      <c r="AN43" s="36"/>
+      <c r="AM43" s="37"/>
+      <c r="AN43" s="37"/>
       <c r="AO43" s="13" t="n">
         <v>42</v>
       </c>
-      <c r="AP43" s="36" t="n">
+      <c r="AP43" s="37" t="n">
         <v>37</v>
       </c>
-      <c r="AQ43" s="36"/>
+      <c r="AQ43" s="37"/>
     </row>
     <row r="44" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="11" t="n">
@@ -5240,68 +5264,68 @@
       <c r="C44" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D44" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="E44" s="35" t="s">
+      <c r="D44" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="E44" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="F44" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="G44" s="35" t="s">
+      <c r="F44" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="H44" s="36" t="s">
+      <c r="G44" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="H44" s="37" t="s">
         <v>112</v>
       </c>
       <c r="I44" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J44" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="K44" s="36"/>
-      <c r="L44" s="36"/>
+        <v>208</v>
+      </c>
+      <c r="K44" s="37"/>
+      <c r="L44" s="37"/>
       <c r="M44" s="17"/>
       <c r="N44" s="17"/>
       <c r="O44" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="P44" s="36"/>
-      <c r="Q44" s="36"/>
-      <c r="R44" s="36"/>
-      <c r="S44" s="36"/>
-      <c r="T44" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="U44" s="36"/>
-      <c r="V44" s="36"/>
-      <c r="W44" s="36"/>
-      <c r="X44" s="36"/>
-      <c r="Y44" s="36"/>
-      <c r="Z44" s="36"/>
-      <c r="AA44" s="36"/>
-      <c r="AB44" s="36"/>
-      <c r="AC44" s="36"/>
-      <c r="AD44" s="36"/>
-      <c r="AE44" s="36"/>
-      <c r="AF44" s="37"/>
-      <c r="AG44" s="36"/>
-      <c r="AH44" s="36"/>
-      <c r="AI44" s="36"/>
-      <c r="AJ44" s="36"/>
-      <c r="AK44" s="36"/>
+        <v>209</v>
+      </c>
+      <c r="P44" s="37"/>
+      <c r="Q44" s="37"/>
+      <c r="R44" s="37"/>
+      <c r="S44" s="37"/>
+      <c r="T44" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="U44" s="37"/>
+      <c r="V44" s="37"/>
+      <c r="W44" s="37"/>
+      <c r="X44" s="37"/>
+      <c r="Y44" s="37"/>
+      <c r="Z44" s="37"/>
+      <c r="AA44" s="37"/>
+      <c r="AB44" s="37"/>
+      <c r="AC44" s="37"/>
+      <c r="AD44" s="37"/>
+      <c r="AE44" s="37"/>
+      <c r="AF44" s="38"/>
+      <c r="AG44" s="37"/>
+      <c r="AH44" s="37"/>
+      <c r="AI44" s="37"/>
+      <c r="AJ44" s="37"/>
+      <c r="AK44" s="37"/>
       <c r="AL44" s="13"/>
-      <c r="AM44" s="36"/>
-      <c r="AN44" s="36"/>
+      <c r="AM44" s="37"/>
+      <c r="AN44" s="37"/>
       <c r="AO44" s="13" t="n">
         <v>43</v>
       </c>
-      <c r="AP44" s="36" t="n">
+      <c r="AP44" s="37" t="n">
         <v>24</v>
       </c>
-      <c r="AQ44" s="36"/>
+      <c r="AQ44" s="37"/>
     </row>
     <row r="45" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="n">
@@ -5313,70 +5337,70 @@
       <c r="C45" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="E45" s="35" t="s">
+      <c r="D45" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="E45" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="F45" s="35" t="s">
-        <v>209</v>
-      </c>
-      <c r="G45" s="35" t="s">
+      <c r="F45" s="36" t="s">
         <v>210</v>
       </c>
-      <c r="H45" s="36" t="s">
+      <c r="G45" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="H45" s="37" t="s">
         <v>119</v>
       </c>
       <c r="I45" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J45" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="K45" s="36"/>
-      <c r="L45" s="36"/>
+        <v>208</v>
+      </c>
+      <c r="K45" s="37"/>
+      <c r="L45" s="37"/>
       <c r="M45" s="17"/>
       <c r="N45" s="17"/>
       <c r="O45" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="P45" s="36"/>
-      <c r="Q45" s="36"/>
-      <c r="R45" s="36"/>
-      <c r="S45" s="36"/>
-      <c r="T45" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="U45" s="36"/>
-      <c r="V45" s="36"/>
-      <c r="W45" s="36"/>
-      <c r="X45" s="36"/>
-      <c r="Y45" s="36"/>
-      <c r="Z45" s="36"/>
-      <c r="AA45" s="36"/>
-      <c r="AB45" s="36"/>
-      <c r="AC45" s="36"/>
-      <c r="AD45" s="36"/>
-      <c r="AE45" s="36"/>
-      <c r="AF45" s="37" t="n">
+        <v>212</v>
+      </c>
+      <c r="P45" s="37"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="37"/>
+      <c r="S45" s="37"/>
+      <c r="T45" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="U45" s="37"/>
+      <c r="V45" s="37"/>
+      <c r="W45" s="37"/>
+      <c r="X45" s="37"/>
+      <c r="Y45" s="37"/>
+      <c r="Z45" s="37"/>
+      <c r="AA45" s="37"/>
+      <c r="AB45" s="37"/>
+      <c r="AC45" s="37"/>
+      <c r="AD45" s="37"/>
+      <c r="AE45" s="37"/>
+      <c r="AF45" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="AG45" s="36"/>
-      <c r="AH45" s="36"/>
-      <c r="AI45" s="36"/>
-      <c r="AJ45" s="36"/>
-      <c r="AK45" s="36"/>
+      <c r="AG45" s="37"/>
+      <c r="AH45" s="37"/>
+      <c r="AI45" s="37"/>
+      <c r="AJ45" s="37"/>
+      <c r="AK45" s="37"/>
       <c r="AL45" s="13"/>
-      <c r="AM45" s="36"/>
-      <c r="AN45" s="36"/>
+      <c r="AM45" s="37"/>
+      <c r="AN45" s="37"/>
       <c r="AO45" s="13" t="n">
         <v>44</v>
       </c>
-      <c r="AP45" s="36" t="n">
+      <c r="AP45" s="37" t="n">
         <v>25</v>
       </c>
-      <c r="AQ45" s="36"/>
+      <c r="AQ45" s="37"/>
     </row>
     <row r="46" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="n">
@@ -5388,70 +5412,70 @@
       <c r="C46" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D46" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="E46" s="35" t="s">
+      <c r="D46" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="E46" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="F46" s="35" t="s">
-        <v>209</v>
-      </c>
-      <c r="G46" s="35" t="s">
+      <c r="F46" s="36" t="s">
         <v>210</v>
       </c>
-      <c r="H46" s="36" t="s">
+      <c r="G46" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="H46" s="37" t="s">
         <v>142</v>
       </c>
       <c r="I46" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J46" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="K46" s="36"/>
-      <c r="L46" s="36"/>
+        <v>208</v>
+      </c>
+      <c r="K46" s="37"/>
+      <c r="L46" s="37"/>
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
       <c r="O46" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="P46" s="36"/>
-      <c r="Q46" s="36"/>
-      <c r="R46" s="36"/>
-      <c r="S46" s="36"/>
-      <c r="T46" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="U46" s="36"/>
-      <c r="V46" s="36"/>
-      <c r="W46" s="36"/>
-      <c r="X46" s="36"/>
-      <c r="Y46" s="36"/>
-      <c r="Z46" s="36"/>
-      <c r="AA46" s="36"/>
-      <c r="AB46" s="36"/>
-      <c r="AC46" s="36"/>
-      <c r="AD46" s="36"/>
-      <c r="AE46" s="36"/>
-      <c r="AF46" s="37" t="n">
+        <v>213</v>
+      </c>
+      <c r="P46" s="37"/>
+      <c r="Q46" s="37"/>
+      <c r="R46" s="37"/>
+      <c r="S46" s="37"/>
+      <c r="T46" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="U46" s="37"/>
+      <c r="V46" s="37"/>
+      <c r="W46" s="37"/>
+      <c r="X46" s="37"/>
+      <c r="Y46" s="37"/>
+      <c r="Z46" s="37"/>
+      <c r="AA46" s="37"/>
+      <c r="AB46" s="37"/>
+      <c r="AC46" s="37"/>
+      <c r="AD46" s="37"/>
+      <c r="AE46" s="37"/>
+      <c r="AF46" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="AG46" s="36"/>
-      <c r="AH46" s="36"/>
-      <c r="AI46" s="36"/>
-      <c r="AJ46" s="36"/>
-      <c r="AK46" s="36"/>
+      <c r="AG46" s="37"/>
+      <c r="AH46" s="37"/>
+      <c r="AI46" s="37"/>
+      <c r="AJ46" s="37"/>
+      <c r="AK46" s="37"/>
       <c r="AL46" s="13"/>
-      <c r="AM46" s="36"/>
-      <c r="AN46" s="36"/>
+      <c r="AM46" s="37"/>
+      <c r="AN46" s="37"/>
       <c r="AO46" s="13" t="n">
         <v>45</v>
       </c>
-      <c r="AP46" s="36" t="n">
+      <c r="AP46" s="37" t="n">
         <v>29</v>
       </c>
-      <c r="AQ46" s="36"/>
+      <c r="AQ46" s="37"/>
     </row>
     <row r="47" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="n">
@@ -5463,70 +5487,70 @@
       <c r="C47" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D47" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="E47" s="35" t="s">
+      <c r="D47" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="E47" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="F47" s="35" t="s">
-        <v>213</v>
-      </c>
-      <c r="G47" s="35" t="s">
+      <c r="F47" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="H47" s="36" t="s">
+      <c r="G47" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="H47" s="37" t="s">
         <v>154</v>
       </c>
       <c r="I47" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J47" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="K47" s="36"/>
-      <c r="L47" s="36"/>
+        <v>208</v>
+      </c>
+      <c r="K47" s="37"/>
+      <c r="L47" s="37"/>
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
       <c r="O47" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="P47" s="36"/>
-      <c r="Q47" s="36"/>
-      <c r="R47" s="36"/>
-      <c r="S47" s="36"/>
-      <c r="T47" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="U47" s="36"/>
-      <c r="V47" s="36"/>
-      <c r="W47" s="36"/>
-      <c r="X47" s="36"/>
-      <c r="Y47" s="36"/>
-      <c r="Z47" s="36"/>
-      <c r="AA47" s="36"/>
-      <c r="AB47" s="36"/>
-      <c r="AC47" s="36"/>
-      <c r="AD47" s="36"/>
-      <c r="AE47" s="36"/>
-      <c r="AF47" s="37" t="n">
+        <v>216</v>
+      </c>
+      <c r="P47" s="37"/>
+      <c r="Q47" s="37"/>
+      <c r="R47" s="37"/>
+      <c r="S47" s="37"/>
+      <c r="T47" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="U47" s="37"/>
+      <c r="V47" s="37"/>
+      <c r="W47" s="37"/>
+      <c r="X47" s="37"/>
+      <c r="Y47" s="37"/>
+      <c r="Z47" s="37"/>
+      <c r="AA47" s="37"/>
+      <c r="AB47" s="37"/>
+      <c r="AC47" s="37"/>
+      <c r="AD47" s="37"/>
+      <c r="AE47" s="37"/>
+      <c r="AF47" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="AG47" s="36"/>
-      <c r="AH47" s="36"/>
-      <c r="AI47" s="36"/>
-      <c r="AJ47" s="36"/>
-      <c r="AK47" s="36"/>
-      <c r="AL47" s="38"/>
-      <c r="AM47" s="36"/>
-      <c r="AN47" s="36"/>
+      <c r="AG47" s="37"/>
+      <c r="AH47" s="37"/>
+      <c r="AI47" s="37"/>
+      <c r="AJ47" s="37"/>
+      <c r="AK47" s="37"/>
+      <c r="AL47" s="39"/>
+      <c r="AM47" s="37"/>
+      <c r="AN47" s="37"/>
       <c r="AO47" s="13" t="n">
         <v>46</v>
       </c>
-      <c r="AP47" s="36" t="n">
+      <c r="AP47" s="37" t="n">
         <v>32</v>
       </c>
-      <c r="AQ47" s="36"/>
+      <c r="AQ47" s="37"/>
     </row>
     <row r="48" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="n">
@@ -5538,70 +5562,70 @@
       <c r="C48" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D48" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="E48" s="35" t="s">
+      <c r="D48" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="E48" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="F48" s="35" t="s">
-        <v>213</v>
-      </c>
-      <c r="G48" s="35" t="s">
+      <c r="F48" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="H48" s="36" t="s">
+      <c r="G48" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="H48" s="37" t="s">
         <v>159</v>
       </c>
       <c r="I48" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J48" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="K48" s="36"/>
-      <c r="L48" s="36"/>
+        <v>208</v>
+      </c>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
       <c r="M48" s="17"/>
       <c r="N48" s="17"/>
       <c r="O48" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="P48" s="36"/>
-      <c r="Q48" s="36"/>
-      <c r="R48" s="36"/>
-      <c r="S48" s="36"/>
-      <c r="T48" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="U48" s="36"/>
-      <c r="V48" s="36"/>
-      <c r="W48" s="36"/>
-      <c r="X48" s="36"/>
-      <c r="Y48" s="36"/>
-      <c r="Z48" s="36"/>
-      <c r="AA48" s="36"/>
-      <c r="AB48" s="36"/>
-      <c r="AC48" s="36"/>
-      <c r="AD48" s="36"/>
-      <c r="AE48" s="36"/>
-      <c r="AF48" s="37" t="n">
+        <v>217</v>
+      </c>
+      <c r="P48" s="37"/>
+      <c r="Q48" s="37"/>
+      <c r="R48" s="37"/>
+      <c r="S48" s="37"/>
+      <c r="T48" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="U48" s="37"/>
+      <c r="V48" s="37"/>
+      <c r="W48" s="37"/>
+      <c r="X48" s="37"/>
+      <c r="Y48" s="37"/>
+      <c r="Z48" s="37"/>
+      <c r="AA48" s="37"/>
+      <c r="AB48" s="37"/>
+      <c r="AC48" s="37"/>
+      <c r="AD48" s="37"/>
+      <c r="AE48" s="37"/>
+      <c r="AF48" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="AG48" s="36"/>
-      <c r="AH48" s="36"/>
-      <c r="AI48" s="36"/>
-      <c r="AJ48" s="36"/>
-      <c r="AK48" s="36"/>
-      <c r="AL48" s="38"/>
-      <c r="AM48" s="36"/>
-      <c r="AN48" s="36"/>
+      <c r="AG48" s="37"/>
+      <c r="AH48" s="37"/>
+      <c r="AI48" s="37"/>
+      <c r="AJ48" s="37"/>
+      <c r="AK48" s="37"/>
+      <c r="AL48" s="39"/>
+      <c r="AM48" s="37"/>
+      <c r="AN48" s="37"/>
       <c r="AO48" s="13" t="n">
         <v>47</v>
       </c>
-      <c r="AP48" s="36" t="n">
+      <c r="AP48" s="37" t="n">
         <v>33</v>
       </c>
-      <c r="AQ48" s="36"/>
+      <c r="AQ48" s="37"/>
     </row>
     <row r="49" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="n">
@@ -5613,70 +5637,70 @@
       <c r="C49" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D49" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="E49" s="35" t="s">
+      <c r="D49" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="E49" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="F49" s="35" t="s">
-        <v>213</v>
-      </c>
-      <c r="G49" s="35" t="s">
+      <c r="F49" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="H49" s="36" t="s">
-        <v>169</v>
+      <c r="G49" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="H49" s="37" t="s">
+        <v>170</v>
       </c>
       <c r="I49" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J49" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="K49" s="36"/>
-      <c r="L49" s="36"/>
+        <v>208</v>
+      </c>
+      <c r="K49" s="37"/>
+      <c r="L49" s="37"/>
       <c r="M49" s="17"/>
       <c r="N49" s="17"/>
       <c r="O49" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="P49" s="36"/>
-      <c r="Q49" s="36"/>
-      <c r="R49" s="36"/>
-      <c r="S49" s="36"/>
-      <c r="T49" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="U49" s="36"/>
-      <c r="V49" s="36"/>
-      <c r="W49" s="36"/>
-      <c r="X49" s="36"/>
-      <c r="Y49" s="36"/>
-      <c r="Z49" s="36"/>
-      <c r="AA49" s="36"/>
-      <c r="AB49" s="36"/>
-      <c r="AC49" s="36"/>
-      <c r="AD49" s="36"/>
-      <c r="AE49" s="36"/>
-      <c r="AF49" s="37" t="n">
+        <v>218</v>
+      </c>
+      <c r="P49" s="37"/>
+      <c r="Q49" s="37"/>
+      <c r="R49" s="37"/>
+      <c r="S49" s="37"/>
+      <c r="T49" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="U49" s="37"/>
+      <c r="V49" s="37"/>
+      <c r="W49" s="37"/>
+      <c r="X49" s="37"/>
+      <c r="Y49" s="37"/>
+      <c r="Z49" s="37"/>
+      <c r="AA49" s="37"/>
+      <c r="AB49" s="37"/>
+      <c r="AC49" s="37"/>
+      <c r="AD49" s="37"/>
+      <c r="AE49" s="37"/>
+      <c r="AF49" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="AG49" s="36"/>
-      <c r="AH49" s="36"/>
-      <c r="AI49" s="36"/>
-      <c r="AJ49" s="36"/>
-      <c r="AK49" s="36"/>
-      <c r="AL49" s="38"/>
-      <c r="AM49" s="36"/>
-      <c r="AN49" s="36"/>
+      <c r="AG49" s="37"/>
+      <c r="AH49" s="37"/>
+      <c r="AI49" s="37"/>
+      <c r="AJ49" s="37"/>
+      <c r="AK49" s="37"/>
+      <c r="AL49" s="39"/>
+      <c r="AM49" s="37"/>
+      <c r="AN49" s="37"/>
       <c r="AO49" s="13" t="n">
         <v>48</v>
       </c>
-      <c r="AP49" s="36" t="n">
+      <c r="AP49" s="37" t="n">
         <v>36</v>
       </c>
-      <c r="AQ49" s="36"/>
+      <c r="AQ49" s="37"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AS42"/>
@@ -5704,51 +5728,54 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.093023255814"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="40" t="s">
-        <v>218</v>
-      </c>
-      <c r="H1" s="40" t="s">
+      <c r="G1" s="41" t="s">
         <v>219</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="H1" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="I1" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="40" t="s">
-        <v>220</v>
-      </c>
-      <c r="L1" s="40" t="s">
+      <c r="K1" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="L1" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="M1" s="41" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="41" t="s">
-        <v>221</v>
+      <c r="B4" s="42" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>